<commit_message>
Remove preview as can't make DNS challenge
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timja/projects/moj-reform/platform/bulk-scan-shared-infrastrucutre/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E81F4A6-9466-894E-8A65-319105D520CF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DBF466-F05E-9547-A271-DDA76D1A2AFB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15000" tabRatio="500" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -893,9 +893,6 @@
     <t>openingDate</t>
   </si>
   <si>
-    <t>https://url.for.bulk.scan.orchestrator</t>
-  </si>
-  <si>
     <t>https://url.for.service.endpoint</t>
   </si>
   <si>
@@ -918,6 +915,9 @@
   </si>
   <si>
     <t>caseworker-bulkscan</t>
+  </si>
+  <si>
+    <t>http://docker.host.internal:8582/callback/about-to-submit</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1999,7 +1999,7 @@
         <v>43384</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>170</v>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>170</v>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>170</v>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>170</v>
@@ -2284,7 +2284,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="60" t="s">
         <v>170</v>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D9" s="60" t="s">
         <v>170</v>
@@ -2338,7 +2338,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>170</v>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>170</v>
@@ -2392,7 +2392,7 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D12" s="60" t="s">
         <v>170</v>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>213</v>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>257</v>
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="B8" s="60"/>
       <c r="C8" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>223</v>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>235</v>
@@ -2810,7 +2810,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" t="s">
         <v>182</v>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>213</v>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>223</v>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>235</v>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" t="s">
         <v>182</v>
@@ -3233,7 +3233,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>213</v>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>223</v>
@@ -4239,10 +4239,10 @@
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>198</v>
@@ -4358,13 +4358,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F4" s="117" t="s">
         <v>198</v>
@@ -4375,13 +4375,13 @@
         <v>43101</v>
       </c>
       <c r="C5" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>215</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F5" s="119" t="s">
         <v>198</v>
@@ -4392,13 +4392,13 @@
         <v>43101</v>
       </c>
       <c r="C6" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F6" s="119" t="s">
         <v>198</v>
@@ -4409,13 +4409,13 @@
         <v>43101</v>
       </c>
       <c r="C7" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F7" s="119" t="s">
         <v>198</v>
@@ -4426,13 +4426,13 @@
         <v>43101</v>
       </c>
       <c r="C8" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>213</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F8" s="119" t="s">
         <v>198</v>
@@ -4443,13 +4443,13 @@
         <v>43101</v>
       </c>
       <c r="C9" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>257</v>
       </c>
       <c r="E9" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F9" s="119" t="s">
         <v>198</v>
@@ -4460,13 +4460,13 @@
         <v>43101</v>
       </c>
       <c r="C10" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F10" s="119" t="s">
         <v>198</v>
@@ -4477,13 +4477,13 @@
         <v>43101</v>
       </c>
       <c r="C11" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E11" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F11" s="119" t="s">
         <v>198</v>
@@ -4494,13 +4494,13 @@
         <v>43101</v>
       </c>
       <c r="C12" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>223</v>
       </c>
       <c r="E12" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F12" s="119" t="s">
         <v>198</v>
@@ -5346,13 +5346,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>219</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F4" s="117" t="s">
         <v>198</v>
@@ -5364,13 +5364,13 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>217</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F5" s="119" t="s">
         <v>198</v>
@@ -5382,13 +5382,13 @@
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>125</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F6" s="123" t="s">
         <v>198</v>
@@ -5400,13 +5400,13 @@
       </c>
       <c r="B7" s="122"/>
       <c r="C7" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F7" s="119" t="s">
         <v>198</v>
@@ -5418,13 +5418,13 @@
       </c>
       <c r="B8" s="124"/>
       <c r="C8" s="115" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>127</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F8" s="121" t="s">
         <v>198</v>
@@ -5461,7 +5461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -6286,13 +6286,13 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="136" t="s">
         <v>95</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F4" s="137" t="s">
         <v>198</v>
@@ -6304,13 +6304,13 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>245</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F5" s="138" t="s">
         <v>198</v>
@@ -6322,13 +6322,13 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>246</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F6" s="138" t="s">
         <v>198</v>
@@ -6340,13 +6340,13 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="139" t="s">
         <v>96</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F7" s="140" t="s">
         <v>198</v>
@@ -6358,13 +6358,13 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="139" t="s">
         <v>252</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F8" s="140" t="s">
         <v>198</v>
@@ -6480,13 +6480,13 @@
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>263</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -6624,14 +6624,14 @@
         <v>43101</v>
       </c>
       <c r="C4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>265</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -6862,7 +6862,7 @@
       </c>
       <c r="B4" s="50"/>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
@@ -6887,7 +6887,7 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>215</v>
@@ -6912,7 +6912,7 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
@@ -6935,7 +6935,7 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
@@ -6958,7 +6958,7 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>213</v>
@@ -6981,7 +6981,7 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>257</v>
@@ -7004,7 +7004,7 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>56</v>
@@ -7029,7 +7029,7 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>59</v>
@@ -7054,7 +7054,7 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>223</v>
@@ -7707,7 +7707,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>95</v>
@@ -7728,7 +7728,7 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>245</v>
@@ -7749,7 +7749,7 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>246</v>
@@ -7769,7 +7769,7 @@
         <v>43101</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>96</v>
@@ -7789,7 +7789,7 @@
         <v>43101</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>252</v>
@@ -7828,8 +7828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8018,7 +8018,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>219</v>
@@ -8050,7 +8050,7 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>217</v>
@@ -8072,11 +8072,11 @@
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="L5" s="144" t="s">
+        <v>266</v>
+      </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="144" t="s">
-        <v>258</v>
-      </c>
+      <c r="N5" s="144"/>
       <c r="P5" s="51" t="s">
         <v>122</v>
       </c>
@@ -8093,7 +8093,7 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>218</v>
@@ -8113,15 +8113,14 @@
       <c r="I6" s="60" t="s">
         <v>246</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="J6" s="144" t="s">
+        <v>258</v>
+      </c>
       <c r="K6" s="5"/>
       <c r="L6" s="144" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="144" t="s">
-        <v>259</v>
-      </c>
       <c r="P6" s="5" t="s">
         <v>122</v>
       </c>
@@ -8138,7 +8137,7 @@
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>125</v>
@@ -8179,7 +8178,7 @@
       </c>
       <c r="B8" s="71"/>
       <c r="C8" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>127</v>
@@ -8225,9 +8224,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="N6" r:id="rId1" xr:uid="{0AEF91E4-C31B-6948-8CA6-C50706B87B14}"/>
-    <hyperlink ref="N5" r:id="rId2" xr:uid="{52614C83-3AC1-0148-BC43-821E043636BC}"/>
-    <hyperlink ref="L6" r:id="rId3" xr:uid="{B25A138A-C0B9-AC4C-9B54-D281FFD0AE41}"/>
+    <hyperlink ref="L6" r:id="rId1" xr:uid="{0AEF91E4-C31B-6948-8CA6-C50706B87B14}"/>
+    <hyperlink ref="J6" r:id="rId2" xr:uid="{B25A138A-C0B9-AC4C-9B54-D281FFD0AE41}"/>
+    <hyperlink ref="L5" r:id="rId3" xr:uid="{D3BED0F9-6D61-CD46-85DF-3DD6C0330875}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -8403,7 +8402,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>219</v>
@@ -8437,7 +8436,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>219</v>
@@ -8471,7 +8470,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>219</v>
@@ -8505,7 +8504,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>219</v>
@@ -8539,7 +8538,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>219</v>
@@ -8573,7 +8572,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>219</v>
@@ -8607,7 +8606,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>219</v>
@@ -8641,7 +8640,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>219</v>
@@ -8675,7 +8674,7 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>217</v>
@@ -8709,7 +8708,7 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>217</v>
@@ -8743,7 +8742,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D14" s="60" t="s">
         <v>125</v>
@@ -8777,7 +8776,7 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D15" s="60" t="s">
         <v>125</v>
@@ -8811,7 +8810,7 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>218</v>
@@ -8845,7 +8844,7 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>218</v>
@@ -8879,7 +8878,7 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D18" s="60" t="s">
         <v>127</v>
@@ -8909,7 +8908,7 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D19" s="60" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
Update fields and types for exception record create event
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E81F4A6-9466-894E-8A65-319105D520CF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C97E3D-B696-6B45-A615-450DAF5FEA8C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="268">
   <si>
     <t>Change History</t>
   </si>
@@ -809,18 +809,6 @@
     <t>ocr</t>
   </si>
   <si>
-    <t>documentType</t>
-  </si>
-  <si>
-    <t>documentLink</t>
-  </si>
-  <si>
-    <t>documentControlNumber</t>
-  </si>
-  <si>
-    <t>filename</t>
-  </si>
-  <si>
     <t>Create new case from exception</t>
   </si>
   <si>
@@ -836,9 +824,6 @@
     <t>ScannedDocument</t>
   </si>
   <si>
-    <t>docScanDate</t>
-  </si>
-  <si>
     <t>Scanned Date</t>
   </si>
   <si>
@@ -918,6 +903,24 @@
   </si>
   <si>
     <t>caseworker-bulkscan</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>controlNumber</t>
+  </si>
+  <si>
+    <t>fileName</t>
+  </si>
+  <si>
+    <t>scannedDate</t>
+  </si>
+  <si>
+    <t>Review fields and types for new exception event</t>
   </si>
 </sst>
 </file>
@@ -1945,16 +1948,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="60.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="5" width="11.5"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
     <col min="7" max="1025" width="11.5"/>
   </cols>
@@ -1990,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1999,14 +2003,25 @@
         <v>43384</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6">
+        <v>43399</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="5"/>
@@ -2176,7 +2191,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>170</v>
@@ -2203,7 +2218,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>170</v>
@@ -2230,7 +2245,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>170</v>
@@ -2257,7 +2272,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>170</v>
@@ -2284,7 +2299,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D8" s="60" t="s">
         <v>170</v>
@@ -2311,7 +2326,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D9" s="60" t="s">
         <v>170</v>
@@ -2326,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="I9" s="86">
         <v>6</v>
@@ -2338,7 +2353,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>170</v>
@@ -2365,7 +2380,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>170</v>
@@ -2392,7 +2407,7 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D12" s="60" t="s">
         <v>170</v>
@@ -2401,7 +2416,7 @@
         <v>229</v>
       </c>
       <c r="F12" s="60" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="G12" s="86">
         <v>3</v>
@@ -2526,7 +2541,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>213</v>
@@ -2565,13 +2580,13 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
@@ -2583,7 +2598,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
@@ -2601,7 +2616,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
@@ -2619,7 +2634,7 @@
       </c>
       <c r="B8" s="60"/>
       <c r="C8" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>223</v>
@@ -2787,10 +2802,10 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>55</v>
@@ -2810,7 +2825,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" t="s">
         <v>182</v>
@@ -2849,7 +2864,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>213</v>
@@ -2888,7 +2903,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>223</v>
@@ -3155,10 +3170,10 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>55</v>
@@ -3194,7 +3209,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" t="s">
         <v>182</v>
@@ -3233,7 +3248,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>213</v>
@@ -3272,7 +3287,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>223</v>
@@ -4239,10 +4254,10 @@
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>198</v>
@@ -4358,13 +4373,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F4" s="117" t="s">
         <v>198</v>
@@ -4375,13 +4390,13 @@
         <v>43101</v>
       </c>
       <c r="C5" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>215</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F5" s="119" t="s">
         <v>198</v>
@@ -4392,13 +4407,13 @@
         <v>43101</v>
       </c>
       <c r="C6" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F6" s="119" t="s">
         <v>198</v>
@@ -4409,13 +4424,13 @@
         <v>43101</v>
       </c>
       <c r="C7" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F7" s="119" t="s">
         <v>198</v>
@@ -4426,13 +4441,13 @@
         <v>43101</v>
       </c>
       <c r="C8" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>213</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F8" s="119" t="s">
         <v>198</v>
@@ -4443,13 +4458,13 @@
         <v>43101</v>
       </c>
       <c r="C9" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E9" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F9" s="119" t="s">
         <v>198</v>
@@ -4460,13 +4475,13 @@
         <v>43101</v>
       </c>
       <c r="C10" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F10" s="119" t="s">
         <v>198</v>
@@ -4477,13 +4492,13 @@
         <v>43101</v>
       </c>
       <c r="C11" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E11" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F11" s="119" t="s">
         <v>198</v>
@@ -4494,13 +4509,13 @@
         <v>43101</v>
       </c>
       <c r="C12" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>223</v>
       </c>
       <c r="E12" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F12" s="119" t="s">
         <v>198</v>
@@ -5346,13 +5361,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>219</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F4" s="117" t="s">
         <v>198</v>
@@ -5364,13 +5379,13 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>217</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F5" s="119" t="s">
         <v>198</v>
@@ -5382,13 +5397,13 @@
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>125</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F6" s="123" t="s">
         <v>198</v>
@@ -5400,13 +5415,13 @@
       </c>
       <c r="B7" s="122"/>
       <c r="C7" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F7" s="119" t="s">
         <v>198</v>
@@ -5418,13 +5433,13 @@
       </c>
       <c r="B8" s="124"/>
       <c r="C8" s="115" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>127</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F8" s="121" t="s">
         <v>198</v>
@@ -5461,7 +5476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -6286,13 +6301,13 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="136" t="s">
         <v>95</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F4" s="137" t="s">
         <v>198</v>
@@ -6304,13 +6319,13 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F5" s="138" t="s">
         <v>198</v>
@@ -6322,13 +6337,13 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F6" s="138" t="s">
         <v>198</v>
@@ -6340,13 +6355,13 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D7" s="139" t="s">
         <v>96</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F7" s="140" t="s">
         <v>198</v>
@@ -6358,13 +6373,13 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D8" s="139" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F8" s="140" t="s">
         <v>198</v>
@@ -6480,13 +6495,13 @@
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -6624,14 +6639,14 @@
         <v>43101</v>
       </c>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -6655,8 +6670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6862,13 +6877,13 @@
       </c>
       <c r="B4" s="50"/>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F4" s="73" t="s">
         <v>51</v>
@@ -6887,7 +6902,7 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>215</v>
@@ -6896,7 +6911,7 @@
         <v>216</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>52</v>
@@ -6912,7 +6927,7 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
@@ -6935,7 +6950,7 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
@@ -6958,7 +6973,7 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>213</v>
@@ -6981,13 +6996,13 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F9" s="73"/>
       <c r="G9" s="5" t="s">
@@ -7004,7 +7019,7 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>56</v>
@@ -7017,7 +7032,7 @@
         <v>58</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>32</v>
@@ -7029,13 +7044,13 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F11" s="73"/>
       <c r="G11" s="5" t="s">
@@ -7054,7 +7069,7 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>223</v>
@@ -7094,7 +7109,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7303,7 +7318,7 @@
         <v>43101</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>74</v>
@@ -7324,16 +7339,16 @@
         <v>43101</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>76</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>75</v>
@@ -7348,17 +7363,17 @@
       </c>
       <c r="B8" s="55"/>
       <c r="C8" s="65" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>231</v>
+        <v>263</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="60"/>
@@ -7378,10 +7393,10 @@
         <v>43101</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>52</v>
@@ -7399,10 +7414,10 @@
         <v>43101</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>52</v>
@@ -7420,17 +7435,17 @@
         <v>43101</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="K11" s="60" t="s">
         <v>32</v>
@@ -7537,13 +7552,13 @@
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="56" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D4" s="57" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F4" s="60"/>
       <c r="H4" s="5"/>
@@ -7564,7 +7579,7 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="61" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D5" s="62" t="s">
         <v>85</v>
@@ -7601,7 +7616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C8"/>
     </sheetView>
   </sheetViews>
@@ -7707,7 +7722,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>95</v>
@@ -7728,16 +7743,16 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F5" s="60" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G5" s="72">
         <v>2</v>
@@ -7749,16 +7764,16 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G6" s="72">
         <v>3</v>
@@ -7769,7 +7784,7 @@
         <v>43101</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>96</v>
@@ -7789,16 +7804,16 @@
         <v>43101</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G8" s="72">
         <v>5</v>
@@ -7829,7 +7844,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8018,7 +8033,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>219</v>
@@ -8050,7 +8065,7 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>217</v>
@@ -8068,14 +8083,14 @@
         <v>95</v>
       </c>
       <c r="I5" s="60" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="144" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="P5" s="51" t="s">
         <v>122</v>
@@ -8093,13 +8108,13 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F6" t="s">
         <v>221</v>
@@ -8111,16 +8126,16 @@
         <v>95</v>
       </c>
       <c r="I6" s="60" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="144" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="144" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>122</v>
@@ -8138,7 +8153,7 @@
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>125</v>
@@ -8179,7 +8194,7 @@
       </c>
       <c r="B8" s="71"/>
       <c r="C8" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>127</v>
@@ -8197,7 +8212,7 @@
         <v>95</v>
       </c>
       <c r="I8" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="P8" s="51" t="s">
         <v>122</v>
@@ -8236,10 +8251,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AB31"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8403,19 +8418,19 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="F4" s="72">
         <v>1</v>
       </c>
-      <c r="G4" s="51" t="s">
-        <v>152</v>
+      <c r="G4" s="84" t="s">
+        <v>154</v>
       </c>
       <c r="H4" s="72">
         <v>1</v>
@@ -8437,13 +8452,13 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>215</v>
+        <v>56</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
@@ -8471,19 +8486,19 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>219</v>
+        <v>259</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>125</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>211</v>
+        <v>59</v>
       </c>
       <c r="F6" s="72">
-        <v>3</v>
-      </c>
-      <c r="G6" s="84" t="s">
-        <v>154</v>
+        <v>1</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>152</v>
       </c>
       <c r="H6" s="72">
         <v>1</v>
@@ -8505,19 +8520,19 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>212</v>
+        <v>259</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="60" t="s">
+        <v>56</v>
       </c>
       <c r="F7" s="72">
-        <v>4</v>
-      </c>
-      <c r="G7" s="84" t="s">
-        <v>154</v>
+        <v>2</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>152</v>
       </c>
       <c r="H7" s="72">
         <v>1</v>
@@ -8539,16 +8554,16 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>213</v>
+        <v>218</v>
+      </c>
+      <c r="E8" s="60" t="s">
+        <v>56</v>
       </c>
       <c r="F8" s="72">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G8" s="84" t="s">
         <v>154</v>
@@ -8573,16 +8588,16 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>257</v>
+        <v>59</v>
       </c>
       <c r="F9" s="72">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G9" s="84" t="s">
         <v>154</v>
@@ -8601,25 +8616,25 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A10" s="25">
         <v>43101</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E10" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="60" t="s">
         <v>56</v>
       </c>
       <c r="F10" s="72">
-        <v>7</v>
-      </c>
-      <c r="G10" s="84" t="s">
-        <v>154</v>
+        <v>1</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>152</v>
       </c>
       <c r="H10" s="72">
         <v>1</v>
@@ -8630,30 +8645,26 @@
       <c r="K10" s="72">
         <v>1</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A11" s="25">
         <v>43101</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>219</v>
+        <v>259</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>127</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F11" s="72">
-        <v>8</v>
-      </c>
-      <c r="G11" s="84" t="s">
-        <v>154</v>
+        <v>2</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>152</v>
       </c>
       <c r="H11" s="72">
         <v>1</v>
@@ -8664,305 +8675,37 @@
       <c r="K11" s="72">
         <v>1</v>
       </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="25">
-        <v>43101</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="F12" s="72">
-        <v>1</v>
-      </c>
-      <c r="G12" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="H12" s="72">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="K12" s="72">
-        <v>1</v>
-      </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="25">
-        <v>43101</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E13" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="72">
-        <v>2</v>
-      </c>
-      <c r="G13" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="H13" s="72">
-        <v>1</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="K13" s="72">
-        <v>1</v>
-      </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="25">
-        <v>43101</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D14" s="60" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="72">
-        <v>1</v>
-      </c>
-      <c r="G14" s="51" t="s">
-        <v>152</v>
-      </c>
-      <c r="H14" s="72">
-        <v>1</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="K14" s="72">
-        <v>1</v>
-      </c>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="25">
-        <v>43101</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D15" s="60" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="72">
-        <v>2</v>
-      </c>
-      <c r="G15" s="51" t="s">
-        <v>152</v>
-      </c>
-      <c r="H15" s="72">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="K15" s="72">
-        <v>1</v>
-      </c>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="25">
-        <v>43101</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E16" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="72">
-        <v>1</v>
-      </c>
-      <c r="G16" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="H16" s="72">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="K16" s="72">
-        <v>1</v>
-      </c>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="25">
-        <v>43101</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="72">
-        <v>2</v>
-      </c>
-      <c r="G17" s="84" t="s">
-        <v>154</v>
-      </c>
-      <c r="H17" s="72">
-        <v>1</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="K17" s="72">
-        <v>1</v>
-      </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A18" s="25">
-        <v>43101</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D18" s="60" t="s">
-        <v>127</v>
-      </c>
-      <c r="E18" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="72">
-        <v>1</v>
-      </c>
-      <c r="G18" s="51" t="s">
-        <v>152</v>
-      </c>
-      <c r="H18" s="72">
-        <v>1</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="K18" s="72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A19" s="25">
-        <v>43101</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D19" s="60" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="72">
-        <v>2</v>
-      </c>
-      <c r="G19" s="51" t="s">
-        <v>152</v>
-      </c>
-      <c r="H19" s="72">
-        <v>1</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="K19" s="72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="E16" s="60"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="E24" s="60"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="E31" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A19" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Update to DateTime field type
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C97E3D-B696-6B45-A615-450DAF5FEA8C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59631A2B-3333-E841-8F58-AB11C3D5D48E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="270">
   <si>
     <t>Change History</t>
   </si>
@@ -921,6 +921,12 @@
   </si>
   <si>
     <t>Review fields and types for new exception event</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Delivery and Opening dates are of DateTime type</t>
   </si>
 </sst>
 </file>
@@ -1949,7 +1955,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2024,10 +2030,21 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="5"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6">
+        <v>43399</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5"/>
@@ -6670,8 +6687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6983,7 +7000,7 @@
       </c>
       <c r="F8" s="73"/>
       <c r="G8" s="5" t="s">
-        <v>4</v>
+        <v>268</v>
       </c>
       <c r="H8" s="5"/>
       <c r="J8" s="5" t="s">
@@ -7006,7 +7023,7 @@
       </c>
       <c r="F9" s="73"/>
       <c r="G9" s="5" t="s">
-        <v>4</v>
+        <v>268</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" s="5" t="s">

</xml_diff>

<commit_message>
added the callback urls
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/projects/moj/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57568FC1-7D77-4A4B-9B9C-45C976AEEF15}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E4E34A-AD5F-1F4C-8D63-DCF3F2AEF73D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="272">
   <si>
     <t>Change History</t>
   </si>
@@ -878,9 +878,6 @@
     <t>openingDate</t>
   </si>
   <si>
-    <t>https://url.for.bulk.scan.orchestrator</t>
-  </si>
-  <si>
     <t>https://url.for.service.endpoint</t>
   </si>
   <si>
@@ -933,6 +930,9 @@
   </si>
   <si>
     <t>Changed scannedDate field in ScannedDocument complex type to DateTime type</t>
+  </si>
+  <si>
+    <t>http://host.docker.internal:8582/callback/attach_case</t>
   </si>
 </sst>
 </file>
@@ -1961,7 +1961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2007,7 +2007,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -2016,7 +2016,7 @@
         <v>43384</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2024,7 +2024,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -2033,7 +2033,7 @@
         <v>43399</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2041,7 +2041,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -2050,7 +2050,7 @@
         <v>43399</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -2058,7 +2058,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -2067,7 +2067,7 @@
         <v>43404</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>170</v>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>170</v>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>170</v>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>170</v>
@@ -2334,7 +2334,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="60" t="s">
         <v>170</v>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D9" s="60" t="s">
         <v>170</v>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>170</v>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>170</v>
@@ -2442,7 +2442,7 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D12" s="60" t="s">
         <v>170</v>
@@ -2576,7 +2576,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>213</v>
@@ -2615,7 +2615,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>252</v>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="B8" s="60"/>
       <c r="C8" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>223</v>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>231</v>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" t="s">
         <v>182</v>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>213</v>
@@ -2938,7 +2938,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>223</v>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>231</v>
@@ -3244,7 +3244,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" t="s">
         <v>182</v>
@@ -3283,7 +3283,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>213</v>
@@ -3322,7 +3322,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>223</v>
@@ -4289,10 +4289,10 @@
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>198</v>
@@ -4408,13 +4408,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F4" s="117" t="s">
         <v>198</v>
@@ -4425,13 +4425,13 @@
         <v>43101</v>
       </c>
       <c r="C5" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>215</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F5" s="119" t="s">
         <v>198</v>
@@ -4442,13 +4442,13 @@
         <v>43101</v>
       </c>
       <c r="C6" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F6" s="119" t="s">
         <v>198</v>
@@ -4459,13 +4459,13 @@
         <v>43101</v>
       </c>
       <c r="C7" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F7" s="119" t="s">
         <v>198</v>
@@ -4476,13 +4476,13 @@
         <v>43101</v>
       </c>
       <c r="C8" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>213</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F8" s="119" t="s">
         <v>198</v>
@@ -4493,13 +4493,13 @@
         <v>43101</v>
       </c>
       <c r="C9" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>252</v>
       </c>
       <c r="E9" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F9" s="119" t="s">
         <v>198</v>
@@ -4510,13 +4510,13 @@
         <v>43101</v>
       </c>
       <c r="C10" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F10" s="119" t="s">
         <v>198</v>
@@ -4527,13 +4527,13 @@
         <v>43101</v>
       </c>
       <c r="C11" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E11" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F11" s="119" t="s">
         <v>198</v>
@@ -4544,13 +4544,13 @@
         <v>43101</v>
       </c>
       <c r="C12" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>223</v>
       </c>
       <c r="E12" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F12" s="119" t="s">
         <v>198</v>
@@ -5396,13 +5396,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>219</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F4" s="117" t="s">
         <v>198</v>
@@ -5414,13 +5414,13 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>217</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F5" s="119" t="s">
         <v>198</v>
@@ -5432,13 +5432,13 @@
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>125</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F6" s="123" t="s">
         <v>198</v>
@@ -5450,13 +5450,13 @@
       </c>
       <c r="B7" s="122"/>
       <c r="C7" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F7" s="119" t="s">
         <v>198</v>
@@ -5468,13 +5468,13 @@
       </c>
       <c r="B8" s="124"/>
       <c r="C8" s="115" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>127</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F8" s="121" t="s">
         <v>198</v>
@@ -6336,13 +6336,13 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="136" t="s">
         <v>95</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F4" s="137" t="s">
         <v>198</v>
@@ -6354,13 +6354,13 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>240</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F5" s="138" t="s">
         <v>198</v>
@@ -6372,13 +6372,13 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>241</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F6" s="138" t="s">
         <v>198</v>
@@ -6390,13 +6390,13 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="139" t="s">
         <v>96</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F7" s="140" t="s">
         <v>198</v>
@@ -6408,13 +6408,13 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="139" t="s">
         <v>247</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F8" s="140" t="s">
         <v>198</v>
@@ -6530,13 +6530,13 @@
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>258</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -6674,14 +6674,14 @@
         <v>43101</v>
       </c>
       <c r="C4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>259</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>260</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -6912,7 +6912,7 @@
       </c>
       <c r="B4" s="50"/>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
@@ -6937,7 +6937,7 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>215</v>
@@ -6962,7 +6962,7 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
@@ -6985,7 +6985,7 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
@@ -7008,7 +7008,7 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>213</v>
@@ -7018,7 +7018,7 @@
       </c>
       <c r="F8" s="73"/>
       <c r="G8" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H8" s="5"/>
       <c r="J8" s="5" t="s">
@@ -7031,7 +7031,7 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>252</v>
@@ -7041,7 +7041,7 @@
       </c>
       <c r="F9" s="73"/>
       <c r="G9" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" s="5" t="s">
@@ -7054,7 +7054,7 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>56</v>
@@ -7079,7 +7079,7 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>59</v>
@@ -7104,7 +7104,7 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>223</v>
@@ -7377,7 +7377,7 @@
         <v>234</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>76</v>
@@ -7401,7 +7401,7 @@
         <v>234</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>77</v>
@@ -7431,7 +7431,7 @@
         <v>234</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>52</v>
@@ -7452,7 +7452,7 @@
         <v>234</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>52</v>
@@ -7473,10 +7473,10 @@
         <v>234</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
@@ -7651,7 +7651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C8"/>
     </sheetView>
   </sheetViews>
@@ -7757,7 +7757,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>95</v>
@@ -7778,7 +7778,7 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>240</v>
@@ -7799,7 +7799,7 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>241</v>
@@ -7819,7 +7819,7 @@
         <v>43101</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>96</v>
@@ -7839,7 +7839,7 @@
         <v>43101</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>247</v>
@@ -7878,8 +7878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8068,7 +8068,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>219</v>
@@ -8100,7 +8100,7 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>217</v>
@@ -8122,11 +8122,11 @@
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="L5" s="144" t="s">
+        <v>271</v>
+      </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="144" t="s">
-        <v>253</v>
-      </c>
+      <c r="N5" s="144"/>
       <c r="P5" s="51" t="s">
         <v>122</v>
       </c>
@@ -8143,7 +8143,7 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>218</v>
@@ -8166,12 +8166,10 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="144" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="144" t="s">
-        <v>254</v>
-      </c>
+      <c r="N6" s="144"/>
       <c r="P6" s="5" t="s">
         <v>122</v>
       </c>
@@ -8188,7 +8186,7 @@
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>125</v>
@@ -8229,7 +8227,7 @@
       </c>
       <c r="B8" s="71"/>
       <c r="C8" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>127</v>
@@ -8275,9 +8273,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="N6" r:id="rId1" xr:uid="{0AEF91E4-C31B-6948-8CA6-C50706B87B14}"/>
-    <hyperlink ref="N5" r:id="rId2" xr:uid="{52614C83-3AC1-0148-BC43-821E043636BC}"/>
-    <hyperlink ref="L6" r:id="rId3" xr:uid="{B25A138A-C0B9-AC4C-9B54-D281FFD0AE41}"/>
+    <hyperlink ref="L6" r:id="rId1" xr:uid="{B25A138A-C0B9-AC4C-9B54-D281FFD0AE41}"/>
+    <hyperlink ref="L5" r:id="rId2" xr:uid="{BD332970-043F-BE47-B1B2-E15775C88764}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -8453,7 +8450,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>217</v>
@@ -8487,7 +8484,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>217</v>
@@ -8521,7 +8518,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>125</v>
@@ -8555,7 +8552,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>125</v>
@@ -8589,7 +8586,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>218</v>
@@ -8623,7 +8620,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>218</v>
@@ -8657,7 +8654,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>127</v>
@@ -8687,7 +8684,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
added the callback url
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/projects/moj/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57568FC1-7D77-4A4B-9B9C-45C976AEEF15}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2627B5F0-6ECB-684C-968F-32FD0CCCC632}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="271">
   <si>
     <t>Change History</t>
   </si>
@@ -878,12 +878,6 @@
     <t>openingDate</t>
   </si>
   <si>
-    <t>https://url.for.bulk.scan.orchestrator</t>
-  </si>
-  <si>
-    <t>https://url.for.service.endpoint</t>
-  </si>
-  <si>
     <t>Initial definition file for Exception Record</t>
   </si>
   <si>
@@ -933,6 +927,9 @@
   </si>
   <si>
     <t>Changed scannedDate field in ScannedDocument complex type to DateTime type</t>
+  </si>
+  <si>
+    <t>${BULK_SCAN_ORCHESTRATOR_BASE_URL}/callback/attach_case</t>
   </si>
 </sst>
 </file>
@@ -1961,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2007,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -2016,7 +2013,7 @@
         <v>43384</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2024,7 +2021,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -2033,7 +2030,7 @@
         <v>43399</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2041,7 +2038,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -2050,7 +2047,7 @@
         <v>43399</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -2058,7 +2055,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -2067,7 +2064,7 @@
         <v>43404</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -2098,7 +2095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N1048545"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -2226,7 +2223,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>170</v>
@@ -2253,7 +2250,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>170</v>
@@ -2280,7 +2277,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>170</v>
@@ -2307,7 +2304,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>170</v>
@@ -2334,7 +2331,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D8" s="60" t="s">
         <v>170</v>
@@ -2361,7 +2358,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D9" s="60" t="s">
         <v>170</v>
@@ -2388,7 +2385,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>170</v>
@@ -2415,7 +2412,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>170</v>
@@ -2442,7 +2439,7 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D12" s="60" t="s">
         <v>170</v>
@@ -2497,7 +2494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2576,7 +2573,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>213</v>
@@ -2615,7 +2612,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>252</v>
@@ -2633,7 +2630,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
@@ -2651,7 +2648,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
@@ -2669,7 +2666,7 @@
       </c>
       <c r="B8" s="60"/>
       <c r="C8" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>223</v>
@@ -2744,7 +2741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView zoomScale="138" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C7"/>
     </sheetView>
   </sheetViews>
@@ -2837,7 +2834,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>231</v>
@@ -2860,7 +2857,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" t="s">
         <v>182</v>
@@ -2899,7 +2896,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>213</v>
@@ -2938,7 +2935,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>223</v>
@@ -2988,7 +2985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
@@ -3111,7 +3108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C7"/>
     </sheetView>
   </sheetViews>
@@ -3205,7 +3202,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>231</v>
@@ -3244,7 +3241,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" t="s">
         <v>182</v>
@@ -3283,7 +3280,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>213</v>
@@ -3322,7 +3319,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>223</v>
@@ -3368,7 +3365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -3470,7 +3467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:IU4"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -4289,10 +4286,10 @@
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="D4" s="51" t="s">
         <v>259</v>
-      </c>
-      <c r="D4" s="51" t="s">
-        <v>261</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>198</v>
@@ -4315,7 +4312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="136" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4408,13 +4405,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F4" s="117" t="s">
         <v>198</v>
@@ -4425,13 +4422,13 @@
         <v>43101</v>
       </c>
       <c r="C5" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>215</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F5" s="119" t="s">
         <v>198</v>
@@ -4442,13 +4439,13 @@
         <v>43101</v>
       </c>
       <c r="C6" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F6" s="119" t="s">
         <v>198</v>
@@ -4459,13 +4456,13 @@
         <v>43101</v>
       </c>
       <c r="C7" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F7" s="119" t="s">
         <v>198</v>
@@ -4476,13 +4473,13 @@
         <v>43101</v>
       </c>
       <c r="C8" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>213</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F8" s="119" t="s">
         <v>198</v>
@@ -4493,13 +4490,13 @@
         <v>43101</v>
       </c>
       <c r="C9" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>252</v>
       </c>
       <c r="E9" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F9" s="119" t="s">
         <v>198</v>
@@ -4510,13 +4507,13 @@
         <v>43101</v>
       </c>
       <c r="C10" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F10" s="119" t="s">
         <v>198</v>
@@ -4527,13 +4524,13 @@
         <v>43101</v>
       </c>
       <c r="C11" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E11" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F11" s="119" t="s">
         <v>198</v>
@@ -4544,13 +4541,13 @@
         <v>43101</v>
       </c>
       <c r="C12" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>223</v>
       </c>
       <c r="E12" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F12" s="119" t="s">
         <v>198</v>
@@ -4572,7 +4569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="166" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD13"/>
     </sheetView>
   </sheetViews>
@@ -5396,13 +5393,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>219</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F4" s="117" t="s">
         <v>198</v>
@@ -5414,13 +5411,13 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>217</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F5" s="119" t="s">
         <v>198</v>
@@ -5432,13 +5429,13 @@
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>125</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F6" s="123" t="s">
         <v>198</v>
@@ -5450,13 +5447,13 @@
       </c>
       <c r="B7" s="122"/>
       <c r="C7" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F7" s="119" t="s">
         <v>198</v>
@@ -5468,13 +5465,13 @@
       </c>
       <c r="B8" s="124"/>
       <c r="C8" s="115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>127</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F8" s="121" t="s">
         <v>198</v>
@@ -5511,7 +5508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -6336,13 +6333,13 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="136" t="s">
         <v>95</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F4" s="137" t="s">
         <v>198</v>
@@ -6354,13 +6351,13 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>240</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F5" s="138" t="s">
         <v>198</v>
@@ -6372,13 +6369,13 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>241</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F6" s="138" t="s">
         <v>198</v>
@@ -6390,13 +6387,13 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="139" t="s">
         <v>96</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F7" s="140" t="s">
         <v>198</v>
@@ -6408,13 +6405,13 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D8" s="139" t="s">
         <v>247</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F8" s="140" t="s">
         <v>198</v>
@@ -6445,7 +6442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -6530,13 +6527,13 @@
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -6559,7 +6556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -6674,14 +6671,14 @@
         <v>43101</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -6912,7 +6909,7 @@
       </c>
       <c r="B4" s="50"/>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
@@ -6937,7 +6934,7 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>215</v>
@@ -6962,7 +6959,7 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>211</v>
@@ -6985,7 +6982,7 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>212</v>
@@ -7008,7 +7005,7 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>213</v>
@@ -7018,7 +7015,7 @@
       </c>
       <c r="F8" s="73"/>
       <c r="G8" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H8" s="5"/>
       <c r="J8" s="5" t="s">
@@ -7031,7 +7028,7 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>252</v>
@@ -7041,7 +7038,7 @@
       </c>
       <c r="F9" s="73"/>
       <c r="G9" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" s="5" t="s">
@@ -7054,7 +7051,7 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>56</v>
@@ -7079,7 +7076,7 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>59</v>
@@ -7104,7 +7101,7 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>223</v>
@@ -7143,7 +7140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -7377,7 +7374,7 @@
         <v>234</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>76</v>
@@ -7401,7 +7398,7 @@
         <v>234</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>77</v>
@@ -7431,7 +7428,7 @@
         <v>234</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>52</v>
@@ -7452,7 +7449,7 @@
         <v>234</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>52</v>
@@ -7473,10 +7470,10 @@
         <v>234</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>266</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>268</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
@@ -7502,7 +7499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -7651,7 +7648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C8"/>
     </sheetView>
   </sheetViews>
@@ -7757,7 +7754,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>95</v>
@@ -7778,7 +7775,7 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>240</v>
@@ -7799,7 +7796,7 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>241</v>
@@ -7819,7 +7816,7 @@
         <v>43101</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>96</v>
@@ -7839,7 +7836,7 @@
         <v>43101</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>247</v>
@@ -7878,8 +7875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="J2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8068,7 +8065,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>219</v>
@@ -8100,7 +8097,7 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>217</v>
@@ -8125,7 +8122,7 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="144" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="P5" s="51" t="s">
         <v>122</v>
@@ -8143,7 +8140,7 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>218</v>
@@ -8165,13 +8162,9 @@
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="144" t="s">
-        <v>254</v>
-      </c>
+      <c r="L6" s="144"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="144" t="s">
-        <v>254</v>
-      </c>
+      <c r="N6" s="144"/>
       <c r="P6" s="5" t="s">
         <v>122</v>
       </c>
@@ -8188,7 +8181,7 @@
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>125</v>
@@ -8229,7 +8222,7 @@
       </c>
       <c r="B8" s="71"/>
       <c r="C8" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>127</v>
@@ -8274,11 +8267,6 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="N6" r:id="rId1" xr:uid="{0AEF91E4-C31B-6948-8CA6-C50706B87B14}"/>
-    <hyperlink ref="N5" r:id="rId2" xr:uid="{52614C83-3AC1-0148-BC43-821E043636BC}"/>
-    <hyperlink ref="L6" r:id="rId3" xr:uid="{B25A138A-C0B9-AC4C-9B54-D281FFD0AE41}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -8288,7 +8276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -8453,7 +8441,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>217</v>
@@ -8487,7 +8475,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>217</v>
@@ -8521,7 +8509,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>125</v>
@@ -8555,7 +8543,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>125</v>
@@ -8589,7 +8577,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>218</v>
@@ -8623,7 +8611,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>218</v>
@@ -8657,7 +8645,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>127</v>
@@ -8687,7 +8675,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
added the callback url to the env file.
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/projects/moj/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2627B5F0-6ECB-684C-968F-32FD0CCCC632}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93144524-C797-B74D-A1B6-29DBAA624589}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -929,7 +929,7 @@
     <t>Changed scannedDate field in ScannedDocument complex type to DateTime type</t>
   </si>
   <si>
-    <t>${BULK_SCAN_ORCHESTRATOR_BASE_URL}/callback/attach_case</t>
+    <t xml:space="preserve"> ${BULK_SCAN_ORCHESTRATOR_BASE_URL}/callback/attach_case</t>
   </si>
 </sst>
 </file>
@@ -1959,7 +1959,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2095,7 +2095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N1048545"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -2494,7 +2494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2741,7 +2741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="138" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C7"/>
     </sheetView>
   </sheetViews>
@@ -2985,7 +2985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
@@ -3108,7 +3108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C7"/>
     </sheetView>
   </sheetViews>
@@ -3365,7 +3365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -3467,7 +3467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:IU4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -4312,7 +4312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="136" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4569,7 +4569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="166" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD13"/>
     </sheetView>
   </sheetViews>
@@ -5508,7 +5508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -6442,7 +6442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -6556,7 +6556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -7140,7 +7140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -7499,7 +7499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -7648,7 +7648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C8"/>
     </sheetView>
   </sheetViews>
@@ -7875,8 +7875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="J2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView topLeftCell="K2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8119,11 +8119,11 @@
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="L5" s="144" t="s">
+        <v>270</v>
+      </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="144" t="s">
-        <v>270</v>
-      </c>
+      <c r="N5" s="144"/>
       <c r="P5" s="51" t="s">
         <v>122</v>
       </c>
@@ -8267,6 +8267,9 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="L5" r:id="rId1" display="http://host.docker.internal:8582/callback/attach_case" xr:uid="{DF74CB50-765D-A849-802D-91A6F9CAB12C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -8276,7 +8279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Refactored ccd definition for bulk scanning cases and exception records
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/projects/moj/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/Documents/ccd-dedinition-sheets-refactored/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93144524-C797-B74D-A1B6-29DBAA624589}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF9A28A-B7BD-0B44-9E3B-4B186476AFA7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="274">
   <si>
     <t>Change History</t>
   </si>
@@ -228,12 +228,6 @@
   </si>
   <si>
     <t>Case Reference</t>
-  </si>
-  <si>
-    <t>scanRecords</t>
-  </si>
-  <si>
-    <t>Scanned Records</t>
   </si>
   <si>
     <t>Collection</t>
@@ -827,18 +821,12 @@
     <t>Scanned Date</t>
   </si>
   <si>
-    <t>Scanned document url</t>
-  </si>
-  <si>
     <t>cherished</t>
   </si>
   <si>
     <t>Cherished</t>
   </si>
   <si>
-    <t>DocumentType</t>
-  </si>
-  <si>
     <t>ScannedRecordAttachedToCase</t>
   </si>
   <si>
@@ -878,6 +866,9 @@
     <t>openingDate</t>
   </si>
   <si>
+    <t>https://url.for.service.endpoint</t>
+  </si>
+  <si>
     <t>Initial definition file for Exception Record</t>
   </si>
   <si>
@@ -929,7 +920,25 @@
     <t>Changed scannedDate field in ScannedDocument complex type to DateTime type</t>
   </si>
   <si>
-    <t xml:space="preserve"> ${BULK_SCAN_ORCHESTRATOR_BASE_URL}/callback/attach_case</t>
+    <t>scannedDocuments</t>
+  </si>
+  <si>
+    <t>Scanned Documents</t>
+  </si>
+  <si>
+    <t>Document url</t>
+  </si>
+  <si>
+    <t>bulkscan+ccd@gmail.com</t>
+  </si>
+  <si>
+    <t>ScannedDocumentType</t>
+  </si>
+  <si>
+    <t>Refactored to add case fields and rename events</t>
+  </si>
+  <si>
+    <t>${BULK_SCAN_ORCHESTRATOR_BASE_URL}/callback/attach_case</t>
   </si>
 </sst>
 </file>
@@ -1958,8 +1967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2004,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -2013,7 +2022,7 @@
         <v>43384</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2021,7 +2030,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -2030,7 +2039,7 @@
         <v>43399</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2038,7 +2047,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -2047,7 +2056,7 @@
         <v>43399</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -2055,7 +2064,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -2064,15 +2073,25 @@
         <v>43404</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="145">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6">
+        <v>43420</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="7"/>
@@ -2096,7 +2115,7 @@
   <dimension ref="A1:N1048545"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2119,7 +2138,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="42" t="s">
@@ -2152,28 +2171,28 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="G2" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="H2" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="I2" s="85" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="J2" s="75" t="s">
         <v>160</v>
       </c>
-      <c r="I2" s="85" t="s">
+      <c r="K2" s="75" t="s">
         <v>161</v>
-      </c>
-      <c r="J2" s="75" t="s">
-        <v>162</v>
-      </c>
-      <c r="K2" s="75" t="s">
-        <v>163</v>
       </c>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
@@ -2190,28 +2209,28 @@
         <v>43</v>
       </c>
       <c r="D3" s="48" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" s="76" t="s">
         <v>164</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="G3" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="H3" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="76" t="s">
         <v>166</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="J3" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="76" t="s">
         <v>167</v>
-      </c>
-      <c r="H3" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" s="76" t="s">
-        <v>168</v>
-      </c>
-      <c r="J3" s="76" t="s">
-        <v>69</v>
-      </c>
-      <c r="K3" s="76" t="s">
-        <v>169</v>
       </c>
       <c r="L3" s="24"/>
       <c r="M3" s="24"/>
@@ -2223,22 +2242,22 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G4" s="86">
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I4" s="86">
         <v>1</v>
@@ -2250,22 +2269,22 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F5" s="60" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G5" s="86">
         <v>1</v>
       </c>
       <c r="H5" s="60" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I5" s="86">
         <v>2</v>
@@ -2277,22 +2296,22 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G6" s="86">
         <v>1</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I6" s="86">
         <v>3</v>
@@ -2304,22 +2323,22 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F7" s="60" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G7" s="86">
         <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I7" s="86">
         <v>4</v>
@@ -2331,22 +2350,22 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D8" s="60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F8" s="60" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G8" s="86">
         <v>1</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I8" s="86">
         <v>5</v>
@@ -2358,22 +2377,22 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D9" s="60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F9" s="60" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G9" s="86">
         <v>1</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I9" s="86">
         <v>6</v>
@@ -2385,22 +2404,22 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D10" s="60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F10" s="60" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G10" s="86">
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I10" s="86">
         <v>7</v>
@@ -2412,22 +2431,22 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D11" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" s="60" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="60" t="s">
         <v>170</v>
-      </c>
-      <c r="E11" s="60" t="s">
-        <v>171</v>
-      </c>
-      <c r="F11" s="60" t="s">
-        <v>172</v>
       </c>
       <c r="G11" s="86">
         <v>2</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>56</v>
+        <v>267</v>
       </c>
       <c r="I11" s="86">
         <v>1</v>
@@ -2439,28 +2458,28 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D12" s="60" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E12" s="60" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F12" s="60" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G12" s="86">
         <v>3</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I12" s="86">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
@@ -2495,7 +2514,7 @@
   <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2513,7 +2532,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B1" s="87" t="s">
         <v>8</v>
@@ -2538,13 +2557,13 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="67" t="s">
         <v>175</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:27" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2558,13 +2577,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -2573,10 +2592,10 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>54</v>
@@ -2612,13 +2631,13 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
@@ -2630,16 +2649,16 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>53</v>
       </c>
       <c r="F6" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
@@ -2648,16 +2667,16 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F7" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
@@ -2666,16 +2685,16 @@
       </c>
       <c r="B8" s="60"/>
       <c r="C8" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F8" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
@@ -2742,7 +2761,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView zoomScale="138" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2759,7 +2778,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -2789,13 +2808,13 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="67" t="s">
         <v>179</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>181</v>
       </c>
       <c r="G2" s="95"/>
       <c r="H2" s="95"/>
@@ -2814,13 +2833,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G3" s="96"/>
       <c r="H3" s="96"/>
@@ -2834,10 +2853,10 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>55</v>
@@ -2857,16 +2876,16 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="94"/>
       <c r="H5" s="94"/>
@@ -2896,16 +2915,16 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F6" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="94"/>
       <c r="H6" s="94"/>
@@ -2935,16 +2954,16 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F7" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.15">
@@ -3002,7 +3021,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="16" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="100" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B1" s="101" t="s">
         <v>8</v>
@@ -3027,13 +3046,13 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="67" t="s">
         <v>175</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3047,13 +3066,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3109,7 +3128,7 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3127,7 +3146,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="16" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -3157,13 +3176,13 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="67" t="s">
         <v>179</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>181</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -3182,13 +3201,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G3" s="96"/>
       <c r="H3" s="96"/>
@@ -3202,10 +3221,10 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>55</v>
@@ -3241,16 +3260,16 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="94"/>
       <c r="H5" s="94"/>
@@ -3280,16 +3299,16 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F6" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="94"/>
       <c r="H6" s="94"/>
@@ -3319,16 +3338,16 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F7" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
@@ -3366,7 +3385,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3382,7 +3401,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="16" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -3410,13 +3429,13 @@
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>186</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>188</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -3432,16 +3451,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="106" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="106" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="106" t="s">
+      <c r="F3" s="106" t="s">
         <v>190</v>
-      </c>
-      <c r="E3" s="106" t="s">
-        <v>191</v>
-      </c>
-      <c r="F3" s="106" t="s">
-        <v>192</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -3450,12 +3469,22 @@
       <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A4" s="25"/>
+      <c r="A4" s="25">
+        <v>43101</v>
+      </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
+      <c r="C4" s="107" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" s="60" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3468,7 +3497,7 @@
   <dimension ref="A1:IU4"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3483,7 +3512,7 @@
   <sheetData>
     <row r="1" spans="1:255" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -3754,13 +3783,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" s="34" t="s">
         <v>194</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>196</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -4024,10 +4053,10 @@
         <v>43</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -4286,13 +4315,13 @@
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F4" s="5"/>
     </row>
@@ -4313,7 +4342,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="136" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4331,7 +4360,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="108" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -4357,16 +4386,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G2" s="111"/>
       <c r="H2" s="111"/>
@@ -4385,13 +4414,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="113" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E3" s="113" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F3" s="112" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G3" s="110"/>
       <c r="H3" s="110"/>
@@ -4405,16 +4434,16 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F4" s="117" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
@@ -4422,16 +4451,16 @@
         <v>43101</v>
       </c>
       <c r="C5" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F5" s="119" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
@@ -4439,16 +4468,16 @@
         <v>43101</v>
       </c>
       <c r="C6" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F6" s="119" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
@@ -4456,16 +4485,16 @@
         <v>43101</v>
       </c>
       <c r="C7" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F7" s="119" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
@@ -4473,16 +4502,16 @@
         <v>43101</v>
       </c>
       <c r="C8" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F8" s="119" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -4490,16 +4519,16 @@
         <v>43101</v>
       </c>
       <c r="C9" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E9" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F9" s="119" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -4507,16 +4536,16 @@
         <v>43101</v>
       </c>
       <c r="C10" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>56</v>
+        <v>267</v>
       </c>
       <c r="E10" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F10" s="119" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
@@ -4524,16 +4553,16 @@
         <v>43101</v>
       </c>
       <c r="C11" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F11" s="119" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
@@ -4541,16 +4570,16 @@
         <v>43101</v>
       </c>
       <c r="C12" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E12" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F12" s="119" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4586,7 +4615,7 @@
   <sheetData>
     <row r="1" spans="1:255" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -4857,16 +4886,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>194</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>196</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -5129,13 +5158,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="113" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E3" s="113" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -5393,16 +5422,16 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F4" s="117" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:255" x14ac:dyDescent="0.15">
@@ -5411,16 +5440,16 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F5" s="119" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:255" x14ac:dyDescent="0.15">
@@ -5429,16 +5458,16 @@
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F6" s="123" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:255" x14ac:dyDescent="0.15">
@@ -5447,16 +5476,16 @@
       </c>
       <c r="B7" s="122"/>
       <c r="C7" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F7" s="119" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:255" x14ac:dyDescent="0.15">
@@ -5465,16 +5494,16 @@
       </c>
       <c r="B8" s="124"/>
       <c r="C8" s="115" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F8" s="121" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:255" x14ac:dyDescent="0.15">
@@ -5508,7 +5537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -5526,7 +5555,7 @@
   <sheetData>
     <row r="1" spans="1:255" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="127" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B1" s="128" t="s">
         <v>8</v>
@@ -5797,16 +5826,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D2" s="133" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G2" s="134"/>
       <c r="H2" s="134"/>
@@ -6069,13 +6098,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="113" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E3" s="113" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F3" s="135" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G3" s="132"/>
       <c r="H3" s="132"/>
@@ -6333,16 +6362,16 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="136" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F4" s="137" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:255" x14ac:dyDescent="0.15">
@@ -6351,16 +6380,16 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F5" s="138" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:255" x14ac:dyDescent="0.15">
@@ -6369,16 +6398,16 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F6" s="138" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:255" x14ac:dyDescent="0.15">
@@ -6387,16 +6416,16 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="139" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F7" s="140" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:255" x14ac:dyDescent="0.15">
@@ -6405,16 +6434,16 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D8" s="139" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F8" s="140" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:255" x14ac:dyDescent="0.15">
@@ -6442,8 +6471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="156" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6527,13 +6556,13 @@
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -6671,14 +6700,14 @@
         <v>43101</v>
       </c>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -6702,8 +6731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6909,13 +6938,13 @@
       </c>
       <c r="B4" s="50"/>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F4" s="73" t="s">
         <v>51</v>
@@ -6934,16 +6963,16 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>52</v>
@@ -6959,10 +6988,10 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>53</v>
@@ -6982,10 +7011,10 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>7</v>
@@ -7005,17 +7034,17 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F8" s="73"/>
       <c r="G8" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H8" s="5"/>
       <c r="J8" s="5" t="s">
@@ -7028,17 +7057,17 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F9" s="73"/>
       <c r="G9" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" s="5" t="s">
@@ -7051,20 +7080,20 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>56</v>
+        <v>267</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>57</v>
+        <v>268</v>
       </c>
       <c r="F10" s="73"/>
       <c r="G10" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>32</v>
@@ -7076,20 +7105,20 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F11" s="73"/>
       <c r="G11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>32</v>
@@ -7101,16 +7130,16 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F12" s="73" t="s">
         <v>222</v>
-      </c>
-      <c r="F12" s="73" t="s">
-        <v>224</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>52</v>
@@ -7141,7 +7170,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7165,7 +7194,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -7199,10 +7228,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>38</v>
@@ -7211,16 +7240,16 @@
         <v>39</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" s="34" t="s">
         <v>40</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K2" s="34" t="s">
         <v>27</v>
@@ -7248,7 +7277,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E3" s="53" t="s">
         <v>46</v>
@@ -7257,10 +7286,10 @@
         <v>47</v>
       </c>
       <c r="G3" s="53" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I3" s="53" t="s">
         <v>48</v>
@@ -7289,17 +7318,17 @@
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="56" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" s="57" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4" s="57" t="s">
         <v>52</v>
       </c>
       <c r="F4" s="58"/>
       <c r="G4" s="59" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -7320,17 +7349,17 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="61" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E5" s="62" t="s">
         <v>52</v>
       </c>
       <c r="F5" s="63"/>
       <c r="G5" s="64" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="60"/>
@@ -7350,17 +7379,17 @@
         <v>43101</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>44</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>57</v>
+        <v>268</v>
       </c>
       <c r="K6" s="60" t="s">
         <v>32</v>
@@ -7371,19 +7400,19 @@
         <v>43101</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K7" s="60" t="s">
         <v>32</v>
@@ -7395,17 +7424,17 @@
       </c>
       <c r="B8" s="55"/>
       <c r="C8" s="65" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>236</v>
+        <v>269</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="60"/>
@@ -7425,17 +7454,17 @@
         <v>43101</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F9" s="143"/>
       <c r="G9" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K9" s="60" t="s">
         <v>32</v>
@@ -7446,17 +7475,17 @@
         <v>43101</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K10" s="60" t="s">
         <v>32</v>
@@ -7467,17 +7496,17 @@
         <v>43101</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K11" s="60" t="s">
         <v>32</v>
@@ -7500,7 +7529,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7516,7 +7545,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -7542,13 +7571,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="34" t="s">
         <v>81</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>83</v>
       </c>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
@@ -7567,10 +7596,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
@@ -7584,13 +7613,13 @@
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="56" t="s">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="D4" s="57" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F4" s="60"/>
       <c r="H4" s="5"/>
@@ -7611,13 +7640,13 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="61" t="s">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" s="64" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F5" s="60"/>
       <c r="H5" s="5"/>
@@ -7648,8 +7677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C8"/>
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7668,7 +7697,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -7699,19 +7728,19 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="G2" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="G2" s="67" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>92</v>
       </c>
       <c r="I2" s="52"/>
       <c r="J2" s="52"/>
@@ -7738,10 +7767,10 @@
         <v>20</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -7754,16 +7783,16 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E4" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="F4" s="60" t="s">
         <v>207</v>
-      </c>
-      <c r="F4" s="60" t="s">
-        <v>209</v>
       </c>
       <c r="G4" s="72">
         <v>1</v>
@@ -7775,16 +7804,16 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" s="60" t="s">
+        <v>236</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" s="60" t="s">
         <v>240</v>
-      </c>
-      <c r="E5" s="60" t="s">
-        <v>242</v>
-      </c>
-      <c r="F5" s="60" t="s">
-        <v>244</v>
       </c>
       <c r="G5" s="72">
         <v>2</v>
@@ -7796,16 +7825,16 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" s="60" t="s">
         <v>241</v>
-      </c>
-      <c r="E6" s="60" t="s">
-        <v>243</v>
-      </c>
-      <c r="F6" s="60" t="s">
-        <v>245</v>
       </c>
       <c r="G6" s="72">
         <v>3</v>
@@ -7816,16 +7845,16 @@
         <v>43101</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="G7" s="72">
         <v>4</v>
@@ -7836,16 +7865,16 @@
         <v>43101</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G8" s="72">
         <v>5</v>
@@ -7875,8 +7904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="K2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="H2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7907,7 +7936,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -7946,55 +7975,55 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="J2" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="K2" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="75" t="s">
-        <v>104</v>
-      </c>
-      <c r="K2" s="34" t="s">
-        <v>105</v>
-      </c>
       <c r="L2" s="75" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N2" s="75" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P2" s="34" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="R2" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="R2" s="75" t="s">
+      <c r="T2" s="75" t="s">
         <v>107</v>
-      </c>
-      <c r="S2" s="75" t="s">
-        <v>108</v>
-      </c>
-      <c r="T2" s="75" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="16" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -8017,46 +8046,46 @@
         <v>20</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H3" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="77" t="s">
+      <c r="K3" s="76" t="s">
         <v>111</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="L3" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="M3" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="76" t="s">
+      <c r="N3" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="O3" s="76" t="s">
         <v>115</v>
-      </c>
-      <c r="N3" s="76" t="s">
-        <v>116</v>
-      </c>
-      <c r="O3" s="76" t="s">
-        <v>117</v>
       </c>
       <c r="P3" s="46" t="s">
         <v>31</v>
       </c>
       <c r="Q3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="R3" s="78" t="s">
+        <v>117</v>
+      </c>
+      <c r="S3" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="R3" s="78" t="s">
+      <c r="T3" s="78" t="s">
         <v>119</v>
-      </c>
-      <c r="S3" s="78" t="s">
-        <v>120</v>
-      </c>
-      <c r="T3" s="78" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.15">
@@ -8065,22 +8094,22 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G4" s="72">
         <v>1</v>
       </c>
       <c r="I4" s="60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -8088,7 +8117,7 @@
       <c r="M4" s="5"/>
       <c r="N4" s="80"/>
       <c r="P4" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.15">
@@ -8097,41 +8126,41 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G5" s="72">
         <v>2</v>
       </c>
       <c r="H5" s="60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I5" s="60" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="144" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="144"/>
       <c r="P5" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="S5" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.15">
@@ -8140,39 +8169,41 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G6" s="72">
         <v>3</v>
       </c>
       <c r="H6" s="60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I6" s="60" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="144"/>
+      <c r="L6" s="144" t="s">
+        <v>249</v>
+      </c>
       <c r="M6" s="5"/>
       <c r="N6" s="144"/>
       <c r="P6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R6" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="S6" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.15">
@@ -8181,25 +8212,25 @@
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G7" s="72">
         <v>4</v>
       </c>
       <c r="H7" s="60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -8207,13 +8238,13 @@
       <c r="M7" s="5"/>
       <c r="N7" s="144"/>
       <c r="P7" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R7" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="S7" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.15">
@@ -8222,38 +8253,38 @@
       </c>
       <c r="B8" s="71"/>
       <c r="C8" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G8" s="72">
         <v>5</v>
       </c>
       <c r="H8" s="60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="P8" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="S8" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
@@ -8268,7 +8299,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="L5" r:id="rId1" display="http://host.docker.internal:8582/callback/attach_case" xr:uid="{DF74CB50-765D-A849-802D-91A6F9CAB12C}"/>
+    <hyperlink ref="L6" r:id="rId1" xr:uid="{B25A138A-C0B9-AC4C-9B54-D281FFD0AE41}"/>
+    <hyperlink ref="L5" r:id="rId2" display="http://host.docker.internal:8582/callback/attach_case" xr:uid="{BD332970-043F-BE47-B1B2-E15775C88764}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -8279,8 +8311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="D1" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8306,7 +8338,7 @@
   <sheetData>
     <row r="1" spans="1:28" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -8342,40 +8374,40 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="H2" s="75" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="I2" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="J2" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="75" t="s">
+      <c r="K2" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="L2" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="M2" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="L2" s="75" t="s">
+      <c r="N2" s="75" t="s">
         <v>138</v>
       </c>
-      <c r="M2" s="75" t="s">
-        <v>139</v>
-      </c>
-      <c r="N2" s="75" t="s">
-        <v>140</v>
-      </c>
       <c r="O2" s="75" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="P2" s="81"/>
       <c r="Q2" s="81"/>
@@ -8402,40 +8434,40 @@
         <v>43</v>
       </c>
       <c r="D3" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="G3" s="76" t="s">
         <v>142</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="H3" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="I3" s="76" t="s">
         <v>144</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="J3" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="I3" s="76" t="s">
+      <c r="K3" s="76" t="s">
         <v>146</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="L3" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="83" t="s">
         <v>147</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="N3" s="76" t="s">
         <v>148</v>
       </c>
-      <c r="L3" s="76" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" s="83" t="s">
+      <c r="O3" s="76" t="s">
         <v>149</v>
-      </c>
-      <c r="N3" s="76" t="s">
-        <v>150</v>
-      </c>
-      <c r="O3" s="76" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8444,25 +8476,25 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F4" s="72">
         <v>1</v>
       </c>
       <c r="G4" s="84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H4" s="72">
         <v>1</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K4" s="72">
         <v>1</v>
@@ -8478,25 +8510,25 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>56</v>
+        <v>267</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H5" s="72">
         <v>1</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K5" s="72">
         <v>1</v>
@@ -8512,25 +8544,25 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F6" s="72">
         <v>1</v>
       </c>
       <c r="G6" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H6" s="72">
         <v>1</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K6" s="72">
         <v>1</v>
@@ -8546,25 +8578,25 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>56</v>
+        <v>267</v>
       </c>
       <c r="F7" s="72">
         <v>2</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H7" s="72">
         <v>1</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K7" s="72">
         <v>1</v>
@@ -8580,25 +8612,25 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>56</v>
+        <v>267</v>
       </c>
       <c r="F8" s="72">
         <v>1</v>
       </c>
       <c r="G8" s="84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H8" s="72">
         <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K8" s="72">
         <v>1</v>
@@ -8614,25 +8646,25 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F9" s="72">
         <v>2</v>
       </c>
       <c r="G9" s="84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H9" s="72">
         <v>1</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K9" s="72">
         <v>1</v>
@@ -8648,25 +8680,25 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D10" s="60" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>56</v>
+        <v>267</v>
       </c>
       <c r="F10" s="72">
         <v>1</v>
       </c>
       <c r="G10" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H10" s="72">
         <v>1</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K10" s="72">
         <v>1</v>
@@ -8678,25 +8710,25 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D11" s="60" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" s="72">
         <v>2</v>
       </c>
       <c r="G11" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H11" s="72">
         <v>1</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K11" s="72">
         <v>1</v>

</xml_diff>

<commit_message>
Renamed Case reference label as Exception reference in SearchResultsFields tab and WorkBasketResultFields tab
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/Documents/ccd-dedinition-sheets-refactored/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF9A28A-B7BD-0B44-9E3B-4B186476AFA7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B065B8-248A-B24F-8B31-025246BD5735}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,9 +227,6 @@
     <t>Delivery Date</t>
   </si>
   <si>
-    <t>Case Reference</t>
-  </si>
-  <si>
     <t>Collection</t>
   </si>
   <si>
@@ -938,7 +935,10 @@
     <t>Refactored to add case fields and rename events</t>
   </si>
   <si>
-    <t>${BULK_SCAN_ORCHESTRATOR_BASE_URL}/callback/attach_case</t>
+    <t>Exception Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ${BULK_SCAN_ORCHESTRATOR_BASE_URL}/callback/attach_case</t>
   </si>
 </sst>
 </file>
@@ -2013,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -2022,7 +2022,7 @@
         <v>43384</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2030,7 +2030,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -2039,7 +2039,7 @@
         <v>43399</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2047,7 +2047,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -2056,7 +2056,7 @@
         <v>43399</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -2064,7 +2064,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -2073,7 +2073,7 @@
         <v>43404</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -2081,7 +2081,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -2090,7 +2090,7 @@
         <v>43420</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -2138,7 +2138,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="42" t="s">
@@ -2171,28 +2171,28 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="G2" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="H2" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="I2" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="I2" s="85" t="s">
+      <c r="J2" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="K2" s="75" t="s">
         <v>160</v>
-      </c>
-      <c r="K2" s="75" t="s">
-        <v>161</v>
       </c>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
@@ -2209,28 +2209,28 @@
         <v>43</v>
       </c>
       <c r="D3" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="F3" s="76" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="G3" s="76" t="s">
         <v>164</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="H3" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="H3" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="I3" s="76" t="s">
+      <c r="J3" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="76" t="s">
         <v>166</v>
-      </c>
-      <c r="J3" s="76" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" s="76" t="s">
-        <v>167</v>
       </c>
       <c r="L3" s="24"/>
       <c r="M3" s="24"/>
@@ -2242,22 +2242,22 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G4" s="86">
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I4" s="86">
         <v>1</v>
@@ -2269,22 +2269,22 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F5" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G5" s="86">
         <v>1</v>
       </c>
       <c r="H5" s="60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I5" s="86">
         <v>2</v>
@@ -2296,22 +2296,22 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G6" s="86">
         <v>1</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I6" s="86">
         <v>3</v>
@@ -2323,22 +2323,22 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F7" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G7" s="86">
         <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I7" s="86">
         <v>4</v>
@@ -2350,22 +2350,22 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F8" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G8" s="86">
         <v>1</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I8" s="86">
         <v>5</v>
@@ -2377,22 +2377,22 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D9" s="60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F9" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G9" s="86">
         <v>1</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I9" s="86">
         <v>6</v>
@@ -2404,22 +2404,22 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D10" s="60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F10" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G10" s="86">
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I10" s="86">
         <v>7</v>
@@ -2431,22 +2431,22 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D11" s="60" t="s">
+        <v>167</v>
+      </c>
+      <c r="E11" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="F11" s="60" t="s">
         <v>169</v>
-      </c>
-      <c r="F11" s="60" t="s">
-        <v>170</v>
       </c>
       <c r="G11" s="86">
         <v>2</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I11" s="86">
         <v>1</v>
@@ -2458,28 +2458,28 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D12" s="60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E12" s="60" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F12" s="60" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G12" s="86">
         <v>3</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I12" s="86">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
@@ -2513,7 +2513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -2532,7 +2532,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B1" s="87" t="s">
         <v>8</v>
@@ -2557,13 +2557,13 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="67" t="s">
         <v>174</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:27" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2577,13 +2577,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -2592,10 +2592,10 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>54</v>
@@ -2631,13 +2631,13 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
@@ -2649,10 +2649,10 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>53</v>
@@ -2667,13 +2667,13 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>
@@ -2685,13 +2685,13 @@
       </c>
       <c r="B8" s="60"/>
       <c r="C8" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F8" s="2">
         <v>5</v>
@@ -2761,7 +2761,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView zoomScale="138" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2778,7 +2778,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -2808,13 +2808,13 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="67" t="s">
         <v>178</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>179</v>
       </c>
       <c r="G2" s="95"/>
       <c r="H2" s="95"/>
@@ -2833,13 +2833,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G3" s="96"/>
       <c r="H3" s="96"/>
@@ -2853,13 +2853,13 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>55</v>
+        <v>272</v>
       </c>
       <c r="F4" s="141">
         <v>1</v>
@@ -2876,13 +2876,13 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
@@ -2915,10 +2915,10 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>54</v>
@@ -2954,13 +2954,13 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>
@@ -3004,7 +3004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
@@ -3021,7 +3021,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="16" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="100" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" s="101" t="s">
         <v>8</v>
@@ -3046,13 +3046,13 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="67" t="s">
         <v>174</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3066,13 +3066,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3128,7 +3128,7 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3146,7 +3146,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="16" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -3176,13 +3176,13 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="67" t="s">
         <v>178</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>179</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -3201,13 +3201,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G3" s="96"/>
       <c r="H3" s="96"/>
@@ -3221,13 +3221,13 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>55</v>
+        <v>272</v>
       </c>
       <c r="F4" s="141">
         <v>1</v>
@@ -3260,13 +3260,13 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
@@ -3299,10 +3299,10 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>54</v>
@@ -3338,13 +3338,13 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>
@@ -3385,7 +3385,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3401,7 +3401,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="16" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -3429,13 +3429,13 @@
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>185</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>186</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -3451,16 +3451,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="106" t="s">
         <v>187</v>
       </c>
-      <c r="D3" s="106" t="s">
+      <c r="E3" s="106" t="s">
         <v>188</v>
       </c>
-      <c r="E3" s="106" t="s">
+      <c r="F3" s="106" t="s">
         <v>189</v>
-      </c>
-      <c r="F3" s="106" t="s">
-        <v>190</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -3474,16 +3474,16 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="107" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3512,7 +3512,7 @@
   <sheetData>
     <row r="1" spans="1:255" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -3783,13 +3783,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="34" t="s">
         <v>193</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>194</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -4053,10 +4053,10 @@
         <v>43</v>
       </c>
       <c r="D3" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="21" t="s">
         <v>195</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>196</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -4315,13 +4315,13 @@
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F4" s="5"/>
     </row>
@@ -4360,7 +4360,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="108" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -4386,16 +4386,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>199</v>
-      </c>
       <c r="E2" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>193</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>194</v>
       </c>
       <c r="G2" s="111"/>
       <c r="H2" s="111"/>
@@ -4414,13 +4414,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="113" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" s="113" t="s">
+        <v>194</v>
+      </c>
+      <c r="F3" s="112" t="s">
         <v>195</v>
-      </c>
-      <c r="F3" s="112" t="s">
-        <v>196</v>
       </c>
       <c r="G3" s="110"/>
       <c r="H3" s="110"/>
@@ -4434,16 +4434,16 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F4" s="117" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
@@ -4451,16 +4451,16 @@
         <v>43101</v>
       </c>
       <c r="C5" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F5" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
@@ -4468,16 +4468,16 @@
         <v>43101</v>
       </c>
       <c r="C6" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F6" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
@@ -4485,16 +4485,16 @@
         <v>43101</v>
       </c>
       <c r="C7" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F7" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
@@ -4502,16 +4502,16 @@
         <v>43101</v>
       </c>
       <c r="C8" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F8" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -4519,16 +4519,16 @@
         <v>43101</v>
       </c>
       <c r="C9" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E9" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -4536,16 +4536,16 @@
         <v>43101</v>
       </c>
       <c r="C10" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E10" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F10" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
@@ -4553,16 +4553,16 @@
         <v>43101</v>
       </c>
       <c r="C11" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F11" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
@@ -4570,16 +4570,16 @@
         <v>43101</v>
       </c>
       <c r="C12" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E12" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F12" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -4615,7 +4615,7 @@
   <sheetData>
     <row r="1" spans="1:255" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -4886,16 +4886,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="34" t="s">
         <v>193</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>194</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -5158,13 +5158,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="113" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" s="113" t="s">
+        <v>194</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>195</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>196</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -5422,16 +5422,16 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F4" s="117" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:255" x14ac:dyDescent="0.15">
@@ -5440,16 +5440,16 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F5" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:255" x14ac:dyDescent="0.15">
@@ -5458,16 +5458,16 @@
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F6" s="123" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:255" x14ac:dyDescent="0.15">
@@ -5476,16 +5476,16 @@
       </c>
       <c r="B7" s="122"/>
       <c r="C7" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F7" s="119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:255" x14ac:dyDescent="0.15">
@@ -5494,16 +5494,16 @@
       </c>
       <c r="B8" s="124"/>
       <c r="C8" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F8" s="121" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:255" x14ac:dyDescent="0.15">
@@ -5555,7 +5555,7 @@
   <sheetData>
     <row r="1" spans="1:255" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="127" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B1" s="128" t="s">
         <v>8</v>
@@ -5826,16 +5826,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D2" s="133" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>193</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>194</v>
       </c>
       <c r="G2" s="134"/>
       <c r="H2" s="134"/>
@@ -6098,13 +6098,13 @@
         <v>43</v>
       </c>
       <c r="D3" s="113" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E3" s="113" t="s">
+        <v>194</v>
+      </c>
+      <c r="F3" s="135" t="s">
         <v>195</v>
-      </c>
-      <c r="F3" s="135" t="s">
-        <v>196</v>
       </c>
       <c r="G3" s="132"/>
       <c r="H3" s="132"/>
@@ -6362,16 +6362,16 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="136" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F4" s="137" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:255" x14ac:dyDescent="0.15">
@@ -6380,16 +6380,16 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F5" s="138" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:255" x14ac:dyDescent="0.15">
@@ -6398,16 +6398,16 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F6" s="138" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:255" x14ac:dyDescent="0.15">
@@ -6416,16 +6416,16 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="139" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F7" s="140" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:255" x14ac:dyDescent="0.15">
@@ -6434,16 +6434,16 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="139" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F8" s="140" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:255" x14ac:dyDescent="0.15">
@@ -6556,13 +6556,13 @@
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>253</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -6700,14 +6700,14 @@
         <v>43101</v>
       </c>
       <c r="C4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>255</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -6732,7 +6732,7 @@
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6938,13 +6938,13 @@
       </c>
       <c r="B4" s="50"/>
       <c r="C4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F4" s="73" t="s">
         <v>51</v>
@@ -6963,16 +6963,16 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="E5" s="60" t="s">
-        <v>214</v>
-      </c>
       <c r="F5" s="73" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>52</v>
@@ -6988,10 +6988,10 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>53</v>
@@ -7011,10 +7011,10 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>7</v>
@@ -7034,17 +7034,17 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F8" s="73"/>
       <c r="G8" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H8" s="5"/>
       <c r="J8" s="5" t="s">
@@ -7057,17 +7057,17 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F9" s="73"/>
       <c r="G9" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" s="5" t="s">
@@ -7080,20 +7080,20 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>268</v>
       </c>
       <c r="F10" s="73"/>
       <c r="G10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>32</v>
@@ -7105,20 +7105,20 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F11" s="73"/>
       <c r="G11" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>32</v>
@@ -7130,16 +7130,16 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F12" s="73" t="s">
         <v>221</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="F12" s="73" t="s">
-        <v>222</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>52</v>
@@ -7194,7 +7194,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -7228,10 +7228,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>60</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>61</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>38</v>
@@ -7240,16 +7240,16 @@
         <v>39</v>
       </c>
       <c r="G2" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>62</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>63</v>
       </c>
       <c r="I2" s="34" t="s">
         <v>40</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K2" s="34" t="s">
         <v>27</v>
@@ -7277,7 +7277,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="53" t="s">
         <v>46</v>
@@ -7286,10 +7286,10 @@
         <v>47</v>
       </c>
       <c r="G3" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="53" t="s">
         <v>66</v>
-      </c>
-      <c r="H3" s="53" t="s">
-        <v>67</v>
       </c>
       <c r="I3" s="53" t="s">
         <v>48</v>
@@ -7318,17 +7318,17 @@
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="57" t="s">
         <v>52</v>
       </c>
       <c r="F4" s="58"/>
       <c r="G4" s="59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -7349,17 +7349,17 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="62" t="s">
         <v>52</v>
       </c>
       <c r="F5" s="63"/>
       <c r="G5" s="64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="60"/>
@@ -7379,17 +7379,17 @@
         <v>43101</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>44</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K6" s="60" t="s">
         <v>32</v>
@@ -7400,19 +7400,19 @@
         <v>43101</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K7" s="60" t="s">
         <v>32</v>
@@ -7424,17 +7424,17 @@
       </c>
       <c r="B8" s="55"/>
       <c r="C8" s="65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="60"/>
@@ -7454,17 +7454,17 @@
         <v>43101</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F9" s="143"/>
       <c r="G9" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K9" s="60" t="s">
         <v>32</v>
@@ -7475,17 +7475,17 @@
         <v>43101</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K10" s="60" t="s">
         <v>32</v>
@@ -7496,17 +7496,17 @@
         <v>43101</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K11" s="60" t="s">
         <v>32</v>
@@ -7545,7 +7545,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -7571,13 +7571,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="E2" s="34" t="s">
         <v>80</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>81</v>
       </c>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
@@ -7596,10 +7596,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
@@ -7613,13 +7613,13 @@
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="56" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D4" s="57" t="s">
+        <v>233</v>
+      </c>
+      <c r="E4" s="59" t="s">
         <v>234</v>
-      </c>
-      <c r="E4" s="59" t="s">
-        <v>235</v>
       </c>
       <c r="F4" s="60"/>
       <c r="H4" s="5"/>
@@ -7640,13 +7640,13 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="61" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D5" s="62" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="64" t="s">
         <v>83</v>
-      </c>
-      <c r="E5" s="64" t="s">
-        <v>84</v>
       </c>
       <c r="F5" s="60"/>
       <c r="H5" s="5"/>
@@ -7697,7 +7697,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -7728,19 +7728,19 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="H2" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>90</v>
       </c>
       <c r="I2" s="52"/>
       <c r="J2" s="52"/>
@@ -7767,10 +7767,10 @@
         <v>20</v>
       </c>
       <c r="G3" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>91</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>92</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -7783,16 +7783,16 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G4" s="72">
         <v>1</v>
@@ -7804,16 +7804,16 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F5" s="60" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G5" s="72">
         <v>2</v>
@@ -7825,16 +7825,16 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G6" s="72">
         <v>3</v>
@@ -7845,16 +7845,16 @@
         <v>43101</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G7" s="72">
         <v>4</v>
@@ -7865,16 +7865,16 @@
         <v>43101</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>245</v>
       </c>
       <c r="G8" s="72">
         <v>5</v>
@@ -7904,7 +7904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -7936,7 +7936,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -7975,55 +7975,55 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="K2" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="K2" s="34" t="s">
-        <v>103</v>
-      </c>
       <c r="L2" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="M2" s="34" t="s">
-        <v>103</v>
-      </c>
       <c r="N2" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="34" t="s">
         <v>102</v>
-      </c>
-      <c r="O2" s="34" t="s">
-        <v>103</v>
       </c>
       <c r="P2" s="34" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="R2" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="R2" s="75" t="s">
+      <c r="S2" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="S2" s="75" t="s">
+      <c r="T2" s="75" t="s">
         <v>106</v>
-      </c>
-      <c r="T2" s="75" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="16" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -8046,46 +8046,46 @@
         <v>20</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="77" t="s">
+      <c r="J3" s="76" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="K3" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="L3" s="76" t="s">
         <v>111</v>
       </c>
-      <c r="L3" s="76" t="s">
+      <c r="M3" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="N3" s="76" t="s">
         <v>113</v>
       </c>
-      <c r="N3" s="76" t="s">
+      <c r="O3" s="76" t="s">
         <v>114</v>
-      </c>
-      <c r="O3" s="76" t="s">
-        <v>115</v>
       </c>
       <c r="P3" s="46" t="s">
         <v>31</v>
       </c>
       <c r="Q3" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="R3" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="R3" s="78" t="s">
+      <c r="S3" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="S3" s="78" t="s">
+      <c r="T3" s="78" t="s">
         <v>118</v>
-      </c>
-      <c r="T3" s="78" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.15">
@@ -8094,22 +8094,22 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" t="s">
         <v>217</v>
       </c>
-      <c r="E4" t="s">
-        <v>218</v>
-      </c>
       <c r="F4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G4" s="72">
         <v>1</v>
       </c>
       <c r="I4" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -8117,7 +8117,7 @@
       <c r="M4" s="5"/>
       <c r="N4" s="80"/>
       <c r="P4" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.15">
@@ -8126,25 +8126,25 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G5" s="72">
         <v>2</v>
       </c>
       <c r="H5" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I5" s="60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -8154,13 +8154,13 @@
       <c r="M5" s="5"/>
       <c r="N5" s="144"/>
       <c r="P5" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.15">
@@ -8169,41 +8169,41 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G6" s="72">
         <v>3</v>
       </c>
       <c r="H6" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I6" s="60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="144" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="144"/>
       <c r="P6" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.15">
@@ -8212,25 +8212,25 @@
       </c>
       <c r="B7" s="71"/>
       <c r="C7" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G7" s="72">
         <v>4</v>
       </c>
       <c r="H7" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -8238,13 +8238,13 @@
       <c r="M7" s="5"/>
       <c r="N7" s="144"/>
       <c r="P7" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.15">
@@ -8253,34 +8253,34 @@
       </c>
       <c r="B8" s="71"/>
       <c r="C8" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" t="s">
         <v>125</v>
       </c>
-      <c r="E8" t="s">
-        <v>126</v>
-      </c>
       <c r="F8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G8" s="72">
         <v>5</v>
       </c>
       <c r="H8" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P8" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -8300,7 +8300,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="L6" r:id="rId1" xr:uid="{B25A138A-C0B9-AC4C-9B54-D281FFD0AE41}"/>
-    <hyperlink ref="L5" r:id="rId2" display="http://host.docker.internal:8582/callback/attach_case" xr:uid="{BD332970-043F-BE47-B1B2-E15775C88764}"/>
+    <hyperlink ref="L5" r:id="rId2" display="http://bulk-scan-orchestrator-demo.service.core-compute-demo.internal/callback/attach_case" xr:uid="{BD332970-043F-BE47-B1B2-E15775C88764}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -8338,7 +8338,7 @@
   <sheetData>
     <row r="1" spans="1:28" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>8</v>
@@ -8374,40 +8374,40 @@
         <v>34</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="I2" s="75" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="75" t="s">
+      <c r="J2" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="75" t="s">
         <v>135</v>
       </c>
-      <c r="L2" s="75" t="s">
+      <c r="M2" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="M2" s="75" t="s">
+      <c r="N2" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="N2" s="75" t="s">
-        <v>138</v>
-      </c>
       <c r="O2" s="75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P2" s="81"/>
       <c r="Q2" s="81"/>
@@ -8434,40 +8434,40 @@
         <v>43</v>
       </c>
       <c r="D3" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="F3" s="76" t="s">
         <v>140</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="G3" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="H3" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="I3" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="I3" s="76" t="s">
+      <c r="J3" s="76" t="s">
         <v>144</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="K3" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="L3" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" s="83" t="s">
         <v>146</v>
       </c>
-      <c r="L3" s="76" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="83" t="s">
+      <c r="N3" s="76" t="s">
         <v>147</v>
       </c>
-      <c r="N3" s="76" t="s">
+      <c r="O3" s="76" t="s">
         <v>148</v>
-      </c>
-      <c r="O3" s="76" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8476,25 +8476,25 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F4" s="72">
         <v>1</v>
       </c>
       <c r="G4" s="84" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H4" s="72">
         <v>1</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K4" s="72">
         <v>1</v>
@@ -8510,25 +8510,25 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H5" s="72">
         <v>1</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K5" s="72">
         <v>1</v>
@@ -8544,25 +8544,25 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="72">
         <v>1</v>
       </c>
       <c r="G6" s="51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H6" s="72">
         <v>1</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K6" s="72">
         <v>1</v>
@@ -8578,25 +8578,25 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F7" s="72">
         <v>2</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H7" s="72">
         <v>1</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K7" s="72">
         <v>1</v>
@@ -8612,25 +8612,25 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F8" s="72">
         <v>1</v>
       </c>
       <c r="G8" s="84" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H8" s="72">
         <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K8" s="72">
         <v>1</v>
@@ -8646,25 +8646,25 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="72">
         <v>2</v>
       </c>
       <c r="G9" s="84" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H9" s="72">
         <v>1</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K9" s="72">
         <v>1</v>
@@ -8680,25 +8680,25 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D10" s="60" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F10" s="72">
         <v>1</v>
       </c>
       <c r="G10" s="51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H10" s="72">
         <v>1</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K10" s="72">
         <v>1</v>
@@ -8710,25 +8710,25 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D11" s="60" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="72">
         <v>2</v>
       </c>
       <c r="G11" s="51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H11" s="72">
         <v>1</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K11" s="72">
         <v>1</v>

</xml_diff>

<commit_message>
BPS-403 Renamed exception record case type
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B065B8-248A-B24F-8B31-025246BD5735}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD27AE1-93A5-B744-A802-C2A61BEC6F88}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="275">
   <si>
     <t>Change History</t>
   </si>
@@ -878,9 +878,6 @@
     <t>Bulk Scanning</t>
   </si>
   <si>
-    <t>ExceptionRecord</t>
-  </si>
-  <si>
     <t>Exception Record</t>
   </si>
   <si>
@@ -939,6 +936,12 @@
   </si>
   <si>
     <t xml:space="preserve"> ${BULK_SCAN_ORCHESTRATOR_BASE_URL}/callback/attach_case</t>
+  </si>
+  <si>
+    <t>BULKSCAN_ExceptionRecord</t>
+  </si>
+  <si>
+    <t>Renamed exception record case type</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1314,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1534,7 +1537,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1968,7 +1970,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2030,7 +2032,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -2047,7 +2049,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -2060,11 +2062,11 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="145">
+      <c r="A7" s="144">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -2073,15 +2075,15 @@
         <v>43404</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="145">
+      <c r="A8" s="144">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -2090,15 +2092,25 @@
         <v>43420</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="8"/>
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="9">
+        <v>43441</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>263</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -2115,7 +2127,7 @@
   <dimension ref="A1:N1048545"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2241,8 +2253,8 @@
         <v>43101</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="60" t="s">
-        <v>253</v>
+      <c r="C4" t="s">
+        <v>273</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>167</v>
@@ -2268,8 +2280,8 @@
         <v>43101</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="60" t="s">
-        <v>253</v>
+      <c r="C5" t="s">
+        <v>273</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>167</v>
@@ -2295,8 +2307,8 @@
         <v>43101</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="60" t="s">
-        <v>253</v>
+      <c r="C6" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>167</v>
@@ -2322,8 +2334,8 @@
         <v>43101</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="60" t="s">
-        <v>253</v>
+      <c r="C7" t="s">
+        <v>273</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>167</v>
@@ -2349,8 +2361,8 @@
         <v>43101</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="60" t="s">
-        <v>253</v>
+      <c r="C8" t="s">
+        <v>273</v>
       </c>
       <c r="D8" s="60" t="s">
         <v>167</v>
@@ -2376,8 +2388,8 @@
         <v>43101</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="60" t="s">
-        <v>253</v>
+      <c r="C9" t="s">
+        <v>273</v>
       </c>
       <c r="D9" s="60" t="s">
         <v>167</v>
@@ -2403,8 +2415,8 @@
         <v>43101</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="60" t="s">
-        <v>253</v>
+      <c r="C10" t="s">
+        <v>273</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>167</v>
@@ -2430,8 +2442,8 @@
         <v>43101</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="60" t="s">
-        <v>253</v>
+      <c r="C11" t="s">
+        <v>273</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>167</v>
@@ -2446,7 +2458,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I11" s="86">
         <v>1</v>
@@ -2457,8 +2469,8 @@
         <v>43101</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="60" t="s">
-        <v>253</v>
+      <c r="C12" t="s">
+        <v>273</v>
       </c>
       <c r="D12" s="60" t="s">
         <v>167</v>
@@ -2513,8 +2525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2591,8 +2603,8 @@
         <v>43101</v>
       </c>
       <c r="B4" s="60"/>
-      <c r="C4" s="60" t="s">
-        <v>253</v>
+      <c r="C4" t="s">
+        <v>273</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>210</v>
@@ -2630,8 +2642,8 @@
         <v>43101</v>
       </c>
       <c r="B5" s="60"/>
-      <c r="C5" s="60" t="s">
-        <v>253</v>
+      <c r="C5" t="s">
+        <v>273</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>247</v>
@@ -2648,8 +2660,8 @@
         <v>43101</v>
       </c>
       <c r="B6" s="60"/>
-      <c r="C6" s="60" t="s">
-        <v>253</v>
+      <c r="C6" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
@@ -2666,8 +2678,8 @@
         <v>43101</v>
       </c>
       <c r="B7" s="60"/>
-      <c r="C7" s="60" t="s">
-        <v>253</v>
+      <c r="C7" t="s">
+        <v>273</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>209</v>
@@ -2684,8 +2696,8 @@
         <v>43101</v>
       </c>
       <c r="B8" s="60"/>
-      <c r="C8" s="60" t="s">
-        <v>253</v>
+      <c r="C8" t="s">
+        <v>273</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>220</v>
@@ -2761,7 +2773,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView zoomScale="138" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2852,16 +2864,16 @@
         <v>43101</v>
       </c>
       <c r="B4" s="60"/>
-      <c r="C4" s="60" t="s">
-        <v>253</v>
+      <c r="C4" t="s">
+        <v>273</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>228</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="F4" s="141">
+        <v>271</v>
+      </c>
+      <c r="F4" s="140">
         <v>1</v>
       </c>
       <c r="G4" s="96"/>
@@ -2875,8 +2887,8 @@
         <v>43101</v>
       </c>
       <c r="B5" s="60"/>
-      <c r="C5" s="60" t="s">
-        <v>253</v>
+      <c r="C5" t="s">
+        <v>273</v>
       </c>
       <c r="D5" t="s">
         <v>179</v>
@@ -2914,8 +2926,8 @@
         <v>43101</v>
       </c>
       <c r="B6" s="60"/>
-      <c r="C6" s="60" t="s">
-        <v>253</v>
+      <c r="C6" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>210</v>
@@ -2953,8 +2965,8 @@
         <v>43101</v>
       </c>
       <c r="B7" s="60"/>
-      <c r="C7" s="60" t="s">
-        <v>253</v>
+      <c r="C7" t="s">
+        <v>273</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>220</v>
@@ -3004,7 +3016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
@@ -3128,7 +3140,7 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3220,16 +3232,16 @@
         <v>43101</v>
       </c>
       <c r="B4" s="60"/>
-      <c r="C4" s="60" t="s">
-        <v>253</v>
+      <c r="C4" t="s">
+        <v>273</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>228</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="F4" s="141">
+        <v>271</v>
+      </c>
+      <c r="F4" s="140">
         <v>1</v>
       </c>
       <c r="G4" s="97"/>
@@ -3259,8 +3271,8 @@
         <v>43101</v>
       </c>
       <c r="B5" s="60"/>
-      <c r="C5" s="60" t="s">
-        <v>253</v>
+      <c r="C5" t="s">
+        <v>273</v>
       </c>
       <c r="D5" t="s">
         <v>179</v>
@@ -3298,8 +3310,8 @@
         <v>43101</v>
       </c>
       <c r="B6" s="60"/>
-      <c r="C6" s="60" t="s">
-        <v>253</v>
+      <c r="C6" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>210</v>
@@ -3337,8 +3349,8 @@
         <v>43101</v>
       </c>
       <c r="B7" s="60"/>
-      <c r="C7" s="60" t="s">
-        <v>253</v>
+      <c r="C7" t="s">
+        <v>273</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>220</v>
@@ -3385,7 +3397,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3474,13 +3486,13 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="107" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>253</v>
+      <c r="E4" t="s">
+        <v>273</v>
       </c>
       <c r="F4" s="60" t="s">
         <v>92</v>
@@ -3497,7 +3509,7 @@
   <dimension ref="A1:IU4"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4314,11 +4326,11 @@
         <v>43101</v>
       </c>
       <c r="B4" s="51"/>
-      <c r="C4" s="51" t="s">
-        <v>253</v>
+      <c r="C4" t="s">
+        <v>273</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>195</v>
@@ -4342,7 +4354,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="136" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4433,152 +4445,152 @@
         <v>43101</v>
       </c>
       <c r="B4" s="58"/>
-      <c r="C4" s="115" t="s">
-        <v>253</v>
+      <c r="C4" t="s">
+        <v>273</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="E4" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F4" s="117" t="s">
+      <c r="E4" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" s="116" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A5" s="118">
+      <c r="A5" s="117">
         <v>43101</v>
       </c>
-      <c r="C5" s="115" t="s">
-        <v>253</v>
+      <c r="C5" t="s">
+        <v>273</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="E5" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F5" s="119" t="s">
+      <c r="E5" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F5" s="118" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A6" s="118">
+      <c r="A6" s="117">
         <v>43101</v>
       </c>
-      <c r="C6" s="115" t="s">
-        <v>253</v>
+      <c r="C6" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="E6" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F6" s="119" t="s">
+      <c r="E6" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="118" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A7" s="118">
+      <c r="A7" s="117">
         <v>43101</v>
       </c>
-      <c r="C7" s="115" t="s">
-        <v>253</v>
+      <c r="C7" t="s">
+        <v>273</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E7" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F7" s="119" t="s">
+      <c r="E7" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F7" s="118" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A8" s="118">
+      <c r="A8" s="117">
         <v>43101</v>
       </c>
-      <c r="C8" s="115" t="s">
-        <v>253</v>
+      <c r="C8" t="s">
+        <v>273</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E8" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F8" s="119" t="s">
+      <c r="E8" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F8" s="118" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A9" s="118">
+      <c r="A9" s="117">
         <v>43101</v>
       </c>
-      <c r="C9" s="115" t="s">
-        <v>253</v>
+      <c r="C9" t="s">
+        <v>273</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="E9" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F9" s="119" t="s">
+      <c r="E9" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F9" s="118" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A10" s="118">
+      <c r="A10" s="117">
         <v>43101</v>
       </c>
-      <c r="C10" s="115" t="s">
-        <v>253</v>
+      <c r="C10" t="s">
+        <v>273</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="E10" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F10" s="119" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F10" s="118" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A11" s="118">
+      <c r="A11" s="117">
         <v>43101</v>
       </c>
-      <c r="C11" s="115" t="s">
-        <v>253</v>
+      <c r="C11" t="s">
+        <v>273</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F11" s="119" t="s">
+      <c r="E11" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F11" s="118" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A12" s="118">
+      <c r="A12" s="117">
         <v>43101</v>
       </c>
-      <c r="C12" s="115" t="s">
-        <v>253</v>
+      <c r="C12" t="s">
+        <v>273</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="E12" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F12" s="119" t="s">
+      <c r="E12" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F12" s="118" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4599,7 +4611,7 @@
   <dimension ref="A1:IU17"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="166" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5421,88 +5433,88 @@
         <v>43101</v>
       </c>
       <c r="B4" s="58"/>
-      <c r="C4" s="115" t="s">
-        <v>253</v>
+      <c r="C4" t="s">
+        <v>273</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E4" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F4" s="117" t="s">
+      <c r="E4" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" s="116" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:255" x14ac:dyDescent="0.15">
-      <c r="A5" s="118">
+      <c r="A5" s="117">
         <v>43101</v>
       </c>
       <c r="B5" s="16"/>
-      <c r="C5" s="115" t="s">
-        <v>253</v>
+      <c r="C5" t="s">
+        <v>273</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="E5" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F5" s="119" t="s">
+      <c r="E5" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F5" s="118" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:255" x14ac:dyDescent="0.15">
-      <c r="A6" s="118">
+      <c r="A6" s="117">
         <v>43101</v>
       </c>
       <c r="B6" s="51"/>
-      <c r="C6" s="115" t="s">
-        <v>253</v>
+      <c r="C6" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E6" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F6" s="123" t="s">
+      <c r="E6" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="122" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:255" x14ac:dyDescent="0.15">
-      <c r="A7" s="118">
+      <c r="A7" s="117">
         <v>43101</v>
       </c>
-      <c r="B7" s="122"/>
-      <c r="C7" s="115" t="s">
-        <v>253</v>
+      <c r="B7" s="121"/>
+      <c r="C7" t="s">
+        <v>273</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="E7" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F7" s="119" t="s">
+      <c r="E7" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F7" s="118" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:255" x14ac:dyDescent="0.15">
-      <c r="A8" s="120">
+      <c r="A8" s="119">
         <v>43101</v>
       </c>
-      <c r="B8" s="124"/>
-      <c r="C8" s="115" t="s">
-        <v>253</v>
+      <c r="B8" s="123"/>
+      <c r="C8" t="s">
+        <v>273</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E8" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F8" s="121" t="s">
+      <c r="E8" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F8" s="120" t="s">
         <v>195</v>
       </c>
     </row>
@@ -5538,285 +5550,285 @@
   <dimension ref="A1:AMK15"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="125" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="125" customWidth="1"/>
-    <col min="3" max="3" width="44" style="125" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" style="125" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" style="125" customWidth="1"/>
-    <col min="6" max="6" width="36" style="126" customWidth="1"/>
-    <col min="7" max="255" width="12.5" style="125" customWidth="1"/>
-    <col min="256" max="1025" width="7.1640625" style="125" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" style="124" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="124" customWidth="1"/>
+    <col min="3" max="3" width="44" style="124" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" style="124" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" style="124" customWidth="1"/>
+    <col min="6" max="6" width="36" style="125" customWidth="1"/>
+    <col min="7" max="255" width="12.5" style="124" customWidth="1"/>
+    <col min="256" max="1025" width="7.1640625" style="124" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="126" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="128" t="s">
+      <c r="B1" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="129" t="s">
+      <c r="C1" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="132"/>
-      <c r="R1" s="132"/>
-      <c r="S1" s="132"/>
-      <c r="T1" s="132"/>
-      <c r="U1" s="132"/>
-      <c r="V1" s="132"/>
-      <c r="W1" s="132"/>
-      <c r="X1" s="132"/>
-      <c r="Y1" s="132"/>
-      <c r="Z1" s="132"/>
-      <c r="AA1" s="132"/>
-      <c r="AB1" s="132"/>
-      <c r="AC1" s="132"/>
-      <c r="AD1" s="132"/>
-      <c r="AE1" s="132"/>
-      <c r="AF1" s="132"/>
-      <c r="AG1" s="132"/>
-      <c r="AH1" s="132"/>
-      <c r="AI1" s="132"/>
-      <c r="AJ1" s="132"/>
-      <c r="AK1" s="132"/>
-      <c r="AL1" s="132"/>
-      <c r="AM1" s="132"/>
-      <c r="AN1" s="132"/>
-      <c r="AO1" s="132"/>
-      <c r="AP1" s="132"/>
-      <c r="AQ1" s="132"/>
-      <c r="AR1" s="132"/>
-      <c r="AS1" s="132"/>
-      <c r="AT1" s="132"/>
-      <c r="AU1" s="132"/>
-      <c r="AV1" s="132"/>
-      <c r="AW1" s="132"/>
-      <c r="AX1" s="132"/>
-      <c r="AY1" s="132"/>
-      <c r="AZ1" s="132"/>
-      <c r="BA1" s="132"/>
-      <c r="BB1" s="132"/>
-      <c r="BC1" s="132"/>
-      <c r="BD1" s="132"/>
-      <c r="BE1" s="132"/>
-      <c r="BF1" s="132"/>
-      <c r="BG1" s="132"/>
-      <c r="BH1" s="132"/>
-      <c r="BI1" s="132"/>
-      <c r="BJ1" s="132"/>
-      <c r="BK1" s="132"/>
-      <c r="BL1" s="132"/>
-      <c r="BM1" s="132"/>
-      <c r="BN1" s="132"/>
-      <c r="BO1" s="132"/>
-      <c r="BP1" s="132"/>
-      <c r="BQ1" s="132"/>
-      <c r="BR1" s="132"/>
-      <c r="BS1" s="132"/>
-      <c r="BT1" s="132"/>
-      <c r="BU1" s="132"/>
-      <c r="BV1" s="132"/>
-      <c r="BW1" s="132"/>
-      <c r="BX1" s="132"/>
-      <c r="BY1" s="132"/>
-      <c r="BZ1" s="132"/>
-      <c r="CA1" s="132"/>
-      <c r="CB1" s="132"/>
-      <c r="CC1" s="132"/>
-      <c r="CD1" s="132"/>
-      <c r="CE1" s="132"/>
-      <c r="CF1" s="132"/>
-      <c r="CG1" s="132"/>
-      <c r="CH1" s="132"/>
-      <c r="CI1" s="132"/>
-      <c r="CJ1" s="132"/>
-      <c r="CK1" s="132"/>
-      <c r="CL1" s="132"/>
-      <c r="CM1" s="132"/>
-      <c r="CN1" s="132"/>
-      <c r="CO1" s="132"/>
-      <c r="CP1" s="132"/>
-      <c r="CQ1" s="132"/>
-      <c r="CR1" s="132"/>
-      <c r="CS1" s="132"/>
-      <c r="CT1" s="132"/>
-      <c r="CU1" s="132"/>
-      <c r="CV1" s="132"/>
-      <c r="CW1" s="132"/>
-      <c r="CX1" s="132"/>
-      <c r="CY1" s="132"/>
-      <c r="CZ1" s="132"/>
-      <c r="DA1" s="132"/>
-      <c r="DB1" s="132"/>
-      <c r="DC1" s="132"/>
-      <c r="DD1" s="132"/>
-      <c r="DE1" s="132"/>
-      <c r="DF1" s="132"/>
-      <c r="DG1" s="132"/>
-      <c r="DH1" s="132"/>
-      <c r="DI1" s="132"/>
-      <c r="DJ1" s="132"/>
-      <c r="DK1" s="132"/>
-      <c r="DL1" s="132"/>
-      <c r="DM1" s="132"/>
-      <c r="DN1" s="132"/>
-      <c r="DO1" s="132"/>
-      <c r="DP1" s="132"/>
-      <c r="DQ1" s="132"/>
-      <c r="DR1" s="132"/>
-      <c r="DS1" s="132"/>
-      <c r="DT1" s="132"/>
-      <c r="DU1" s="132"/>
-      <c r="DV1" s="132"/>
-      <c r="DW1" s="132"/>
-      <c r="DX1" s="132"/>
-      <c r="DY1" s="132"/>
-      <c r="DZ1" s="132"/>
-      <c r="EA1" s="132"/>
-      <c r="EB1" s="132"/>
-      <c r="EC1" s="132"/>
-      <c r="ED1" s="132"/>
-      <c r="EE1" s="132"/>
-      <c r="EF1" s="132"/>
-      <c r="EG1" s="132"/>
-      <c r="EH1" s="132"/>
-      <c r="EI1" s="132"/>
-      <c r="EJ1" s="132"/>
-      <c r="EK1" s="132"/>
-      <c r="EL1" s="132"/>
-      <c r="EM1" s="132"/>
-      <c r="EN1" s="132"/>
-      <c r="EO1" s="132"/>
-      <c r="EP1" s="132"/>
-      <c r="EQ1" s="132"/>
-      <c r="ER1" s="132"/>
-      <c r="ES1" s="132"/>
-      <c r="ET1" s="132"/>
-      <c r="EU1" s="132"/>
-      <c r="EV1" s="132"/>
-      <c r="EW1" s="132"/>
-      <c r="EX1" s="132"/>
-      <c r="EY1" s="132"/>
-      <c r="EZ1" s="132"/>
-      <c r="FA1" s="132"/>
-      <c r="FB1" s="132"/>
-      <c r="FC1" s="132"/>
-      <c r="FD1" s="132"/>
-      <c r="FE1" s="132"/>
-      <c r="FF1" s="132"/>
-      <c r="FG1" s="132"/>
-      <c r="FH1" s="132"/>
-      <c r="FI1" s="132"/>
-      <c r="FJ1" s="132"/>
-      <c r="FK1" s="132"/>
-      <c r="FL1" s="132"/>
-      <c r="FM1" s="132"/>
-      <c r="FN1" s="132"/>
-      <c r="FO1" s="132"/>
-      <c r="FP1" s="132"/>
-      <c r="FQ1" s="132"/>
-      <c r="FR1" s="132"/>
-      <c r="FS1" s="132"/>
-      <c r="FT1" s="132"/>
-      <c r="FU1" s="132"/>
-      <c r="FV1" s="132"/>
-      <c r="FW1" s="132"/>
-      <c r="FX1" s="132"/>
-      <c r="FY1" s="132"/>
-      <c r="FZ1" s="132"/>
-      <c r="GA1" s="132"/>
-      <c r="GB1" s="132"/>
-      <c r="GC1" s="132"/>
-      <c r="GD1" s="132"/>
-      <c r="GE1" s="132"/>
-      <c r="GF1" s="132"/>
-      <c r="GG1" s="132"/>
-      <c r="GH1" s="132"/>
-      <c r="GI1" s="132"/>
-      <c r="GJ1" s="132"/>
-      <c r="GK1" s="132"/>
-      <c r="GL1" s="132"/>
-      <c r="GM1" s="132"/>
-      <c r="GN1" s="132"/>
-      <c r="GO1" s="132"/>
-      <c r="GP1" s="132"/>
-      <c r="GQ1" s="132"/>
-      <c r="GR1" s="132"/>
-      <c r="GS1" s="132"/>
-      <c r="GT1" s="132"/>
-      <c r="GU1" s="132"/>
-      <c r="GV1" s="132"/>
-      <c r="GW1" s="132"/>
-      <c r="GX1" s="132"/>
-      <c r="GY1" s="132"/>
-      <c r="GZ1" s="132"/>
-      <c r="HA1" s="132"/>
-      <c r="HB1" s="132"/>
-      <c r="HC1" s="132"/>
-      <c r="HD1" s="132"/>
-      <c r="HE1" s="132"/>
-      <c r="HF1" s="132"/>
-      <c r="HG1" s="132"/>
-      <c r="HH1" s="132"/>
-      <c r="HI1" s="132"/>
-      <c r="HJ1" s="132"/>
-      <c r="HK1" s="132"/>
-      <c r="HL1" s="132"/>
-      <c r="HM1" s="132"/>
-      <c r="HN1" s="132"/>
-      <c r="HO1" s="132"/>
-      <c r="HP1" s="132"/>
-      <c r="HQ1" s="132"/>
-      <c r="HR1" s="132"/>
-      <c r="HS1" s="132"/>
-      <c r="HT1" s="132"/>
-      <c r="HU1" s="132"/>
-      <c r="HV1" s="132"/>
-      <c r="HW1" s="132"/>
-      <c r="HX1" s="132"/>
-      <c r="HY1" s="132"/>
-      <c r="HZ1" s="132"/>
-      <c r="IA1" s="132"/>
-      <c r="IB1" s="132"/>
-      <c r="IC1" s="132"/>
-      <c r="ID1" s="132"/>
-      <c r="IE1" s="132"/>
-      <c r="IF1" s="132"/>
-      <c r="IG1" s="132"/>
-      <c r="IH1" s="132"/>
-      <c r="II1" s="132"/>
-      <c r="IJ1" s="132"/>
-      <c r="IK1" s="132"/>
-      <c r="IL1" s="132"/>
-      <c r="IM1" s="132"/>
-      <c r="IN1" s="132"/>
-      <c r="IO1" s="132"/>
-      <c r="IP1" s="132"/>
-      <c r="IQ1" s="132"/>
-      <c r="IR1" s="132"/>
-      <c r="IS1" s="132"/>
-      <c r="IT1" s="132"/>
-      <c r="IU1" s="132"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="131"/>
+      <c r="R1" s="131"/>
+      <c r="S1" s="131"/>
+      <c r="T1" s="131"/>
+      <c r="U1" s="131"/>
+      <c r="V1" s="131"/>
+      <c r="W1" s="131"/>
+      <c r="X1" s="131"/>
+      <c r="Y1" s="131"/>
+      <c r="Z1" s="131"/>
+      <c r="AA1" s="131"/>
+      <c r="AB1" s="131"/>
+      <c r="AC1" s="131"/>
+      <c r="AD1" s="131"/>
+      <c r="AE1" s="131"/>
+      <c r="AF1" s="131"/>
+      <c r="AG1" s="131"/>
+      <c r="AH1" s="131"/>
+      <c r="AI1" s="131"/>
+      <c r="AJ1" s="131"/>
+      <c r="AK1" s="131"/>
+      <c r="AL1" s="131"/>
+      <c r="AM1" s="131"/>
+      <c r="AN1" s="131"/>
+      <c r="AO1" s="131"/>
+      <c r="AP1" s="131"/>
+      <c r="AQ1" s="131"/>
+      <c r="AR1" s="131"/>
+      <c r="AS1" s="131"/>
+      <c r="AT1" s="131"/>
+      <c r="AU1" s="131"/>
+      <c r="AV1" s="131"/>
+      <c r="AW1" s="131"/>
+      <c r="AX1" s="131"/>
+      <c r="AY1" s="131"/>
+      <c r="AZ1" s="131"/>
+      <c r="BA1" s="131"/>
+      <c r="BB1" s="131"/>
+      <c r="BC1" s="131"/>
+      <c r="BD1" s="131"/>
+      <c r="BE1" s="131"/>
+      <c r="BF1" s="131"/>
+      <c r="BG1" s="131"/>
+      <c r="BH1" s="131"/>
+      <c r="BI1" s="131"/>
+      <c r="BJ1" s="131"/>
+      <c r="BK1" s="131"/>
+      <c r="BL1" s="131"/>
+      <c r="BM1" s="131"/>
+      <c r="BN1" s="131"/>
+      <c r="BO1" s="131"/>
+      <c r="BP1" s="131"/>
+      <c r="BQ1" s="131"/>
+      <c r="BR1" s="131"/>
+      <c r="BS1" s="131"/>
+      <c r="BT1" s="131"/>
+      <c r="BU1" s="131"/>
+      <c r="BV1" s="131"/>
+      <c r="BW1" s="131"/>
+      <c r="BX1" s="131"/>
+      <c r="BY1" s="131"/>
+      <c r="BZ1" s="131"/>
+      <c r="CA1" s="131"/>
+      <c r="CB1" s="131"/>
+      <c r="CC1" s="131"/>
+      <c r="CD1" s="131"/>
+      <c r="CE1" s="131"/>
+      <c r="CF1" s="131"/>
+      <c r="CG1" s="131"/>
+      <c r="CH1" s="131"/>
+      <c r="CI1" s="131"/>
+      <c r="CJ1" s="131"/>
+      <c r="CK1" s="131"/>
+      <c r="CL1" s="131"/>
+      <c r="CM1" s="131"/>
+      <c r="CN1" s="131"/>
+      <c r="CO1" s="131"/>
+      <c r="CP1" s="131"/>
+      <c r="CQ1" s="131"/>
+      <c r="CR1" s="131"/>
+      <c r="CS1" s="131"/>
+      <c r="CT1" s="131"/>
+      <c r="CU1" s="131"/>
+      <c r="CV1" s="131"/>
+      <c r="CW1" s="131"/>
+      <c r="CX1" s="131"/>
+      <c r="CY1" s="131"/>
+      <c r="CZ1" s="131"/>
+      <c r="DA1" s="131"/>
+      <c r="DB1" s="131"/>
+      <c r="DC1" s="131"/>
+      <c r="DD1" s="131"/>
+      <c r="DE1" s="131"/>
+      <c r="DF1" s="131"/>
+      <c r="DG1" s="131"/>
+      <c r="DH1" s="131"/>
+      <c r="DI1" s="131"/>
+      <c r="DJ1" s="131"/>
+      <c r="DK1" s="131"/>
+      <c r="DL1" s="131"/>
+      <c r="DM1" s="131"/>
+      <c r="DN1" s="131"/>
+      <c r="DO1" s="131"/>
+      <c r="DP1" s="131"/>
+      <c r="DQ1" s="131"/>
+      <c r="DR1" s="131"/>
+      <c r="DS1" s="131"/>
+      <c r="DT1" s="131"/>
+      <c r="DU1" s="131"/>
+      <c r="DV1" s="131"/>
+      <c r="DW1" s="131"/>
+      <c r="DX1" s="131"/>
+      <c r="DY1" s="131"/>
+      <c r="DZ1" s="131"/>
+      <c r="EA1" s="131"/>
+      <c r="EB1" s="131"/>
+      <c r="EC1" s="131"/>
+      <c r="ED1" s="131"/>
+      <c r="EE1" s="131"/>
+      <c r="EF1" s="131"/>
+      <c r="EG1" s="131"/>
+      <c r="EH1" s="131"/>
+      <c r="EI1" s="131"/>
+      <c r="EJ1" s="131"/>
+      <c r="EK1" s="131"/>
+      <c r="EL1" s="131"/>
+      <c r="EM1" s="131"/>
+      <c r="EN1" s="131"/>
+      <c r="EO1" s="131"/>
+      <c r="EP1" s="131"/>
+      <c r="EQ1" s="131"/>
+      <c r="ER1" s="131"/>
+      <c r="ES1" s="131"/>
+      <c r="ET1" s="131"/>
+      <c r="EU1" s="131"/>
+      <c r="EV1" s="131"/>
+      <c r="EW1" s="131"/>
+      <c r="EX1" s="131"/>
+      <c r="EY1" s="131"/>
+      <c r="EZ1" s="131"/>
+      <c r="FA1" s="131"/>
+      <c r="FB1" s="131"/>
+      <c r="FC1" s="131"/>
+      <c r="FD1" s="131"/>
+      <c r="FE1" s="131"/>
+      <c r="FF1" s="131"/>
+      <c r="FG1" s="131"/>
+      <c r="FH1" s="131"/>
+      <c r="FI1" s="131"/>
+      <c r="FJ1" s="131"/>
+      <c r="FK1" s="131"/>
+      <c r="FL1" s="131"/>
+      <c r="FM1" s="131"/>
+      <c r="FN1" s="131"/>
+      <c r="FO1" s="131"/>
+      <c r="FP1" s="131"/>
+      <c r="FQ1" s="131"/>
+      <c r="FR1" s="131"/>
+      <c r="FS1" s="131"/>
+      <c r="FT1" s="131"/>
+      <c r="FU1" s="131"/>
+      <c r="FV1" s="131"/>
+      <c r="FW1" s="131"/>
+      <c r="FX1" s="131"/>
+      <c r="FY1" s="131"/>
+      <c r="FZ1" s="131"/>
+      <c r="GA1" s="131"/>
+      <c r="GB1" s="131"/>
+      <c r="GC1" s="131"/>
+      <c r="GD1" s="131"/>
+      <c r="GE1" s="131"/>
+      <c r="GF1" s="131"/>
+      <c r="GG1" s="131"/>
+      <c r="GH1" s="131"/>
+      <c r="GI1" s="131"/>
+      <c r="GJ1" s="131"/>
+      <c r="GK1" s="131"/>
+      <c r="GL1" s="131"/>
+      <c r="GM1" s="131"/>
+      <c r="GN1" s="131"/>
+      <c r="GO1" s="131"/>
+      <c r="GP1" s="131"/>
+      <c r="GQ1" s="131"/>
+      <c r="GR1" s="131"/>
+      <c r="GS1" s="131"/>
+      <c r="GT1" s="131"/>
+      <c r="GU1" s="131"/>
+      <c r="GV1" s="131"/>
+      <c r="GW1" s="131"/>
+      <c r="GX1" s="131"/>
+      <c r="GY1" s="131"/>
+      <c r="GZ1" s="131"/>
+      <c r="HA1" s="131"/>
+      <c r="HB1" s="131"/>
+      <c r="HC1" s="131"/>
+      <c r="HD1" s="131"/>
+      <c r="HE1" s="131"/>
+      <c r="HF1" s="131"/>
+      <c r="HG1" s="131"/>
+      <c r="HH1" s="131"/>
+      <c r="HI1" s="131"/>
+      <c r="HJ1" s="131"/>
+      <c r="HK1" s="131"/>
+      <c r="HL1" s="131"/>
+      <c r="HM1" s="131"/>
+      <c r="HN1" s="131"/>
+      <c r="HO1" s="131"/>
+      <c r="HP1" s="131"/>
+      <c r="HQ1" s="131"/>
+      <c r="HR1" s="131"/>
+      <c r="HS1" s="131"/>
+      <c r="HT1" s="131"/>
+      <c r="HU1" s="131"/>
+      <c r="HV1" s="131"/>
+      <c r="HW1" s="131"/>
+      <c r="HX1" s="131"/>
+      <c r="HY1" s="131"/>
+      <c r="HZ1" s="131"/>
+      <c r="IA1" s="131"/>
+      <c r="IB1" s="131"/>
+      <c r="IC1" s="131"/>
+      <c r="ID1" s="131"/>
+      <c r="IE1" s="131"/>
+      <c r="IF1" s="131"/>
+      <c r="IG1" s="131"/>
+      <c r="IH1" s="131"/>
+      <c r="II1" s="131"/>
+      <c r="IJ1" s="131"/>
+      <c r="IK1" s="131"/>
+      <c r="IL1" s="131"/>
+      <c r="IM1" s="131"/>
+      <c r="IN1" s="131"/>
+      <c r="IO1" s="131"/>
+      <c r="IP1" s="131"/>
+      <c r="IQ1" s="131"/>
+      <c r="IR1" s="131"/>
+      <c r="IS1" s="131"/>
+      <c r="IT1" s="131"/>
+      <c r="IU1" s="131"/>
     </row>
     <row r="2" spans="1:255" s="16" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
@@ -5828,7 +5840,7 @@
       <c r="C2" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="D2" s="133" t="s">
+      <c r="D2" s="132" t="s">
         <v>202</v>
       </c>
       <c r="E2" s="18" t="s">
@@ -5837,261 +5849,261 @@
       <c r="F2" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="132"/>
-      <c r="M2" s="132"/>
-      <c r="N2" s="132"/>
-      <c r="O2" s="132"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="132"/>
-      <c r="R2" s="132"/>
-      <c r="S2" s="132"/>
-      <c r="T2" s="132"/>
-      <c r="U2" s="132"/>
-      <c r="V2" s="132"/>
-      <c r="W2" s="132"/>
-      <c r="X2" s="132"/>
-      <c r="Y2" s="132"/>
-      <c r="Z2" s="132"/>
-      <c r="AA2" s="132"/>
-      <c r="AB2" s="132"/>
-      <c r="AC2" s="132"/>
-      <c r="AD2" s="132"/>
-      <c r="AE2" s="132"/>
-      <c r="AF2" s="132"/>
-      <c r="AG2" s="132"/>
-      <c r="AH2" s="132"/>
-      <c r="AI2" s="132"/>
-      <c r="AJ2" s="132"/>
-      <c r="AK2" s="132"/>
-      <c r="AL2" s="132"/>
-      <c r="AM2" s="132"/>
-      <c r="AN2" s="132"/>
-      <c r="AO2" s="132"/>
-      <c r="AP2" s="132"/>
-      <c r="AQ2" s="132"/>
-      <c r="AR2" s="132"/>
-      <c r="AS2" s="132"/>
-      <c r="AT2" s="132"/>
-      <c r="AU2" s="132"/>
-      <c r="AV2" s="132"/>
-      <c r="AW2" s="132"/>
-      <c r="AX2" s="132"/>
-      <c r="AY2" s="132"/>
-      <c r="AZ2" s="132"/>
-      <c r="BA2" s="132"/>
-      <c r="BB2" s="132"/>
-      <c r="BC2" s="132"/>
-      <c r="BD2" s="132"/>
-      <c r="BE2" s="132"/>
-      <c r="BF2" s="132"/>
-      <c r="BG2" s="132"/>
-      <c r="BH2" s="132"/>
-      <c r="BI2" s="132"/>
-      <c r="BJ2" s="132"/>
-      <c r="BK2" s="132"/>
-      <c r="BL2" s="132"/>
-      <c r="BM2" s="132"/>
-      <c r="BN2" s="132"/>
-      <c r="BO2" s="132"/>
-      <c r="BP2" s="132"/>
-      <c r="BQ2" s="132"/>
-      <c r="BR2" s="132"/>
-      <c r="BS2" s="132"/>
-      <c r="BT2" s="132"/>
-      <c r="BU2" s="132"/>
-      <c r="BV2" s="132"/>
-      <c r="BW2" s="132"/>
-      <c r="BX2" s="132"/>
-      <c r="BY2" s="132"/>
-      <c r="BZ2" s="132"/>
-      <c r="CA2" s="132"/>
-      <c r="CB2" s="132"/>
-      <c r="CC2" s="132"/>
-      <c r="CD2" s="132"/>
-      <c r="CE2" s="132"/>
-      <c r="CF2" s="132"/>
-      <c r="CG2" s="132"/>
-      <c r="CH2" s="132"/>
-      <c r="CI2" s="132"/>
-      <c r="CJ2" s="132"/>
-      <c r="CK2" s="132"/>
-      <c r="CL2" s="132"/>
-      <c r="CM2" s="132"/>
-      <c r="CN2" s="132"/>
-      <c r="CO2" s="132"/>
-      <c r="CP2" s="132"/>
-      <c r="CQ2" s="132"/>
-      <c r="CR2" s="132"/>
-      <c r="CS2" s="132"/>
-      <c r="CT2" s="132"/>
-      <c r="CU2" s="132"/>
-      <c r="CV2" s="132"/>
-      <c r="CW2" s="132"/>
-      <c r="CX2" s="132"/>
-      <c r="CY2" s="132"/>
-      <c r="CZ2" s="132"/>
-      <c r="DA2" s="132"/>
-      <c r="DB2" s="132"/>
-      <c r="DC2" s="132"/>
-      <c r="DD2" s="132"/>
-      <c r="DE2" s="132"/>
-      <c r="DF2" s="132"/>
-      <c r="DG2" s="132"/>
-      <c r="DH2" s="132"/>
-      <c r="DI2" s="132"/>
-      <c r="DJ2" s="132"/>
-      <c r="DK2" s="132"/>
-      <c r="DL2" s="132"/>
-      <c r="DM2" s="132"/>
-      <c r="DN2" s="132"/>
-      <c r="DO2" s="132"/>
-      <c r="DP2" s="132"/>
-      <c r="DQ2" s="132"/>
-      <c r="DR2" s="132"/>
-      <c r="DS2" s="132"/>
-      <c r="DT2" s="132"/>
-      <c r="DU2" s="132"/>
-      <c r="DV2" s="132"/>
-      <c r="DW2" s="132"/>
-      <c r="DX2" s="132"/>
-      <c r="DY2" s="132"/>
-      <c r="DZ2" s="132"/>
-      <c r="EA2" s="132"/>
-      <c r="EB2" s="132"/>
-      <c r="EC2" s="132"/>
-      <c r="ED2" s="132"/>
-      <c r="EE2" s="132"/>
-      <c r="EF2" s="132"/>
-      <c r="EG2" s="132"/>
-      <c r="EH2" s="132"/>
-      <c r="EI2" s="132"/>
-      <c r="EJ2" s="132"/>
-      <c r="EK2" s="132"/>
-      <c r="EL2" s="132"/>
-      <c r="EM2" s="132"/>
-      <c r="EN2" s="132"/>
-      <c r="EO2" s="132"/>
-      <c r="EP2" s="132"/>
-      <c r="EQ2" s="132"/>
-      <c r="ER2" s="132"/>
-      <c r="ES2" s="132"/>
-      <c r="ET2" s="132"/>
-      <c r="EU2" s="132"/>
-      <c r="EV2" s="132"/>
-      <c r="EW2" s="132"/>
-      <c r="EX2" s="132"/>
-      <c r="EY2" s="132"/>
-      <c r="EZ2" s="132"/>
-      <c r="FA2" s="132"/>
-      <c r="FB2" s="132"/>
-      <c r="FC2" s="132"/>
-      <c r="FD2" s="132"/>
-      <c r="FE2" s="132"/>
-      <c r="FF2" s="132"/>
-      <c r="FG2" s="132"/>
-      <c r="FH2" s="132"/>
-      <c r="FI2" s="132"/>
-      <c r="FJ2" s="132"/>
-      <c r="FK2" s="132"/>
-      <c r="FL2" s="132"/>
-      <c r="FM2" s="132"/>
-      <c r="FN2" s="132"/>
-      <c r="FO2" s="132"/>
-      <c r="FP2" s="132"/>
-      <c r="FQ2" s="132"/>
-      <c r="FR2" s="132"/>
-      <c r="FS2" s="132"/>
-      <c r="FT2" s="132"/>
-      <c r="FU2" s="132"/>
-      <c r="FV2" s="132"/>
-      <c r="FW2" s="132"/>
-      <c r="FX2" s="132"/>
-      <c r="FY2" s="132"/>
-      <c r="FZ2" s="132"/>
-      <c r="GA2" s="132"/>
-      <c r="GB2" s="132"/>
-      <c r="GC2" s="132"/>
-      <c r="GD2" s="132"/>
-      <c r="GE2" s="132"/>
-      <c r="GF2" s="132"/>
-      <c r="GG2" s="132"/>
-      <c r="GH2" s="132"/>
-      <c r="GI2" s="132"/>
-      <c r="GJ2" s="132"/>
-      <c r="GK2" s="132"/>
-      <c r="GL2" s="132"/>
-      <c r="GM2" s="132"/>
-      <c r="GN2" s="132"/>
-      <c r="GO2" s="132"/>
-      <c r="GP2" s="132"/>
-      <c r="GQ2" s="132"/>
-      <c r="GR2" s="132"/>
-      <c r="GS2" s="132"/>
-      <c r="GT2" s="132"/>
-      <c r="GU2" s="132"/>
-      <c r="GV2" s="132"/>
-      <c r="GW2" s="132"/>
-      <c r="GX2" s="132"/>
-      <c r="GY2" s="132"/>
-      <c r="GZ2" s="132"/>
-      <c r="HA2" s="132"/>
-      <c r="HB2" s="132"/>
-      <c r="HC2" s="132"/>
-      <c r="HD2" s="132"/>
-      <c r="HE2" s="132"/>
-      <c r="HF2" s="132"/>
-      <c r="HG2" s="132"/>
-      <c r="HH2" s="132"/>
-      <c r="HI2" s="132"/>
-      <c r="HJ2" s="132"/>
-      <c r="HK2" s="132"/>
-      <c r="HL2" s="132"/>
-      <c r="HM2" s="132"/>
-      <c r="HN2" s="132"/>
-      <c r="HO2" s="132"/>
-      <c r="HP2" s="132"/>
-      <c r="HQ2" s="132"/>
-      <c r="HR2" s="132"/>
-      <c r="HS2" s="132"/>
-      <c r="HT2" s="132"/>
-      <c r="HU2" s="132"/>
-      <c r="HV2" s="132"/>
-      <c r="HW2" s="132"/>
-      <c r="HX2" s="132"/>
-      <c r="HY2" s="132"/>
-      <c r="HZ2" s="132"/>
-      <c r="IA2" s="132"/>
-      <c r="IB2" s="132"/>
-      <c r="IC2" s="132"/>
-      <c r="ID2" s="132"/>
-      <c r="IE2" s="132"/>
-      <c r="IF2" s="132"/>
-      <c r="IG2" s="132"/>
-      <c r="IH2" s="132"/>
-      <c r="II2" s="132"/>
-      <c r="IJ2" s="132"/>
-      <c r="IK2" s="132"/>
-      <c r="IL2" s="132"/>
-      <c r="IM2" s="132"/>
-      <c r="IN2" s="132"/>
-      <c r="IO2" s="132"/>
-      <c r="IP2" s="132"/>
-      <c r="IQ2" s="132"/>
-      <c r="IR2" s="132"/>
-      <c r="IS2" s="132"/>
-      <c r="IT2" s="132"/>
-      <c r="IU2" s="132"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="131"/>
+      <c r="U2" s="131"/>
+      <c r="V2" s="131"/>
+      <c r="W2" s="131"/>
+      <c r="X2" s="131"/>
+      <c r="Y2" s="131"/>
+      <c r="Z2" s="131"/>
+      <c r="AA2" s="131"/>
+      <c r="AB2" s="131"/>
+      <c r="AC2" s="131"/>
+      <c r="AD2" s="131"/>
+      <c r="AE2" s="131"/>
+      <c r="AF2" s="131"/>
+      <c r="AG2" s="131"/>
+      <c r="AH2" s="131"/>
+      <c r="AI2" s="131"/>
+      <c r="AJ2" s="131"/>
+      <c r="AK2" s="131"/>
+      <c r="AL2" s="131"/>
+      <c r="AM2" s="131"/>
+      <c r="AN2" s="131"/>
+      <c r="AO2" s="131"/>
+      <c r="AP2" s="131"/>
+      <c r="AQ2" s="131"/>
+      <c r="AR2" s="131"/>
+      <c r="AS2" s="131"/>
+      <c r="AT2" s="131"/>
+      <c r="AU2" s="131"/>
+      <c r="AV2" s="131"/>
+      <c r="AW2" s="131"/>
+      <c r="AX2" s="131"/>
+      <c r="AY2" s="131"/>
+      <c r="AZ2" s="131"/>
+      <c r="BA2" s="131"/>
+      <c r="BB2" s="131"/>
+      <c r="BC2" s="131"/>
+      <c r="BD2" s="131"/>
+      <c r="BE2" s="131"/>
+      <c r="BF2" s="131"/>
+      <c r="BG2" s="131"/>
+      <c r="BH2" s="131"/>
+      <c r="BI2" s="131"/>
+      <c r="BJ2" s="131"/>
+      <c r="BK2" s="131"/>
+      <c r="BL2" s="131"/>
+      <c r="BM2" s="131"/>
+      <c r="BN2" s="131"/>
+      <c r="BO2" s="131"/>
+      <c r="BP2" s="131"/>
+      <c r="BQ2" s="131"/>
+      <c r="BR2" s="131"/>
+      <c r="BS2" s="131"/>
+      <c r="BT2" s="131"/>
+      <c r="BU2" s="131"/>
+      <c r="BV2" s="131"/>
+      <c r="BW2" s="131"/>
+      <c r="BX2" s="131"/>
+      <c r="BY2" s="131"/>
+      <c r="BZ2" s="131"/>
+      <c r="CA2" s="131"/>
+      <c r="CB2" s="131"/>
+      <c r="CC2" s="131"/>
+      <c r="CD2" s="131"/>
+      <c r="CE2" s="131"/>
+      <c r="CF2" s="131"/>
+      <c r="CG2" s="131"/>
+      <c r="CH2" s="131"/>
+      <c r="CI2" s="131"/>
+      <c r="CJ2" s="131"/>
+      <c r="CK2" s="131"/>
+      <c r="CL2" s="131"/>
+      <c r="CM2" s="131"/>
+      <c r="CN2" s="131"/>
+      <c r="CO2" s="131"/>
+      <c r="CP2" s="131"/>
+      <c r="CQ2" s="131"/>
+      <c r="CR2" s="131"/>
+      <c r="CS2" s="131"/>
+      <c r="CT2" s="131"/>
+      <c r="CU2" s="131"/>
+      <c r="CV2" s="131"/>
+      <c r="CW2" s="131"/>
+      <c r="CX2" s="131"/>
+      <c r="CY2" s="131"/>
+      <c r="CZ2" s="131"/>
+      <c r="DA2" s="131"/>
+      <c r="DB2" s="131"/>
+      <c r="DC2" s="131"/>
+      <c r="DD2" s="131"/>
+      <c r="DE2" s="131"/>
+      <c r="DF2" s="131"/>
+      <c r="DG2" s="131"/>
+      <c r="DH2" s="131"/>
+      <c r="DI2" s="131"/>
+      <c r="DJ2" s="131"/>
+      <c r="DK2" s="131"/>
+      <c r="DL2" s="131"/>
+      <c r="DM2" s="131"/>
+      <c r="DN2" s="131"/>
+      <c r="DO2" s="131"/>
+      <c r="DP2" s="131"/>
+      <c r="DQ2" s="131"/>
+      <c r="DR2" s="131"/>
+      <c r="DS2" s="131"/>
+      <c r="DT2" s="131"/>
+      <c r="DU2" s="131"/>
+      <c r="DV2" s="131"/>
+      <c r="DW2" s="131"/>
+      <c r="DX2" s="131"/>
+      <c r="DY2" s="131"/>
+      <c r="DZ2" s="131"/>
+      <c r="EA2" s="131"/>
+      <c r="EB2" s="131"/>
+      <c r="EC2" s="131"/>
+      <c r="ED2" s="131"/>
+      <c r="EE2" s="131"/>
+      <c r="EF2" s="131"/>
+      <c r="EG2" s="131"/>
+      <c r="EH2" s="131"/>
+      <c r="EI2" s="131"/>
+      <c r="EJ2" s="131"/>
+      <c r="EK2" s="131"/>
+      <c r="EL2" s="131"/>
+      <c r="EM2" s="131"/>
+      <c r="EN2" s="131"/>
+      <c r="EO2" s="131"/>
+      <c r="EP2" s="131"/>
+      <c r="EQ2" s="131"/>
+      <c r="ER2" s="131"/>
+      <c r="ES2" s="131"/>
+      <c r="ET2" s="131"/>
+      <c r="EU2" s="131"/>
+      <c r="EV2" s="131"/>
+      <c r="EW2" s="131"/>
+      <c r="EX2" s="131"/>
+      <c r="EY2" s="131"/>
+      <c r="EZ2" s="131"/>
+      <c r="FA2" s="131"/>
+      <c r="FB2" s="131"/>
+      <c r="FC2" s="131"/>
+      <c r="FD2" s="131"/>
+      <c r="FE2" s="131"/>
+      <c r="FF2" s="131"/>
+      <c r="FG2" s="131"/>
+      <c r="FH2" s="131"/>
+      <c r="FI2" s="131"/>
+      <c r="FJ2" s="131"/>
+      <c r="FK2" s="131"/>
+      <c r="FL2" s="131"/>
+      <c r="FM2" s="131"/>
+      <c r="FN2" s="131"/>
+      <c r="FO2" s="131"/>
+      <c r="FP2" s="131"/>
+      <c r="FQ2" s="131"/>
+      <c r="FR2" s="131"/>
+      <c r="FS2" s="131"/>
+      <c r="FT2" s="131"/>
+      <c r="FU2" s="131"/>
+      <c r="FV2" s="131"/>
+      <c r="FW2" s="131"/>
+      <c r="FX2" s="131"/>
+      <c r="FY2" s="131"/>
+      <c r="FZ2" s="131"/>
+      <c r="GA2" s="131"/>
+      <c r="GB2" s="131"/>
+      <c r="GC2" s="131"/>
+      <c r="GD2" s="131"/>
+      <c r="GE2" s="131"/>
+      <c r="GF2" s="131"/>
+      <c r="GG2" s="131"/>
+      <c r="GH2" s="131"/>
+      <c r="GI2" s="131"/>
+      <c r="GJ2" s="131"/>
+      <c r="GK2" s="131"/>
+      <c r="GL2" s="131"/>
+      <c r="GM2" s="131"/>
+      <c r="GN2" s="131"/>
+      <c r="GO2" s="131"/>
+      <c r="GP2" s="131"/>
+      <c r="GQ2" s="131"/>
+      <c r="GR2" s="131"/>
+      <c r="GS2" s="131"/>
+      <c r="GT2" s="131"/>
+      <c r="GU2" s="131"/>
+      <c r="GV2" s="131"/>
+      <c r="GW2" s="131"/>
+      <c r="GX2" s="131"/>
+      <c r="GY2" s="131"/>
+      <c r="GZ2" s="131"/>
+      <c r="HA2" s="131"/>
+      <c r="HB2" s="131"/>
+      <c r="HC2" s="131"/>
+      <c r="HD2" s="131"/>
+      <c r="HE2" s="131"/>
+      <c r="HF2" s="131"/>
+      <c r="HG2" s="131"/>
+      <c r="HH2" s="131"/>
+      <c r="HI2" s="131"/>
+      <c r="HJ2" s="131"/>
+      <c r="HK2" s="131"/>
+      <c r="HL2" s="131"/>
+      <c r="HM2" s="131"/>
+      <c r="HN2" s="131"/>
+      <c r="HO2" s="131"/>
+      <c r="HP2" s="131"/>
+      <c r="HQ2" s="131"/>
+      <c r="HR2" s="131"/>
+      <c r="HS2" s="131"/>
+      <c r="HT2" s="131"/>
+      <c r="HU2" s="131"/>
+      <c r="HV2" s="131"/>
+      <c r="HW2" s="131"/>
+      <c r="HX2" s="131"/>
+      <c r="HY2" s="131"/>
+      <c r="HZ2" s="131"/>
+      <c r="IA2" s="131"/>
+      <c r="IB2" s="131"/>
+      <c r="IC2" s="131"/>
+      <c r="ID2" s="131"/>
+      <c r="IE2" s="131"/>
+      <c r="IF2" s="131"/>
+      <c r="IG2" s="131"/>
+      <c r="IH2" s="131"/>
+      <c r="II2" s="131"/>
+      <c r="IJ2" s="131"/>
+      <c r="IK2" s="131"/>
+      <c r="IL2" s="131"/>
+      <c r="IM2" s="131"/>
+      <c r="IN2" s="131"/>
+      <c r="IO2" s="131"/>
+      <c r="IP2" s="131"/>
+      <c r="IQ2" s="131"/>
+      <c r="IR2" s="131"/>
+      <c r="IS2" s="131"/>
+      <c r="IT2" s="131"/>
+      <c r="IU2" s="131"/>
     </row>
     <row r="3" spans="1:255" s="16" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="135" t="s">
+      <c r="A3" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="134" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="113" t="s">
@@ -6103,274 +6115,274 @@
       <c r="E3" s="113" t="s">
         <v>194</v>
       </c>
-      <c r="F3" s="135" t="s">
+      <c r="F3" s="134" t="s">
         <v>195</v>
       </c>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
-      <c r="M3" s="132"/>
-      <c r="N3" s="132"/>
-      <c r="O3" s="132"/>
-      <c r="P3" s="132"/>
-      <c r="Q3" s="132"/>
-      <c r="R3" s="132"/>
-      <c r="S3" s="132"/>
-      <c r="T3" s="132"/>
-      <c r="U3" s="132"/>
-      <c r="V3" s="132"/>
-      <c r="W3" s="132"/>
-      <c r="X3" s="132"/>
-      <c r="Y3" s="132"/>
-      <c r="Z3" s="132"/>
-      <c r="AA3" s="132"/>
-      <c r="AB3" s="132"/>
-      <c r="AC3" s="132"/>
-      <c r="AD3" s="132"/>
-      <c r="AE3" s="132"/>
-      <c r="AF3" s="132"/>
-      <c r="AG3" s="132"/>
-      <c r="AH3" s="132"/>
-      <c r="AI3" s="132"/>
-      <c r="AJ3" s="132"/>
-      <c r="AK3" s="132"/>
-      <c r="AL3" s="132"/>
-      <c r="AM3" s="132"/>
-      <c r="AN3" s="132"/>
-      <c r="AO3" s="132"/>
-      <c r="AP3" s="132"/>
-      <c r="AQ3" s="132"/>
-      <c r="AR3" s="132"/>
-      <c r="AS3" s="132"/>
-      <c r="AT3" s="132"/>
-      <c r="AU3" s="132"/>
-      <c r="AV3" s="132"/>
-      <c r="AW3" s="132"/>
-      <c r="AX3" s="132"/>
-      <c r="AY3" s="132"/>
-      <c r="AZ3" s="132"/>
-      <c r="BA3" s="132"/>
-      <c r="BB3" s="132"/>
-      <c r="BC3" s="132"/>
-      <c r="BD3" s="132"/>
-      <c r="BE3" s="132"/>
-      <c r="BF3" s="132"/>
-      <c r="BG3" s="132"/>
-      <c r="BH3" s="132"/>
-      <c r="BI3" s="132"/>
-      <c r="BJ3" s="132"/>
-      <c r="BK3" s="132"/>
-      <c r="BL3" s="132"/>
-      <c r="BM3" s="132"/>
-      <c r="BN3" s="132"/>
-      <c r="BO3" s="132"/>
-      <c r="BP3" s="132"/>
-      <c r="BQ3" s="132"/>
-      <c r="BR3" s="132"/>
-      <c r="BS3" s="132"/>
-      <c r="BT3" s="132"/>
-      <c r="BU3" s="132"/>
-      <c r="BV3" s="132"/>
-      <c r="BW3" s="132"/>
-      <c r="BX3" s="132"/>
-      <c r="BY3" s="132"/>
-      <c r="BZ3" s="132"/>
-      <c r="CA3" s="132"/>
-      <c r="CB3" s="132"/>
-      <c r="CC3" s="132"/>
-      <c r="CD3" s="132"/>
-      <c r="CE3" s="132"/>
-      <c r="CF3" s="132"/>
-      <c r="CG3" s="132"/>
-      <c r="CH3" s="132"/>
-      <c r="CI3" s="132"/>
-      <c r="CJ3" s="132"/>
-      <c r="CK3" s="132"/>
-      <c r="CL3" s="132"/>
-      <c r="CM3" s="132"/>
-      <c r="CN3" s="132"/>
-      <c r="CO3" s="132"/>
-      <c r="CP3" s="132"/>
-      <c r="CQ3" s="132"/>
-      <c r="CR3" s="132"/>
-      <c r="CS3" s="132"/>
-      <c r="CT3" s="132"/>
-      <c r="CU3" s="132"/>
-      <c r="CV3" s="132"/>
-      <c r="CW3" s="132"/>
-      <c r="CX3" s="132"/>
-      <c r="CY3" s="132"/>
-      <c r="CZ3" s="132"/>
-      <c r="DA3" s="132"/>
-      <c r="DB3" s="132"/>
-      <c r="DC3" s="132"/>
-      <c r="DD3" s="132"/>
-      <c r="DE3" s="132"/>
-      <c r="DF3" s="132"/>
-      <c r="DG3" s="132"/>
-      <c r="DH3" s="132"/>
-      <c r="DI3" s="132"/>
-      <c r="DJ3" s="132"/>
-      <c r="DK3" s="132"/>
-      <c r="DL3" s="132"/>
-      <c r="DM3" s="132"/>
-      <c r="DN3" s="132"/>
-      <c r="DO3" s="132"/>
-      <c r="DP3" s="132"/>
-      <c r="DQ3" s="132"/>
-      <c r="DR3" s="132"/>
-      <c r="DS3" s="132"/>
-      <c r="DT3" s="132"/>
-      <c r="DU3" s="132"/>
-      <c r="DV3" s="132"/>
-      <c r="DW3" s="132"/>
-      <c r="DX3" s="132"/>
-      <c r="DY3" s="132"/>
-      <c r="DZ3" s="132"/>
-      <c r="EA3" s="132"/>
-      <c r="EB3" s="132"/>
-      <c r="EC3" s="132"/>
-      <c r="ED3" s="132"/>
-      <c r="EE3" s="132"/>
-      <c r="EF3" s="132"/>
-      <c r="EG3" s="132"/>
-      <c r="EH3" s="132"/>
-      <c r="EI3" s="132"/>
-      <c r="EJ3" s="132"/>
-      <c r="EK3" s="132"/>
-      <c r="EL3" s="132"/>
-      <c r="EM3" s="132"/>
-      <c r="EN3" s="132"/>
-      <c r="EO3" s="132"/>
-      <c r="EP3" s="132"/>
-      <c r="EQ3" s="132"/>
-      <c r="ER3" s="132"/>
-      <c r="ES3" s="132"/>
-      <c r="ET3" s="132"/>
-      <c r="EU3" s="132"/>
-      <c r="EV3" s="132"/>
-      <c r="EW3" s="132"/>
-      <c r="EX3" s="132"/>
-      <c r="EY3" s="132"/>
-      <c r="EZ3" s="132"/>
-      <c r="FA3" s="132"/>
-      <c r="FB3" s="132"/>
-      <c r="FC3" s="132"/>
-      <c r="FD3" s="132"/>
-      <c r="FE3" s="132"/>
-      <c r="FF3" s="132"/>
-      <c r="FG3" s="132"/>
-      <c r="FH3" s="132"/>
-      <c r="FI3" s="132"/>
-      <c r="FJ3" s="132"/>
-      <c r="FK3" s="132"/>
-      <c r="FL3" s="132"/>
-      <c r="FM3" s="132"/>
-      <c r="FN3" s="132"/>
-      <c r="FO3" s="132"/>
-      <c r="FP3" s="132"/>
-      <c r="FQ3" s="132"/>
-      <c r="FR3" s="132"/>
-      <c r="FS3" s="132"/>
-      <c r="FT3" s="132"/>
-      <c r="FU3" s="132"/>
-      <c r="FV3" s="132"/>
-      <c r="FW3" s="132"/>
-      <c r="FX3" s="132"/>
-      <c r="FY3" s="132"/>
-      <c r="FZ3" s="132"/>
-      <c r="GA3" s="132"/>
-      <c r="GB3" s="132"/>
-      <c r="GC3" s="132"/>
-      <c r="GD3" s="132"/>
-      <c r="GE3" s="132"/>
-      <c r="GF3" s="132"/>
-      <c r="GG3" s="132"/>
-      <c r="GH3" s="132"/>
-      <c r="GI3" s="132"/>
-      <c r="GJ3" s="132"/>
-      <c r="GK3" s="132"/>
-      <c r="GL3" s="132"/>
-      <c r="GM3" s="132"/>
-      <c r="GN3" s="132"/>
-      <c r="GO3" s="132"/>
-      <c r="GP3" s="132"/>
-      <c r="GQ3" s="132"/>
-      <c r="GR3" s="132"/>
-      <c r="GS3" s="132"/>
-      <c r="GT3" s="132"/>
-      <c r="GU3" s="132"/>
-      <c r="GV3" s="132"/>
-      <c r="GW3" s="132"/>
-      <c r="GX3" s="132"/>
-      <c r="GY3" s="132"/>
-      <c r="GZ3" s="132"/>
-      <c r="HA3" s="132"/>
-      <c r="HB3" s="132"/>
-      <c r="HC3" s="132"/>
-      <c r="HD3" s="132"/>
-      <c r="HE3" s="132"/>
-      <c r="HF3" s="132"/>
-      <c r="HG3" s="132"/>
-      <c r="HH3" s="132"/>
-      <c r="HI3" s="132"/>
-      <c r="HJ3" s="132"/>
-      <c r="HK3" s="132"/>
-      <c r="HL3" s="132"/>
-      <c r="HM3" s="132"/>
-      <c r="HN3" s="132"/>
-      <c r="HO3" s="132"/>
-      <c r="HP3" s="132"/>
-      <c r="HQ3" s="132"/>
-      <c r="HR3" s="132"/>
-      <c r="HS3" s="132"/>
-      <c r="HT3" s="132"/>
-      <c r="HU3" s="132"/>
-      <c r="HV3" s="132"/>
-      <c r="HW3" s="132"/>
-      <c r="HX3" s="132"/>
-      <c r="HY3" s="132"/>
-      <c r="HZ3" s="132"/>
-      <c r="IA3" s="132"/>
-      <c r="IB3" s="132"/>
-      <c r="IC3" s="132"/>
-      <c r="ID3" s="132"/>
-      <c r="IE3" s="132"/>
-      <c r="IF3" s="132"/>
-      <c r="IG3" s="132"/>
-      <c r="IH3" s="132"/>
-      <c r="II3" s="132"/>
-      <c r="IJ3" s="132"/>
-      <c r="IK3" s="132"/>
-      <c r="IL3" s="132"/>
-      <c r="IM3" s="132"/>
-      <c r="IN3" s="132"/>
-      <c r="IO3" s="132"/>
-      <c r="IP3" s="132"/>
-      <c r="IQ3" s="132"/>
-      <c r="IR3" s="132"/>
-      <c r="IS3" s="132"/>
-      <c r="IT3" s="132"/>
-      <c r="IU3" s="132"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="131"/>
+      <c r="M3" s="131"/>
+      <c r="N3" s="131"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="131"/>
+      <c r="Q3" s="131"/>
+      <c r="R3" s="131"/>
+      <c r="S3" s="131"/>
+      <c r="T3" s="131"/>
+      <c r="U3" s="131"/>
+      <c r="V3" s="131"/>
+      <c r="W3" s="131"/>
+      <c r="X3" s="131"/>
+      <c r="Y3" s="131"/>
+      <c r="Z3" s="131"/>
+      <c r="AA3" s="131"/>
+      <c r="AB3" s="131"/>
+      <c r="AC3" s="131"/>
+      <c r="AD3" s="131"/>
+      <c r="AE3" s="131"/>
+      <c r="AF3" s="131"/>
+      <c r="AG3" s="131"/>
+      <c r="AH3" s="131"/>
+      <c r="AI3" s="131"/>
+      <c r="AJ3" s="131"/>
+      <c r="AK3" s="131"/>
+      <c r="AL3" s="131"/>
+      <c r="AM3" s="131"/>
+      <c r="AN3" s="131"/>
+      <c r="AO3" s="131"/>
+      <c r="AP3" s="131"/>
+      <c r="AQ3" s="131"/>
+      <c r="AR3" s="131"/>
+      <c r="AS3" s="131"/>
+      <c r="AT3" s="131"/>
+      <c r="AU3" s="131"/>
+      <c r="AV3" s="131"/>
+      <c r="AW3" s="131"/>
+      <c r="AX3" s="131"/>
+      <c r="AY3" s="131"/>
+      <c r="AZ3" s="131"/>
+      <c r="BA3" s="131"/>
+      <c r="BB3" s="131"/>
+      <c r="BC3" s="131"/>
+      <c r="BD3" s="131"/>
+      <c r="BE3" s="131"/>
+      <c r="BF3" s="131"/>
+      <c r="BG3" s="131"/>
+      <c r="BH3" s="131"/>
+      <c r="BI3" s="131"/>
+      <c r="BJ3" s="131"/>
+      <c r="BK3" s="131"/>
+      <c r="BL3" s="131"/>
+      <c r="BM3" s="131"/>
+      <c r="BN3" s="131"/>
+      <c r="BO3" s="131"/>
+      <c r="BP3" s="131"/>
+      <c r="BQ3" s="131"/>
+      <c r="BR3" s="131"/>
+      <c r="BS3" s="131"/>
+      <c r="BT3" s="131"/>
+      <c r="BU3" s="131"/>
+      <c r="BV3" s="131"/>
+      <c r="BW3" s="131"/>
+      <c r="BX3" s="131"/>
+      <c r="BY3" s="131"/>
+      <c r="BZ3" s="131"/>
+      <c r="CA3" s="131"/>
+      <c r="CB3" s="131"/>
+      <c r="CC3" s="131"/>
+      <c r="CD3" s="131"/>
+      <c r="CE3" s="131"/>
+      <c r="CF3" s="131"/>
+      <c r="CG3" s="131"/>
+      <c r="CH3" s="131"/>
+      <c r="CI3" s="131"/>
+      <c r="CJ3" s="131"/>
+      <c r="CK3" s="131"/>
+      <c r="CL3" s="131"/>
+      <c r="CM3" s="131"/>
+      <c r="CN3" s="131"/>
+      <c r="CO3" s="131"/>
+      <c r="CP3" s="131"/>
+      <c r="CQ3" s="131"/>
+      <c r="CR3" s="131"/>
+      <c r="CS3" s="131"/>
+      <c r="CT3" s="131"/>
+      <c r="CU3" s="131"/>
+      <c r="CV3" s="131"/>
+      <c r="CW3" s="131"/>
+      <c r="CX3" s="131"/>
+      <c r="CY3" s="131"/>
+      <c r="CZ3" s="131"/>
+      <c r="DA3" s="131"/>
+      <c r="DB3" s="131"/>
+      <c r="DC3" s="131"/>
+      <c r="DD3" s="131"/>
+      <c r="DE3" s="131"/>
+      <c r="DF3" s="131"/>
+      <c r="DG3" s="131"/>
+      <c r="DH3" s="131"/>
+      <c r="DI3" s="131"/>
+      <c r="DJ3" s="131"/>
+      <c r="DK3" s="131"/>
+      <c r="DL3" s="131"/>
+      <c r="DM3" s="131"/>
+      <c r="DN3" s="131"/>
+      <c r="DO3" s="131"/>
+      <c r="DP3" s="131"/>
+      <c r="DQ3" s="131"/>
+      <c r="DR3" s="131"/>
+      <c r="DS3" s="131"/>
+      <c r="DT3" s="131"/>
+      <c r="DU3" s="131"/>
+      <c r="DV3" s="131"/>
+      <c r="DW3" s="131"/>
+      <c r="DX3" s="131"/>
+      <c r="DY3" s="131"/>
+      <c r="DZ3" s="131"/>
+      <c r="EA3" s="131"/>
+      <c r="EB3" s="131"/>
+      <c r="EC3" s="131"/>
+      <c r="ED3" s="131"/>
+      <c r="EE3" s="131"/>
+      <c r="EF3" s="131"/>
+      <c r="EG3" s="131"/>
+      <c r="EH3" s="131"/>
+      <c r="EI3" s="131"/>
+      <c r="EJ3" s="131"/>
+      <c r="EK3" s="131"/>
+      <c r="EL3" s="131"/>
+      <c r="EM3" s="131"/>
+      <c r="EN3" s="131"/>
+      <c r="EO3" s="131"/>
+      <c r="EP3" s="131"/>
+      <c r="EQ3" s="131"/>
+      <c r="ER3" s="131"/>
+      <c r="ES3" s="131"/>
+      <c r="ET3" s="131"/>
+      <c r="EU3" s="131"/>
+      <c r="EV3" s="131"/>
+      <c r="EW3" s="131"/>
+      <c r="EX3" s="131"/>
+      <c r="EY3" s="131"/>
+      <c r="EZ3" s="131"/>
+      <c r="FA3" s="131"/>
+      <c r="FB3" s="131"/>
+      <c r="FC3" s="131"/>
+      <c r="FD3" s="131"/>
+      <c r="FE3" s="131"/>
+      <c r="FF3" s="131"/>
+      <c r="FG3" s="131"/>
+      <c r="FH3" s="131"/>
+      <c r="FI3" s="131"/>
+      <c r="FJ3" s="131"/>
+      <c r="FK3" s="131"/>
+      <c r="FL3" s="131"/>
+      <c r="FM3" s="131"/>
+      <c r="FN3" s="131"/>
+      <c r="FO3" s="131"/>
+      <c r="FP3" s="131"/>
+      <c r="FQ3" s="131"/>
+      <c r="FR3" s="131"/>
+      <c r="FS3" s="131"/>
+      <c r="FT3" s="131"/>
+      <c r="FU3" s="131"/>
+      <c r="FV3" s="131"/>
+      <c r="FW3" s="131"/>
+      <c r="FX3" s="131"/>
+      <c r="FY3" s="131"/>
+      <c r="FZ3" s="131"/>
+      <c r="GA3" s="131"/>
+      <c r="GB3" s="131"/>
+      <c r="GC3" s="131"/>
+      <c r="GD3" s="131"/>
+      <c r="GE3" s="131"/>
+      <c r="GF3" s="131"/>
+      <c r="GG3" s="131"/>
+      <c r="GH3" s="131"/>
+      <c r="GI3" s="131"/>
+      <c r="GJ3" s="131"/>
+      <c r="GK3" s="131"/>
+      <c r="GL3" s="131"/>
+      <c r="GM3" s="131"/>
+      <c r="GN3" s="131"/>
+      <c r="GO3" s="131"/>
+      <c r="GP3" s="131"/>
+      <c r="GQ3" s="131"/>
+      <c r="GR3" s="131"/>
+      <c r="GS3" s="131"/>
+      <c r="GT3" s="131"/>
+      <c r="GU3" s="131"/>
+      <c r="GV3" s="131"/>
+      <c r="GW3" s="131"/>
+      <c r="GX3" s="131"/>
+      <c r="GY3" s="131"/>
+      <c r="GZ3" s="131"/>
+      <c r="HA3" s="131"/>
+      <c r="HB3" s="131"/>
+      <c r="HC3" s="131"/>
+      <c r="HD3" s="131"/>
+      <c r="HE3" s="131"/>
+      <c r="HF3" s="131"/>
+      <c r="HG3" s="131"/>
+      <c r="HH3" s="131"/>
+      <c r="HI3" s="131"/>
+      <c r="HJ3" s="131"/>
+      <c r="HK3" s="131"/>
+      <c r="HL3" s="131"/>
+      <c r="HM3" s="131"/>
+      <c r="HN3" s="131"/>
+      <c r="HO3" s="131"/>
+      <c r="HP3" s="131"/>
+      <c r="HQ3" s="131"/>
+      <c r="HR3" s="131"/>
+      <c r="HS3" s="131"/>
+      <c r="HT3" s="131"/>
+      <c r="HU3" s="131"/>
+      <c r="HV3" s="131"/>
+      <c r="HW3" s="131"/>
+      <c r="HX3" s="131"/>
+      <c r="HY3" s="131"/>
+      <c r="HZ3" s="131"/>
+      <c r="IA3" s="131"/>
+      <c r="IB3" s="131"/>
+      <c r="IC3" s="131"/>
+      <c r="ID3" s="131"/>
+      <c r="IE3" s="131"/>
+      <c r="IF3" s="131"/>
+      <c r="IG3" s="131"/>
+      <c r="IH3" s="131"/>
+      <c r="II3" s="131"/>
+      <c r="IJ3" s="131"/>
+      <c r="IK3" s="131"/>
+      <c r="IL3" s="131"/>
+      <c r="IM3" s="131"/>
+      <c r="IN3" s="131"/>
+      <c r="IO3" s="131"/>
+      <c r="IP3" s="131"/>
+      <c r="IQ3" s="131"/>
+      <c r="IR3" s="131"/>
+      <c r="IS3" s="131"/>
+      <c r="IT3" s="131"/>
+      <c r="IU3" s="131"/>
     </row>
     <row r="4" spans="1:255" x14ac:dyDescent="0.15">
       <c r="A4" s="25">
         <v>43101</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="D4" s="136" t="s">
+      <c r="C4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" s="135" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F4" s="137" t="s">
+      <c r="E4" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" s="136" t="s">
         <v>195</v>
       </c>
     </row>
@@ -6379,16 +6391,16 @@
         <v>43101</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>253</v>
+      <c r="C5" t="s">
+        <v>273</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>235</v>
       </c>
-      <c r="E5" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F5" s="138" t="s">
+      <c r="E5" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F5" s="137" t="s">
         <v>195</v>
       </c>
     </row>
@@ -6397,16 +6409,16 @@
         <v>43101</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>253</v>
+      <c r="C6" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="E6" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F6" s="138" t="s">
+      <c r="E6" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="137" t="s">
         <v>195</v>
       </c>
     </row>
@@ -6415,16 +6427,16 @@
         <v>43101</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="D7" s="139" t="s">
+      <c r="C7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D7" s="138" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F7" s="140" t="s">
+      <c r="E7" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F7" s="139" t="s">
         <v>195</v>
       </c>
     </row>
@@ -6433,16 +6445,16 @@
         <v>43101</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="D8" s="139" t="s">
+      <c r="C8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D8" s="138" t="s">
         <v>242</v>
       </c>
-      <c r="E8" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="F8" s="140" t="s">
+      <c r="E8" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="F8" s="139" t="s">
         <v>195</v>
       </c>
     </row>
@@ -6585,7 +6597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -6700,10 +6712,10 @@
         <v>43101</v>
       </c>
       <c r="C4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
@@ -6731,8 +6743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6742,7 +6754,7 @@
     <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32" style="142" customWidth="1"/>
+    <col min="6" max="6" width="32" style="141" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="21.83203125" customWidth="1"/>
     <col min="9" max="9" width="24.5" customWidth="1"/>
@@ -6938,7 +6950,7 @@
       </c>
       <c r="B4" s="50"/>
       <c r="C4" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>211</v>
@@ -6963,7 +6975,7 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>212</v>
@@ -6988,7 +7000,7 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
@@ -7011,7 +7023,7 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>209</v>
@@ -7034,7 +7046,7 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>210</v>
@@ -7044,7 +7056,7 @@
       </c>
       <c r="F8" s="73"/>
       <c r="G8" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H8" s="5"/>
       <c r="J8" s="5" t="s">
@@ -7057,7 +7069,7 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>247</v>
@@ -7067,7 +7079,7 @@
       </c>
       <c r="F9" s="73"/>
       <c r="G9" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" s="5" t="s">
@@ -7080,13 +7092,13 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="F10" s="73"/>
       <c r="G10" s="5" t="s">
@@ -7105,7 +7117,7 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>56</v>
@@ -7130,7 +7142,7 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>220</v>
@@ -7389,7 +7401,7 @@
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K6" s="60" t="s">
         <v>32</v>
@@ -7403,13 +7415,13 @@
         <v>231</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>72</v>
@@ -7427,14 +7439,14 @@
         <v>231</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>74</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="60"/>
@@ -7457,12 +7469,12 @@
         <v>231</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="143"/>
+      <c r="F9" s="142"/>
       <c r="G9" s="16" t="s">
         <v>75</v>
       </c>
@@ -7478,7 +7490,7 @@
         <v>231</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>52</v>
@@ -7499,10 +7511,10 @@
         <v>231</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
@@ -7613,7 +7625,7 @@
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="56" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D4" s="57" t="s">
         <v>233</v>
@@ -7640,7 +7652,7 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D5" s="62" t="s">
         <v>82</v>
@@ -7678,7 +7690,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7782,8 +7794,8 @@
         <v>43101</v>
       </c>
       <c r="B4" s="71"/>
-      <c r="C4" s="5" t="s">
-        <v>253</v>
+      <c r="C4" t="s">
+        <v>273</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>92</v>
@@ -7803,8 +7815,8 @@
         <v>43101</v>
       </c>
       <c r="B5" s="71"/>
-      <c r="C5" s="5" t="s">
-        <v>253</v>
+      <c r="C5" t="s">
+        <v>273</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>235</v>
@@ -7824,8 +7836,8 @@
         <v>43101</v>
       </c>
       <c r="B6" s="71"/>
-      <c r="C6" s="5" t="s">
-        <v>253</v>
+      <c r="C6" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>236</v>
@@ -7844,8 +7856,8 @@
       <c r="A7" s="25">
         <v>43101</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>253</v>
+      <c r="C7" t="s">
+        <v>273</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>93</v>
@@ -7864,8 +7876,8 @@
       <c r="A8" s="25">
         <v>43101</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>253</v>
+      <c r="C8" t="s">
+        <v>273</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>242</v>
@@ -7904,8 +7916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8093,8 +8105,8 @@
         <v>43101</v>
       </c>
       <c r="B4" s="71"/>
-      <c r="C4" s="5" t="s">
-        <v>253</v>
+      <c r="C4" t="s">
+        <v>273</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>216</v>
@@ -8125,8 +8137,8 @@
         <v>43101</v>
       </c>
       <c r="B5" s="71"/>
-      <c r="C5" s="5" t="s">
-        <v>253</v>
+      <c r="C5" t="s">
+        <v>273</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>214</v>
@@ -8148,11 +8160,11 @@
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="144" t="s">
-        <v>273</v>
+      <c r="L5" s="143" t="s">
+        <v>272</v>
       </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="144"/>
+      <c r="N5" s="143"/>
       <c r="P5" s="51" t="s">
         <v>119</v>
       </c>
@@ -8168,8 +8180,8 @@
         <v>43101</v>
       </c>
       <c r="B6" s="71"/>
-      <c r="C6" s="5" t="s">
-        <v>253</v>
+      <c r="C6" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>215</v>
@@ -8191,11 +8203,11 @@
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="144" t="s">
+      <c r="L6" s="143" t="s">
         <v>248</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="144"/>
+      <c r="N6" s="143"/>
       <c r="P6" s="5" t="s">
         <v>119</v>
       </c>
@@ -8211,8 +8223,8 @@
         <v>43101</v>
       </c>
       <c r="B7" s="71"/>
-      <c r="C7" s="5" t="s">
-        <v>253</v>
+      <c r="C7" t="s">
+        <v>273</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>122</v>
@@ -8236,7 +8248,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="144"/>
+      <c r="N7" s="143"/>
       <c r="P7" s="51" t="s">
         <v>119</v>
       </c>
@@ -8252,8 +8264,8 @@
         <v>43101</v>
       </c>
       <c r="B8" s="71"/>
-      <c r="C8" s="5" t="s">
-        <v>253</v>
+      <c r="C8" t="s">
+        <v>273</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>124</v>
@@ -8311,8 +8323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8475,8 +8487,8 @@
         <v>43101</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="60" t="s">
-        <v>253</v>
+      <c r="C4" t="s">
+        <v>273</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
@@ -8509,14 +8521,14 @@
         <v>43101</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="60" t="s">
-        <v>253</v>
+      <c r="C5" t="s">
+        <v>273</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>214</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
@@ -8543,8 +8555,8 @@
         <v>43101</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="60" t="s">
-        <v>253</v>
+      <c r="C6" t="s">
+        <v>273</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>122</v>
@@ -8577,14 +8589,14 @@
         <v>43101</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="60" t="s">
-        <v>253</v>
+      <c r="C7" t="s">
+        <v>273</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>122</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F7" s="72">
         <v>2</v>
@@ -8611,14 +8623,14 @@
         <v>43101</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="60" t="s">
-        <v>253</v>
+      <c r="C8" t="s">
+        <v>273</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F8" s="72">
         <v>1</v>
@@ -8645,8 +8657,8 @@
         <v>43101</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="60" t="s">
-        <v>253</v>
+      <c r="C9" t="s">
+        <v>273</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>215</v>
@@ -8679,14 +8691,14 @@
         <v>43101</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="60" t="s">
-        <v>253</v>
+      <c r="C10" t="s">
+        <v>273</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>124</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F10" s="72">
         <v>1</v>
@@ -8709,8 +8721,8 @@
         <v>43101</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="60" t="s">
-        <v>253</v>
+      <c r="C11" t="s">
+        <v>273</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
BPS-403 Renamed exception record case name
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD27AE1-93A5-B744-A802-C2A61BEC6F88}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE71B1A9-BA5E-6940-9A5E-20A687777EE2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -878,9 +878,6 @@
     <t>Bulk Scanning</t>
   </si>
   <si>
-    <t>Exception Record</t>
-  </si>
-  <si>
     <t>caseworker-bulkscan</t>
   </si>
   <si>
@@ -942,6 +939,9 @@
   </si>
   <si>
     <t>Renamed exception record case type</t>
+  </si>
+  <si>
+    <t>Bulk Scanning Exception Record</t>
   </si>
 </sst>
 </file>
@@ -952,7 +952,7 @@
     <numFmt numFmtId="164" formatCode="d\ mmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1170,6 +1170,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF424242"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1314,7 +1320,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1583,6 +1589,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -2032,7 +2039,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -2049,7 +2056,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -2066,7 +2073,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -2075,7 +2082,7 @@
         <v>43404</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -2083,7 +2090,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -2092,7 +2099,7 @@
         <v>43420</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -2100,7 +2107,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>6</v>
@@ -2109,7 +2116,7 @@
         <v>43441</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2254,7 +2261,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>167</v>
@@ -2281,7 +2288,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>167</v>
@@ -2308,7 +2315,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>167</v>
@@ -2335,7 +2342,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>167</v>
@@ -2362,7 +2369,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" s="60" t="s">
         <v>167</v>
@@ -2389,7 +2396,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D9" s="60" t="s">
         <v>167</v>
@@ -2416,7 +2423,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>167</v>
@@ -2443,7 +2450,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>167</v>
@@ -2458,7 +2465,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I11" s="86">
         <v>1</v>
@@ -2470,7 +2477,7 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D12" s="60" t="s">
         <v>167</v>
@@ -2604,7 +2611,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>210</v>
@@ -2643,7 +2650,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>247</v>
@@ -2661,7 +2668,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
@@ -2679,7 +2686,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>209</v>
@@ -2697,7 +2704,7 @@
       </c>
       <c r="B8" s="60"/>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>220</v>
@@ -2865,13 +2872,13 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>228</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F4" s="140">
         <v>1</v>
@@ -2888,7 +2895,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" t="s">
         <v>179</v>
@@ -2927,7 +2934,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>210</v>
@@ -2966,7 +2973,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>220</v>
@@ -3233,13 +3240,13 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>228</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F4" s="140">
         <v>1</v>
@@ -3272,7 +3279,7 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" t="s">
         <v>179</v>
@@ -3311,7 +3318,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>210</v>
@@ -3350,7 +3357,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>220</v>
@@ -3486,13 +3493,13 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="107" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>251</v>
       </c>
       <c r="E4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F4" s="60" t="s">
         <v>92</v>
@@ -4327,10 +4334,10 @@
       </c>
       <c r="B4" s="51"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>195</v>
@@ -4446,13 +4453,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E4" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F4" s="116" t="s">
         <v>195</v>
@@ -4463,13 +4470,13 @@
         <v>43101</v>
       </c>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>212</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F5" s="118" t="s">
         <v>195</v>
@@ -4480,13 +4487,13 @@
         <v>43101</v>
       </c>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
       </c>
       <c r="E6" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F6" s="118" t="s">
         <v>195</v>
@@ -4497,13 +4504,13 @@
         <v>43101</v>
       </c>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>209</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="118" t="s">
         <v>195</v>
@@ -4514,13 +4521,13 @@
         <v>43101</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>210</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F8" s="118" t="s">
         <v>195</v>
@@ -4531,13 +4538,13 @@
         <v>43101</v>
       </c>
       <c r="C9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>247</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F9" s="118" t="s">
         <v>195</v>
@@ -4548,13 +4555,13 @@
         <v>43101</v>
       </c>
       <c r="C10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E10" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F10" s="118" t="s">
         <v>195</v>
@@ -4565,13 +4572,13 @@
         <v>43101</v>
       </c>
       <c r="C11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E11" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F11" s="118" t="s">
         <v>195</v>
@@ -4582,13 +4589,13 @@
         <v>43101</v>
       </c>
       <c r="C12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>220</v>
       </c>
       <c r="E12" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F12" s="118" t="s">
         <v>195</v>
@@ -5434,13 +5441,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>216</v>
       </c>
       <c r="E4" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F4" s="116" t="s">
         <v>195</v>
@@ -5452,13 +5459,13 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>214</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F5" s="118" t="s">
         <v>195</v>
@@ -5470,13 +5477,13 @@
       </c>
       <c r="B6" s="51"/>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>122</v>
       </c>
       <c r="E6" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F6" s="122" t="s">
         <v>195</v>
@@ -5488,13 +5495,13 @@
       </c>
       <c r="B7" s="121"/>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="118" t="s">
         <v>195</v>
@@ -5506,13 +5513,13 @@
       </c>
       <c r="B8" s="123"/>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>124</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F8" s="120" t="s">
         <v>195</v>
@@ -6374,13 +6381,13 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="135" t="s">
         <v>92</v>
       </c>
       <c r="E4" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F4" s="136" t="s">
         <v>195</v>
@@ -6392,13 +6399,13 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>235</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F5" s="137" t="s">
         <v>195</v>
@@ -6410,13 +6417,13 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>236</v>
       </c>
       <c r="E6" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F6" s="137" t="s">
         <v>195</v>
@@ -6428,13 +6435,13 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="138" t="s">
         <v>93</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F7" s="139" t="s">
         <v>195</v>
@@ -6446,13 +6453,13 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" s="138" t="s">
         <v>242</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F8" s="139" t="s">
         <v>195</v>
@@ -6597,8 +6604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6712,10 +6719,10 @@
         <v>43101</v>
       </c>
       <c r="C4" t="s">
-        <v>273</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>253</v>
+        <v>272</v>
+      </c>
+      <c r="D4" s="145" t="s">
+        <v>274</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
@@ -6950,7 +6957,7 @@
       </c>
       <c r="B4" s="50"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>211</v>
@@ -6975,7 +6982,7 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>212</v>
@@ -7000,7 +7007,7 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
@@ -7023,7 +7030,7 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>209</v>
@@ -7046,7 +7053,7 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>210</v>
@@ -7056,7 +7063,7 @@
       </c>
       <c r="F8" s="73"/>
       <c r="G8" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H8" s="5"/>
       <c r="J8" s="5" t="s">
@@ -7069,7 +7076,7 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>247</v>
@@ -7079,7 +7086,7 @@
       </c>
       <c r="F9" s="73"/>
       <c r="G9" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" s="5" t="s">
@@ -7092,13 +7099,13 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="F10" s="73"/>
       <c r="G10" s="5" t="s">
@@ -7117,7 +7124,7 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>56</v>
@@ -7142,7 +7149,7 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>220</v>
@@ -7401,7 +7408,7 @@
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K6" s="60" t="s">
         <v>32</v>
@@ -7415,13 +7422,13 @@
         <v>231</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>72</v>
@@ -7439,14 +7446,14 @@
         <v>231</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>74</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="60"/>
@@ -7469,7 +7476,7 @@
         <v>231</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>52</v>
@@ -7490,7 +7497,7 @@
         <v>231</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>52</v>
@@ -7511,10 +7518,10 @@
         <v>231</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
@@ -7625,7 +7632,7 @@
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="56" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D4" s="57" t="s">
         <v>233</v>
@@ -7652,7 +7659,7 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="61" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D5" s="62" t="s">
         <v>82</v>
@@ -7795,7 +7802,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>92</v>
@@ -7816,7 +7823,7 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>235</v>
@@ -7837,7 +7844,7 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>236</v>
@@ -7857,7 +7864,7 @@
         <v>43101</v>
       </c>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>93</v>
@@ -7877,7 +7884,7 @@
         <v>43101</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>242</v>
@@ -7916,7 +7923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -8106,7 +8113,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>216</v>
@@ -8138,7 +8145,7 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>214</v>
@@ -8161,7 +8168,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="143" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="143"/>
@@ -8181,7 +8188,7 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>215</v>
@@ -8224,7 +8231,7 @@
       </c>
       <c r="B7" s="71"/>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>122</v>
@@ -8265,7 +8272,7 @@
       </c>
       <c r="B8" s="71"/>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>124</v>
@@ -8488,7 +8495,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
@@ -8522,13 +8529,13 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>214</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
@@ -8556,7 +8563,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>122</v>
@@ -8590,13 +8597,13 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>122</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F7" s="72">
         <v>2</v>
@@ -8624,13 +8631,13 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F8" s="72">
         <v>1</v>
@@ -8658,7 +8665,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>215</v>
@@ -8692,13 +8699,13 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>124</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F10" s="72">
         <v>1</v>
@@ -8722,7 +8729,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
BPS-449 Added subtype to Document complex type
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE71B1A9-BA5E-6940-9A5E-20A687777EE2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC08258-CCD7-3346-8600-CC85701C7D04}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="278">
   <si>
     <t>Change History</t>
   </si>
@@ -942,6 +942,15 @@
   </si>
   <si>
     <t>Bulk Scanning Exception Record</t>
+  </si>
+  <si>
+    <t>subtype</t>
+  </si>
+  <si>
+    <t>Subtype</t>
+  </si>
+  <si>
+    <t>Added subtype to Document complex type</t>
   </si>
 </sst>
 </file>
@@ -1974,10 +1983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2116,6 +2125,23 @@
         <v>43441</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="144">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="9">
+        <v>43479</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7186,10 +7212,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7437,57 +7463,57 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="25">
         <v>43101</v>
       </c>
-      <c r="B8" s="55"/>
       <c r="C8" s="65" t="s">
         <v>231</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="5"/>
+        <v>276</v>
+      </c>
       <c r="K8" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="25">
         <v>43101</v>
       </c>
+      <c r="B9" s="55"/>
       <c r="C9" s="65" t="s">
         <v>231</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="142"/>
+        <v>74</v>
+      </c>
+      <c r="F9" s="16"/>
       <c r="G9" s="16" t="s">
-        <v>75</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="60" t="s">
         <v>32</v>
       </c>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="25">
@@ -7497,14 +7523,14 @@
         <v>231</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="16"/>
+      <c r="F10" s="142"/>
       <c r="G10" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K10" s="60" t="s">
         <v>32</v>
@@ -7518,22 +7544,43 @@
         <v>231</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>260</v>
+        <v>52</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
-        <v>232</v>
+        <v>76</v>
       </c>
       <c r="K11" s="60" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A12" s="25">
+        <v>43101</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="K12" s="60" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A12" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7923,7 +7970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revert "BPS-449 Added subtype to Document complex type (#56)"
This reverts commit a4029e4
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC08258-CCD7-3346-8600-CC85701C7D04}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE71B1A9-BA5E-6940-9A5E-20A687777EE2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="275">
   <si>
     <t>Change History</t>
   </si>
@@ -942,15 +942,6 @@
   </si>
   <si>
     <t>Bulk Scanning Exception Record</t>
-  </si>
-  <si>
-    <t>subtype</t>
-  </si>
-  <si>
-    <t>Subtype</t>
-  </si>
-  <si>
-    <t>Added subtype to Document complex type</t>
   </si>
 </sst>
 </file>
@@ -1983,10 +1974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2125,23 +2116,6 @@
         <v>43441</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="144">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>277</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="9">
-        <v>43479</v>
-      </c>
-      <c r="E10" s="2" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7212,10 +7186,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7463,57 +7437,57 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="25">
         <v>43101</v>
       </c>
+      <c r="B8" s="55"/>
       <c r="C8" s="65" t="s">
         <v>231</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>276</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="60" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" s="25">
         <v>43101</v>
       </c>
-      <c r="B9" s="55"/>
       <c r="C9" s="65" t="s">
         <v>231</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="16"/>
+        <v>52</v>
+      </c>
+      <c r="F9" s="142"/>
       <c r="G9" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="5"/>
+        <v>75</v>
+      </c>
       <c r="K9" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="25">
@@ -7523,14 +7497,14 @@
         <v>231</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="142"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K10" s="60" t="s">
         <v>32</v>
@@ -7544,43 +7518,22 @@
         <v>231</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>52</v>
+        <v>260</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
-        <v>76</v>
+        <v>232</v>
       </c>
       <c r="K11" s="60" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A12" s="25">
-        <v>43101</v>
-      </c>
-      <c r="C12" s="65" t="s">
-        <v>231</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="K12" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A12" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7970,7 +7923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add fields for referencing a case when attaching exception record
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566FC1C1-A4BB-DE46-A2FC-7101A3A0D95B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CECB56-523A-2B4B-9656-B7E894FD8AC1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,15 @@
     <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId18"/>
     <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -43,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="300">
   <si>
     <t>Change History</t>
   </si>
@@ -782,9 +789,6 @@
     <t>attachToCaseReference</t>
   </si>
   <si>
-    <t>The number of the case to attach the envelop to</t>
-  </si>
-  <si>
     <t>POBox Jurisdiction</t>
   </si>
   <si>
@@ -969,6 +973,57 @@
   </si>
   <si>
     <t>eventHistory</t>
+  </si>
+  <si>
+    <t>The number of the case to attach the envelope to</t>
+  </si>
+  <si>
+    <t>Case Reference Type</t>
+  </si>
+  <si>
+    <t>Select the type of reference on which case needs to be searched</t>
+  </si>
+  <si>
+    <t>ReferenceType</t>
+  </si>
+  <si>
+    <t>caseReference</t>
+  </si>
+  <si>
+    <t>Case Reference</t>
+  </si>
+  <si>
+    <t>searchCaseReferenceType</t>
+  </si>
+  <si>
+    <t>searchCaseReference</t>
+  </si>
+  <si>
+    <t>Attached to Case Reference</t>
+  </si>
+  <si>
+    <t>CCD Case Reference</t>
+  </si>
+  <si>
+    <t>externalCaseReference</t>
+  </si>
+  <si>
+    <t>External Case Reference</t>
+  </si>
+  <si>
+    <t>The CCD reference number of the case the exception record is attached to</t>
+  </si>
+  <si>
+    <t>Changed the Label and HintText of attachToCaseReference field</t>
+  </si>
+  <si>
+    <t>Leszek Gonczar</t>
+  </si>
+  <si>
+    <t>Added searchCaseReference and searchCaseReferenceType fields</t>
+  </si>
+  <si>
+    <t>MANDATORY</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1402,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1617,6 +1672,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -2001,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2012,7 +2069,7 @@
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
     <col min="7" max="1025" width="11.5"/>
@@ -2049,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -2058,7 +2115,7 @@
         <v>43384</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2066,7 +2123,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -2075,7 +2132,7 @@
         <v>43399</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -2083,7 +2140,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -2092,7 +2149,7 @@
         <v>43399</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -2100,7 +2157,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -2109,7 +2166,7 @@
         <v>43404</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -2117,7 +2174,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -2126,7 +2183,7 @@
         <v>43420</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -2134,7 +2191,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>6</v>
@@ -2143,7 +2200,7 @@
         <v>43441</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -2151,7 +2208,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -2160,7 +2217,7 @@
         <v>43481</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -2168,7 +2225,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
@@ -2177,7 +2234,41 @@
         <v>43544</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="144">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>298</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6">
+        <v>43606</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="144">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6">
+        <v>43606</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -2194,15 +2285,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N1048546"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
@@ -2322,22 +2413,22 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>167</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G4" s="86">
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I4" s="86">
         <v>1</v>
@@ -2349,16 +2440,16 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>167</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F5" s="60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G5" s="86">
         <v>2</v>
@@ -2376,16 +2467,16 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>167</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G6" s="86">
         <v>2</v>
@@ -2403,16 +2494,16 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>167</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F7" s="60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G7" s="86">
         <v>2</v>
@@ -2430,16 +2521,16 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="60" t="s">
         <v>167</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F8" s="60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G8" s="86">
         <v>2</v>
@@ -2457,16 +2548,16 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D9" s="60" t="s">
         <v>167</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F9" s="60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G9" s="86">
         <v>2</v>
@@ -2484,22 +2575,22 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>167</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F10" s="60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G10" s="86">
         <v>2</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I10" s="86">
         <v>6</v>
@@ -2511,16 +2602,16 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>167</v>
       </c>
       <c r="E11" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F11" s="60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G11" s="86">
         <v>2</v>
@@ -2538,7 +2629,7 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D12" s="60" t="s">
         <v>167</v>
@@ -2553,7 +2644,7 @@
         <v>3</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I12" s="86">
         <v>1</v>
@@ -2565,16 +2656,16 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D13" s="60" t="s">
         <v>167</v>
       </c>
       <c r="E13" s="60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F13" s="60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G13" s="86">
         <v>4</v>
@@ -2621,7 +2712,7 @@
   <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2699,7 +2790,7 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>210</v>
@@ -2738,13 +2829,13 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
@@ -2756,7 +2847,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
@@ -2774,13 +2865,13 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>209</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>
@@ -2792,7 +2883,7 @@
       </c>
       <c r="B8" s="60"/>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>220</v>
@@ -2960,13 +3051,13 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F4" s="140">
         <v>1</v>
@@ -2983,13 +3074,13 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" t="s">
         <v>179</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
@@ -3022,7 +3113,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>210</v>
@@ -3061,7 +3152,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>220</v>
@@ -3235,7 +3326,7 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3328,13 +3419,13 @@
       </c>
       <c r="B4" s="60"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F4" s="140">
         <v>1</v>
@@ -3367,13 +3458,13 @@
       </c>
       <c r="B5" s="60"/>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" t="s">
         <v>179</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
@@ -3406,7 +3497,7 @@
       </c>
       <c r="B6" s="60"/>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>210</v>
@@ -3445,7 +3536,7 @@
       </c>
       <c r="B7" s="60"/>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>220</v>
@@ -3581,13 +3672,13 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="107" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D4" s="60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F4" s="60" t="s">
         <v>92</v>
@@ -4422,10 +4513,10 @@
       </c>
       <c r="B4" s="51"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>195</v>
@@ -4446,10 +4537,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="136" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="136" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4541,13 +4632,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E4" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F4" s="116" t="s">
         <v>195</v>
@@ -4558,13 +4649,13 @@
         <v>43101</v>
       </c>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>212</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F5" s="118" t="s">
         <v>195</v>
@@ -4575,13 +4666,13 @@
         <v>43101</v>
       </c>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
       </c>
       <c r="E6" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F6" s="118" t="s">
         <v>195</v>
@@ -4592,13 +4683,13 @@
         <v>43101</v>
       </c>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>209</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F7" s="118" t="s">
         <v>195</v>
@@ -4609,13 +4700,13 @@
         <v>43101</v>
       </c>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>210</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F8" s="118" t="s">
         <v>195</v>
@@ -4626,13 +4717,13 @@
         <v>43101</v>
       </c>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F9" s="118" t="s">
         <v>195</v>
@@ -4643,13 +4734,13 @@
         <v>43101</v>
       </c>
       <c r="C10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E10" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F10" s="118" t="s">
         <v>195</v>
@@ -4660,13 +4751,13 @@
         <v>43101</v>
       </c>
       <c r="C11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E11" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F11" s="118" t="s">
         <v>195</v>
@@ -4677,13 +4768,13 @@
         <v>43101</v>
       </c>
       <c r="C12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>220</v>
       </c>
       <c r="E12" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F12" s="118" t="s">
         <v>195</v>
@@ -4694,21 +4785,55 @@
         <v>43101</v>
       </c>
       <c r="C13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E13" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F13" s="118" t="s">
         <v>195</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A14" s="117">
+        <v>43101</v>
+      </c>
+      <c r="C14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="E14" s="115" t="s">
+        <v>252</v>
+      </c>
+      <c r="F14" s="118" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A15" s="117">
+        <v>43101</v>
+      </c>
+      <c r="C15" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E15" s="115" t="s">
+        <v>252</v>
+      </c>
+      <c r="F15" s="118" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A13" xr:uid="{00000000-0002-0000-1000-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5546,13 +5671,13 @@
       </c>
       <c r="B4" s="58"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>216</v>
       </c>
       <c r="E4" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F4" s="116" t="s">
         <v>195</v>
@@ -5564,13 +5689,13 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>214</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F5" s="118" t="s">
         <v>195</v>
@@ -5582,13 +5707,13 @@
       </c>
       <c r="B6" s="51"/>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>122</v>
       </c>
       <c r="E6" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F6" s="122" t="s">
         <v>195</v>
@@ -5600,13 +5725,13 @@
       </c>
       <c r="B7" s="121"/>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F7" s="118" t="s">
         <v>195</v>
@@ -5618,13 +5743,13 @@
       </c>
       <c r="B8" s="123"/>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>124</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F8" s="120" t="s">
         <v>195</v>
@@ -6486,13 +6611,13 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="135" t="s">
         <v>92</v>
       </c>
       <c r="E4" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F4" s="136" t="s">
         <v>195</v>
@@ -6504,13 +6629,13 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F5" s="137" t="s">
         <v>195</v>
@@ -6522,13 +6647,13 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E6" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F6" s="137" t="s">
         <v>195</v>
@@ -6540,13 +6665,13 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="138" t="s">
         <v>93</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F7" s="139" t="s">
         <v>195</v>
@@ -6558,13 +6683,13 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="138" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F8" s="139" t="s">
         <v>195</v>
@@ -6680,13 +6805,13 @@
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>252</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -6824,14 +6949,14 @@
         <v>43101</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="145" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -6853,10 +6978,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ13"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7062,13 +7187,13 @@
       </c>
       <c r="B4" s="50"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F4" s="73" t="s">
         <v>51</v>
@@ -7087,7 +7212,7 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>212</v>
@@ -7096,7 +7221,7 @@
         <v>213</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>52</v>
@@ -7112,7 +7237,7 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
@@ -7135,7 +7260,7 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>209</v>
@@ -7158,7 +7283,7 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>210</v>
@@ -7168,7 +7293,7 @@
       </c>
       <c r="F8" s="73"/>
       <c r="G8" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H8" s="5"/>
       <c r="J8" s="5" t="s">
@@ -7181,17 +7306,17 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F9" s="73"/>
       <c r="G9" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H9" s="5"/>
       <c r="J9" s="5" t="s">
@@ -7204,20 +7329,20 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>265</v>
       </c>
       <c r="F10" s="73"/>
       <c r="G10" s="5" t="s">
         <v>55</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>32</v>
@@ -7229,13 +7354,13 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F11" s="73"/>
       <c r="G11" s="5" t="s">
@@ -7248,22 +7373,22 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" ht="28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:1024" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="25">
         <v>43101</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>220</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>219</v>
+        <v>291</v>
       </c>
       <c r="F12" s="73" t="s">
-        <v>221</v>
+        <v>295</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>52</v>
@@ -7279,30 +7404,82 @@
       </c>
       <c r="B13" s="50"/>
       <c r="C13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F13" s="73"/>
       <c r="G13" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H13" s="5"/>
       <c r="J13" s="5" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="14" spans="1:1024" ht="28" x14ac:dyDescent="0.15">
+      <c r="A14" s="25">
+        <v>43101</v>
+      </c>
+      <c r="B14" s="50"/>
+      <c r="C14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="F14" s="73" t="s">
+        <v>285</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1024" ht="28" x14ac:dyDescent="0.15">
+      <c r="A15" s="25">
+        <v>43101</v>
+      </c>
+      <c r="B15" s="50"/>
+      <c r="C15" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="F15" s="73" t="s">
+        <v>283</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="J15" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A13" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B13" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7316,8 +7493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView topLeftCell="A2" zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7526,7 +7703,7 @@
         <v>43101</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>71</v>
@@ -7536,7 +7713,7 @@
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K6" s="60" t="s">
         <v>32</v>
@@ -7547,16 +7724,16 @@
         <v>43101</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>72</v>
@@ -7570,17 +7747,17 @@
         <v>43101</v>
       </c>
       <c r="C8" s="65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K8" s="60" t="s">
         <v>32</v>
@@ -7592,17 +7769,17 @@
       </c>
       <c r="B9" s="55"/>
       <c r="C9" s="65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>74</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="60"/>
@@ -7622,10 +7799,10 @@
         <v>43101</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>52</v>
@@ -7643,10 +7820,10 @@
         <v>43101</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>52</v>
@@ -7664,17 +7841,17 @@
         <v>43101</v>
       </c>
       <c r="C12" s="65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K12" s="60" t="s">
         <v>32</v>
@@ -7694,10 +7871,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7781,13 +7958,13 @@
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="56" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="59" t="s">
         <v>233</v>
-      </c>
-      <c r="E4" s="59" t="s">
-        <v>234</v>
       </c>
       <c r="F4" s="60"/>
       <c r="H4" s="5"/>
@@ -7808,7 +7985,7 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="61" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D5" s="62" t="s">
         <v>82</v>
@@ -7828,6 +8005,34 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A6" s="146">
+        <v>43101</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A7" s="147">
+        <v>43101</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D7" t="s">
+        <v>293</v>
+      </c>
+      <c r="E7" t="s">
+        <v>294</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -7951,7 +8156,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>92</v>
@@ -7972,16 +8177,16 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F5" s="60" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G5" s="72">
         <v>2</v>
@@ -7993,16 +8198,16 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G6" s="72">
         <v>3</v>
@@ -8013,7 +8218,7 @@
         <v>43101</v>
       </c>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>93</v>
@@ -8033,16 +8238,16 @@
         <v>43101</v>
       </c>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>244</v>
       </c>
       <c r="G8" s="72">
         <v>5</v>
@@ -8072,7 +8277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -8262,7 +8467,7 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>216</v>
@@ -8294,7 +8499,7 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>214</v>
@@ -8312,12 +8517,12 @@
         <v>92</v>
       </c>
       <c r="I5" s="60" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="143" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="143"/>
@@ -8337,13 +8542,13 @@
       </c>
       <c r="B6" s="71"/>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>215</v>
       </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F6" t="s">
         <v>218</v>
@@ -8355,12 +8560,12 @@
         <v>92</v>
       </c>
       <c r="I6" s="60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="143" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="143"/>
@@ -8380,7 +8585,7 @@
       </c>
       <c r="B7" s="71"/>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>122</v>
@@ -8421,7 +8626,7 @@
       </c>
       <c r="B8" s="71"/>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>124</v>
@@ -8439,7 +8644,7 @@
         <v>92</v>
       </c>
       <c r="I8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P8" s="51" t="s">
         <v>119</v>
@@ -8479,8 +8684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B2" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8644,19 +8849,19 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>214</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>220</v>
+        <v>289</v>
       </c>
       <c r="F4" s="72">
         <v>1</v>
       </c>
       <c r="G4" s="84" t="s">
-        <v>151</v>
+        <v>299</v>
       </c>
       <c r="H4" s="72">
         <v>1</v>
@@ -8678,19 +8883,19 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="E5" s="60" t="s">
-        <v>264</v>
+      <c r="E5" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>151</v>
+        <v>299</v>
       </c>
       <c r="H5" s="72">
         <v>1</v>
@@ -8712,19 +8917,19 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>272</v>
-      </c>
-      <c r="D6" s="60" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>56</v>
+        <v>271</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>263</v>
       </c>
       <c r="F6" s="72">
-        <v>1</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>149</v>
+        <v>3</v>
+      </c>
+      <c r="G6" s="84" t="s">
+        <v>151</v>
       </c>
       <c r="H6" s="72">
         <v>1</v>
@@ -8746,16 +8951,16 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="60" t="s">
-        <v>264</v>
+      <c r="E7" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="F7" s="72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="51" t="s">
         <v>149</v>
@@ -8780,19 +8985,19 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>272</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>215</v>
+        <v>271</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>122</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F8" s="72">
-        <v>1</v>
-      </c>
-      <c r="G8" s="84" t="s">
-        <v>151</v>
+        <v>2</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>149</v>
       </c>
       <c r="H8" s="72">
         <v>1</v>
@@ -8814,16 +9019,16 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>56</v>
+      <c r="E9" s="60" t="s">
+        <v>263</v>
       </c>
       <c r="F9" s="72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="84" t="s">
         <v>151</v>
@@ -8848,19 +9053,19 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s">
-        <v>272</v>
-      </c>
-      <c r="D10" s="60" t="s">
-        <v>124</v>
-      </c>
-      <c r="E10" s="60" t="s">
-        <v>264</v>
+        <v>271</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="F10" s="72">
-        <v>1</v>
-      </c>
-      <c r="G10" s="51" t="s">
-        <v>149</v>
+        <v>2</v>
+      </c>
+      <c r="G10" s="84" t="s">
+        <v>151</v>
       </c>
       <c r="H10" s="72">
         <v>1</v>
@@ -8871,6 +9076,10 @@
       <c r="K10" s="72">
         <v>1</v>
       </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A11" s="25">
@@ -8878,16 +9087,16 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>56</v>
+      <c r="E11" s="60" t="s">
+        <v>263</v>
       </c>
       <c r="F11" s="72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="51" t="s">
         <v>149</v>
@@ -8902,6 +9111,36 @@
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A12" s="25">
+        <v>43101</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="72">
+        <v>2</v>
+      </c>
+      <c r="G12" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="H12" s="72">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K12" s="72">
+        <v>1</v>
+      </c>
+    </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.15">
       <c r="E15" s="5"/>
     </row>
@@ -8930,8 +9169,8 @@
       <c r="E23" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0800-000000000000}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A12" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Rename caseReference ReferenceType to ccdCaseReference
... for clarity
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CECB56-523A-2B4B-9656-B7E894FD8AC1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E051C26-09F0-A144-BA21-CCCBE7C1E037}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,6 @@
     <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="301">
   <si>
     <t>Change History</t>
   </si>
@@ -987,9 +986,6 @@
     <t>ReferenceType</t>
   </si>
   <si>
-    <t>caseReference</t>
-  </si>
-  <si>
     <t>Case Reference</t>
   </si>
   <si>
@@ -1024,6 +1020,12 @@
   </si>
   <si>
     <t>MANDATORY</t>
+  </si>
+  <si>
+    <t>ccdCaseReference</t>
+  </si>
+  <si>
+    <t>Ranamed caseReference ReferenceType to ccdCaseReference</t>
   </si>
 </sst>
 </file>
@@ -2058,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2242,7 +2244,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
@@ -2251,7 +2253,7 @@
         <v>43606</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -2259,7 +2261,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
@@ -2268,7 +2270,24 @@
         <v>43606</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="144">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>300</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="6">
+        <v>43613</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -4805,7 +4824,7 @@
         <v>271</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E14" s="115" t="s">
         <v>252</v>
@@ -4822,7 +4841,7 @@
         <v>271</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E15" s="115" t="s">
         <v>252</v>
@@ -7385,10 +7404,10 @@
         <v>220</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F12" s="73" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>52</v>
@@ -7430,7 +7449,7 @@
         <v>271</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>284</v>
@@ -7457,10 +7476,10 @@
         <v>271</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F15" s="73" t="s">
         <v>283</v>
@@ -8014,10 +8033,10 @@
         <v>286</v>
       </c>
       <c r="D6" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="E6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
@@ -8028,10 +8047,10 @@
         <v>286</v>
       </c>
       <c r="D7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E7" t="s">
         <v>293</v>
-      </c>
-      <c r="E7" t="s">
-        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -8855,13 +8874,13 @@
         <v>214</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F4" s="72">
         <v>1</v>
       </c>
       <c r="G4" s="84" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H4" s="72">
         <v>1</v>
@@ -8889,13 +8908,13 @@
         <v>214</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F5" s="72">
         <v>2</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H5" s="72">
         <v>1</v>

</xml_diff>

<commit_message>
Change the display name of externalCaseReference fixed list element
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E051C26-09F0-A144-BA21-CCCBE7C1E037}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FD791F-E933-5744-B18A-1457520B7B60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="302">
   <si>
     <t>Change History</t>
   </si>
@@ -1004,9 +1004,6 @@
     <t>externalCaseReference</t>
   </si>
   <si>
-    <t>External Case Reference</t>
-  </si>
-  <si>
     <t>The CCD reference number of the case the exception record is attached to</t>
   </si>
   <si>
@@ -1026,6 +1023,12 @@
   </si>
   <si>
     <t>Ranamed caseReference ReferenceType to ccdCaseReference</t>
+  </si>
+  <si>
+    <t>Changed externalCaseReference fixed list element's display name</t>
+  </si>
+  <si>
+    <t>Legacy Case Reference</t>
   </si>
 </sst>
 </file>
@@ -2060,10 +2063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2244,7 +2247,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
@@ -2253,7 +2256,7 @@
         <v>43606</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -2261,7 +2264,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
@@ -2270,7 +2273,7 @@
         <v>43606</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -2278,7 +2281,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
@@ -2287,7 +2290,24 @@
         <v>43613</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="144">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>300</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="6">
+        <v>43622</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -7407,7 +7427,7 @@
         <v>290</v>
       </c>
       <c r="F12" s="73" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>52</v>
@@ -7893,7 +7913,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8033,7 +8053,7 @@
         <v>286</v>
       </c>
       <c r="D6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E6" t="s">
         <v>291</v>
@@ -8050,7 +8070,7 @@
         <v>292</v>
       </c>
       <c r="E7" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -8296,7 +8316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -8880,7 +8900,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="84" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H4" s="72">
         <v>1</v>
@@ -8914,7 +8934,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H5" s="72">
         <v>1</v>

</xml_diff>

<commit_message>
Add JourneyClassification in search input and result
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alivenic/projects/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7793DAC-7584-7648-91C2-F881EBA94E87}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A304541F-913A-5E48-A94A-235880920F04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="309">
   <si>
     <t>Change History</t>
   </si>
@@ -1049,6 +1049,9 @@
   </si>
   <si>
     <t>Add AuthorisationComplexType tab</t>
+  </si>
+  <si>
+    <t>Add JourneyClassification to SearchInputFields and WorkBasketResultFields</t>
   </si>
 </sst>
 </file>
@@ -1440,7 +1443,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1728,6 +1731,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -2114,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2393,6 +2397,23 @@
       </c>
       <c r="E17" s="2" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="144">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>308</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="160">
+        <v>43678</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -3336,7 +3357,7 @@
   <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3520,7 +3541,21 @@
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="D9" s="5"/>
+      <c r="A9" s="146">
+        <v>43678</v>
+      </c>
+      <c r="C9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F9" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.15">
       <c r="D10" s="5"/>
@@ -3950,7 +3985,7 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4173,11 +4208,22 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A8" s="25"/>
+      <c r="A8" s="25">
+        <v>43678</v>
+      </c>
       <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="C8" s="60" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="144" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A9" s="25"/>
@@ -7604,8 +7650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ15"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8518,7 +8564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{226FC805-C173-4E4F-B39D-58BF9E1FB96A}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+    <sheetView zoomScale="144" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modify label for search input field for journey classification
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A304541F-913A-5E48-A94A-235880920F04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EABDAA-88C1-9644-AE7F-54FAD1D6CE07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="680" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="311">
   <si>
     <t>Change History</t>
   </si>
@@ -1052,6 +1052,12 @@
   </si>
   <si>
     <t>Add JourneyClassification to SearchInputFields and WorkBasketResultFields</t>
+  </si>
+  <si>
+    <t>Journey Classifation can be new_application, supplementary_evidence or exception.</t>
+  </si>
+  <si>
+    <t>Modify label for JourneyClassification search input</t>
   </si>
 </sst>
 </file>
@@ -2118,10 +2124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2413,6 +2419,23 @@
         <v>43678</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="144">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>310</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="146">
+        <v>43693</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3357,7 +3380,7 @@
   <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3551,7 +3574,7 @@
         <v>212</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>213</v>
+        <v>309</v>
       </c>
       <c r="F9" s="2">
         <v>6</v>

</xml_diff>

<commit_message>
Add extra field just for label ¯\_(ツ)_/¯
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EABDAA-88C1-9644-AE7F-54FAD1D6CE07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AE58FA-6A72-0A4D-BCC4-9348DA50FB81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="680" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="680" windowWidth="28020" windowHeight="14640" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="313">
   <si>
     <t>Change History</t>
   </si>
@@ -1054,10 +1054,16 @@
     <t>Add JourneyClassification to SearchInputFields and WorkBasketResultFields</t>
   </si>
   <si>
-    <t>Journey Classifation can be new_application, supplementary_evidence or exception.</t>
-  </si>
-  <si>
-    <t>Modify label for JourneyClassification search input</t>
+    <t>labelJourneyClassification</t>
+  </si>
+  <si>
+    <t>Add label for JourneyClassification</t>
+  </si>
+  <si>
+    <t># Journey classification label</t>
+  </si>
+  <si>
+    <t>#### Journey Classifation can be new_application, supplementary_evidence or exception.</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1455,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1738,6 +1744,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -2126,7 +2134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -3377,10 +3385,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:AA20"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3564,35 +3572,49 @@
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A9" s="146">
-        <v>43678</v>
-      </c>
+      <c r="A9" s="25">
+        <v>43692</v>
+      </c>
+      <c r="B9" s="60"/>
       <c r="C9" t="s">
         <v>271</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>212</v>
+        <v>309</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F9" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="D10" s="5"/>
+      <c r="A10" s="146">
+        <v>43678</v>
+      </c>
+      <c r="C10" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="D11" s="60"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="D12" s="5"/>
-      <c r="E12" s="60"/>
+      <c r="D12" s="60"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.15">
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="E13" s="60"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.15">
       <c r="D14" s="5"/>
@@ -3615,18 +3637,22 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.15">
       <c r="E20" s="5"/>
     </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="E21" s="5"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B8" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0A00-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3885,7 +3911,7 @@
   <dimension ref="A1:AMK9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4007,8 +4033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4245,7 +4271,7 @@
         <v>213</v>
       </c>
       <c r="F8" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
@@ -5230,10 +5256,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView zoomScale="136" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5521,6 +5547,23 @@
         <v>252</v>
       </c>
       <c r="F15" s="118" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A16" s="146">
+        <v>43693</v>
+      </c>
+      <c r="C16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E16" s="161" t="s">
+        <v>252</v>
+      </c>
+      <c r="F16" s="162" t="s">
         <v>195</v>
       </c>
     </row>
@@ -7671,23 +7714,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ15"/>
+  <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
     <col min="6" max="6" width="32" style="141" customWidth="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" customWidth="1"/>
-    <col min="9" max="9" width="24.5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="20.33203125" customWidth="1"/>
     <col min="12" max="12" width="23.1640625" customWidth="1"/>
@@ -8163,6 +8206,26 @@
       </c>
       <c r="H15" s="5"/>
       <c r="J15" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.15">
+      <c r="A16" s="146">
+        <v>43693</v>
+      </c>
+      <c r="C16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 'Warnings' tab, containing OCR validation warnings
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/workspace/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A304541F-913A-5E48-A94A-235880920F04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90BB6B6-7367-2042-9407-800F46C5479A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -34,11 +34,15 @@
     <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId19"/>
     <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId20"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">CaseTypeTab!$A$2:$K$15</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -49,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="321">
   <si>
     <t>Change History</t>
   </si>
@@ -1052,6 +1056,42 @@
   </si>
   <si>
     <t>Add JourneyClassification to SearchInputFields and WorkBasketResultFields</t>
+  </si>
+  <si>
+    <t>Warnings</t>
+  </si>
+  <si>
+    <t>warnings</t>
+  </si>
+  <si>
+    <t>Add Warnings tab</t>
+  </si>
+  <si>
+    <t>YesOrNo</t>
+  </si>
+  <si>
+    <t>hasWarnings</t>
+  </si>
+  <si>
+    <t>ocrDataValidationWarnings</t>
+  </si>
+  <si>
+    <t>Has warnings</t>
+  </si>
+  <si>
+    <t>TextArea</t>
+  </si>
+  <si>
+    <t>OCR data validation warnings</t>
+  </si>
+  <si>
+    <t>hasWarnings="Yes"</t>
+  </si>
+  <si>
+    <t>Indicates if there are any warnings to display</t>
+  </si>
+  <si>
+    <t>hasWarnings="{NeverShowThisField}"</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1329,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1443,7 +1483,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1732,6 +1772,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -2118,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A4" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2416,6 +2457,23 @@
         <v>249</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="144">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>311</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6">
+        <v>43710</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2430,8 +2488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="C1" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2915,7 +2973,7 @@
       <c r="E23" s="5"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A12" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
@@ -2930,8 +2988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N1048546"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2945,7 +3003,7 @@
     <col min="7" max="7" width="13.83203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="24.83203125" customWidth="1"/>
     <col min="9" max="9" width="20.1640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.1640625" customWidth="1"/>
+    <col min="10" max="10" width="28.5" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="11.5"/>
     <col min="13" max="27" width="7.1640625" customWidth="1"/>
@@ -3063,20 +3121,23 @@
       <c r="D4" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="E4" s="60" t="s">
-        <v>282</v>
-      </c>
-      <c r="F4" s="60" t="s">
-        <v>277</v>
-      </c>
-      <c r="G4" s="86">
+      <c r="E4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F4" t="s">
+        <v>309</v>
+      </c>
+      <c r="G4" s="2">
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="I4" s="86">
+        <v>314</v>
+      </c>
+      <c r="I4" s="2">
         <v>1</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3090,20 +3151,23 @@
       <c r="D5" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="E5" s="60" t="s">
-        <v>224</v>
+      <c r="E5" t="s">
+        <v>310</v>
       </c>
       <c r="F5" s="60" t="s">
-        <v>223</v>
+        <v>309</v>
       </c>
       <c r="G5" s="86">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>313</v>
+      </c>
+      <c r="I5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="I5" s="86">
-        <v>1</v>
+      <c r="J5" s="5" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3118,19 +3182,19 @@
         <v>167</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>224</v>
+        <v>282</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>223</v>
+        <v>277</v>
       </c>
       <c r="G6" s="86">
         <v>2</v>
       </c>
-      <c r="H6" s="60" t="s">
-        <v>212</v>
+      <c r="H6" s="5" t="s">
+        <v>279</v>
       </c>
       <c r="I6" s="86">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3151,13 +3215,13 @@
         <v>223</v>
       </c>
       <c r="G7" s="86">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="I7" s="86">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3178,13 +3242,13 @@
         <v>223</v>
       </c>
       <c r="G8" s="86">
+        <v>3</v>
+      </c>
+      <c r="H8" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="I8" s="86">
         <v>2</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="I8" s="86">
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3205,13 +3269,13 @@
         <v>223</v>
       </c>
       <c r="G9" s="86">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I9" s="86">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3232,13 +3296,13 @@
         <v>223</v>
       </c>
       <c r="G10" s="86">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="I10" s="86">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3259,13 +3323,13 @@
         <v>223</v>
       </c>
       <c r="G11" s="86">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="I11" s="86">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3280,19 +3344,19 @@
         <v>167</v>
       </c>
       <c r="E12" s="60" t="s">
-        <v>168</v>
+        <v>224</v>
       </c>
       <c r="F12" s="60" t="s">
-        <v>169</v>
+        <v>223</v>
       </c>
       <c r="G12" s="86">
         <v>3</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="I12" s="86">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3307,42 +3371,88 @@
         <v>167</v>
       </c>
       <c r="E13" s="60" t="s">
+        <v>224</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>223</v>
+      </c>
+      <c r="G13" s="86">
+        <v>3</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I13" s="86">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A14" s="25">
+        <v>43101</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" s="60" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>169</v>
+      </c>
+      <c r="G14" s="86">
+        <v>4</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I14" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A15" s="25">
+        <v>43101</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="60" t="s">
         <v>225</v>
       </c>
-      <c r="F13" s="60" t="s">
+      <c r="F15" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="G13" s="86">
-        <v>4</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="G15" s="86">
+        <v>5</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I13" s="86">
+      <c r="I15" s="86">
         <v>1</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J15" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A14" s="25"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="H14" s="60"/>
     </row>
     <row r="1048545" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1048546" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
+  <autoFilter ref="A2:K15" xr:uid="{D32A85A1-D1A5-6B42-B8E2-8BB73B4191BA}"/>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B14" xr:uid="{00000000-0002-0000-0900-000001000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5207,10 +5317,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView zoomScale="136" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5218,7 +5328,7 @@
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="39.83203125" customWidth="1"/>
     <col min="5" max="5" width="28.5" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
     <col min="7" max="9" width="8.33203125" customWidth="1"/>
@@ -5501,9 +5611,43 @@
         <v>195</v>
       </c>
     </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A16" s="117">
+        <v>43101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E16" s="115" t="s">
+        <v>252</v>
+      </c>
+      <c r="F16" s="118" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="117">
+        <v>43101</v>
+      </c>
+      <c r="C17" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="E17" s="115" t="s">
+        <v>252</v>
+      </c>
+      <c r="F17" s="118" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15" xr:uid="{00000000-0002-0000-1000-000000000000}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A17" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5517,7 +5661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="166" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="166" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -6570,8 +6714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7648,10 +7792,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ15"/>
+  <dimension ref="A1:AMJ17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8143,14 +8287,61 @@
         <v>32</v>
       </c>
     </row>
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.15">
+      <c r="A16" s="25">
+        <v>43101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E16" t="s">
+        <v>317</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+      <c r="A17" s="25">
+        <v>43101</v>
+      </c>
+      <c r="C17" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="E17" t="s">
+        <v>315</v>
+      </c>
+      <c r="F17" s="141" t="s">
+        <v>319</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="J17" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15" xr:uid="{00000000-0002-0000-0300-000000000000}">
-      <formula1>42736</formula1>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0300-000001000000}">
+      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0300-000001000000}">
-      <formula1>0</formula1>
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A17" xr:uid="{00000000-0002-0000-0300-000000000000}">
+      <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -8161,10 +8352,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D13"/>
+    <sheetView topLeftCell="A2" zoomScale="144" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8548,9 +8739,17 @@
         <v>32</v>
       </c>
     </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A14" s="25"/>
+      <c r="C14" s="161"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="142"/>
+      <c r="G14" s="142"/>
+      <c r="K14" s="60"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A13" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8564,8 +8763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{226FC805-C173-4E4F-B39D-58BF9E1FB96A}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C10"/>
+    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8802,7 +9001,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9205,8 +9404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Rename hasWarnings field to displayWarnings
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90BB6B6-7367-2042-9407-800F46C5479A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7415D5-7E6C-8042-9DA3-A47705E0FFD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -1070,28 +1070,28 @@
     <t>YesOrNo</t>
   </si>
   <si>
-    <t>hasWarnings</t>
-  </si>
-  <si>
     <t>ocrDataValidationWarnings</t>
   </si>
   <si>
-    <t>Has warnings</t>
-  </si>
-  <si>
     <t>TextArea</t>
   </si>
   <si>
     <t>OCR data validation warnings</t>
   </si>
   <si>
-    <t>hasWarnings="Yes"</t>
-  </si>
-  <si>
-    <t>Indicates if there are any warnings to display</t>
-  </si>
-  <si>
-    <t>hasWarnings="{NeverShowThisField}"</t>
+    <t>displayWarnings</t>
+  </si>
+  <si>
+    <t>displayWarnings="Yes"</t>
+  </si>
+  <si>
+    <t>displayWarnings="{NeverShowThisField}"</t>
+  </si>
+  <si>
+    <t>Display warnings</t>
+  </si>
+  <si>
+    <t>Indicates if Warnings tab should be displayed</t>
   </si>
 </sst>
 </file>
@@ -2988,7 +2988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N1048546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -3131,13 +3131,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I4" s="2">
         <v>1</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3161,13 +3161,13 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I5" s="2">
         <v>2</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5619,7 +5619,7 @@
         <v>271</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E16" s="115" t="s">
         <v>252</v>
@@ -5636,7 +5636,7 @@
         <v>271</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E17" s="115" t="s">
         <v>252</v>
@@ -7794,8 +7794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8295,16 +8295,16 @@
         <v>271</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>55</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>32</v>
@@ -8318,13 +8318,13 @@
         <v>271</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E17" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="F17" s="141" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>312</v>
@@ -8335,7 +8335,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>

</xml_diff>

<commit_message>
Include the change in history tab
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7415D5-7E6C-8042-9DA3-A47705E0FFD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F951A36-5B36-3A40-A7A6-679A5880D7B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="322">
   <si>
     <t>Change History</t>
   </si>
@@ -1092,6 +1092,9 @@
   </si>
   <si>
     <t>Indicates if Warnings tab should be displayed</t>
+  </si>
+  <si>
+    <t>Rename hasWarnings field to displayWarnings</t>
   </si>
 </sst>
 </file>
@@ -2159,10 +2162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2471,6 +2474,23 @@
         <v>43710</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="144">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>321</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="6">
+        <v>43717</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>295</v>
       </c>
     </row>
@@ -7794,7 +7814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add envelopeId field to exception record definition
</commit_message>
<xml_diff>
--- a/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
+++ b/docker/ccd-definition-import/data/CCD_Definition_Exception_Record.template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leszekg/MOJ/Reform/bulk-scan-shared-infrastructure/docker/ccd-definition-import/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F951A36-5B36-3A40-A7A6-679A5880D7B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3734D3E7-2D64-EB4C-981F-D1C0DC502EC8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="326">
   <si>
     <t>Change History</t>
   </si>
@@ -1095,6 +1095,18 @@
   </si>
   <si>
     <t>Rename hasWarnings field to displayWarnings</t>
+  </si>
+  <si>
+    <t>Add envelopeId field</t>
+  </si>
+  <si>
+    <t>envelopeId</t>
+  </si>
+  <si>
+    <t>Envelope ID</t>
+  </si>
+  <si>
+    <t>ID of the envelope the exception record was created from</t>
   </si>
 </sst>
 </file>
@@ -2162,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="178" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2491,6 +2503,23 @@
         <v>43717</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="144">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>322</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="6">
+        <v>43724</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>295</v>
       </c>
     </row>
@@ -5337,10 +5366,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScale="136" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5665,9 +5694,26 @@
         <v>195</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="117">
+        <v>43101</v>
+      </c>
+      <c r="C18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="E18" s="115" t="s">
+        <v>252</v>
+      </c>
+      <c r="F18" s="118" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A17" xr:uid="{00000000-0002-0000-1000-000000000000}">
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7812,10 +7858,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ17"/>
+  <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8354,13 +8400,37 @@
         <v>32</v>
       </c>
     </row>
+    <row r="18" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+      <c r="A18" s="25">
+        <v>43101</v>
+      </c>
+      <c r="C18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="E18" t="s">
+        <v>324</v>
+      </c>
+      <c r="F18" s="141" t="s">
+        <v>325</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="J18" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A17" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>